<commit_message>
Update some of commodity sets
</commit_message>
<xml_diff>
--- a/SetRules.xlsx
+++ b/SetRules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06577315-435B-42FF-81FA-6FA260A9A86C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FDB8914-3BCA-46C4-8FA5-88BE1F171036}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{194177E5-D604-47FB-933F-7CD5106C261E}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{194177E5-D604-47FB-933F-7CD5106C261E}"/>
   </bookViews>
   <sheets>
     <sheet name="VEDA_Sets-Comm" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1903" uniqueCount="836">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1880" uniqueCount="821">
   <si>
     <t>~TFM_Psets</t>
   </si>
@@ -2124,15 +2124,6 @@
     <t>DEM</t>
   </si>
   <si>
-    <t>A*,-AGR</t>
-  </si>
-  <si>
-    <t>AGR-DMD</t>
-  </si>
-  <si>
-    <t>Agri-Demand</t>
-  </si>
-  <si>
     <t>I*STM</t>
   </si>
   <si>
@@ -2184,9 +2175,6 @@
     <t>Biomass</t>
   </si>
   <si>
-    <t>COA___,*COA,*COB,*COL,*COH,COL*,COH*,*COK,*DGS</t>
-  </si>
-  <si>
     <t>ALLCOAL</t>
   </si>
   <si>
@@ -2196,21 +2184,12 @@
     <t>ALLELC</t>
   </si>
   <si>
-    <t>GAS___,___GAS,*COG,*BFG,-BIOGAS</t>
-  </si>
-  <si>
     <t>ALLGAS</t>
   </si>
   <si>
-    <t>*GEO</t>
-  </si>
-  <si>
     <t>ALLGEO</t>
   </si>
   <si>
-    <t>Geo</t>
-  </si>
-  <si>
     <t>*H2*,,-BIO*,-*ETH</t>
   </si>
   <si>
@@ -2238,9 +2217,6 @@
     <t>ALLHYD</t>
   </si>
   <si>
-    <t>*NUC*,NUC*</t>
-  </si>
-  <si>
     <t>ALLNUC</t>
   </si>
   <si>
@@ -2283,18 +2259,6 @@
     <t>*CH4*</t>
   </si>
   <si>
-    <t>CH4</t>
-  </si>
-  <si>
-    <t>CHX</t>
-  </si>
-  <si>
-    <t>*CO2*,-SE*,-TOT*,-SNK*,-___SCO2*</t>
-  </si>
-  <si>
-    <t>CO2</t>
-  </si>
-  <si>
     <t>DEM_AGR</t>
   </si>
   <si>
@@ -2304,90 +2268,42 @@
     <t>DEM_COM</t>
   </si>
   <si>
-    <t>Commercial Demands</t>
-  </si>
-  <si>
     <t>DEM_IND</t>
   </si>
   <si>
-    <t>Industrial Demands</t>
-  </si>
-  <si>
     <t>DEM_RSD</t>
   </si>
   <si>
-    <t>Residential Demands</t>
-  </si>
-  <si>
     <t>DEM_TRA</t>
   </si>
   <si>
     <t>Trasport Demand</t>
   </si>
   <si>
-    <t>DEMRHX</t>
-  </si>
-  <si>
-    <t>C___,R___,T__,I__</t>
-  </si>
-  <si>
-    <t>DM</t>
-  </si>
-  <si>
     <t>ENV_CH4</t>
   </si>
   <si>
-    <t>*CO2*,-SE*,-TOT*,-SNK*</t>
-  </si>
-  <si>
     <t>ENV_CO2</t>
   </si>
   <si>
-    <t>*COX*</t>
-  </si>
-  <si>
-    <t>ENV_COX</t>
-  </si>
-  <si>
-    <t>CO</t>
-  </si>
-  <si>
     <t>*N2O*</t>
   </si>
   <si>
     <t>ENV_N2O</t>
   </si>
   <si>
-    <t>*NO*,-*N2O*</t>
-  </si>
-  <si>
     <t>ENV_NOX</t>
   </si>
   <si>
-    <t>*PM*</t>
-  </si>
-  <si>
     <t>ENV_PMX</t>
   </si>
   <si>
-    <t>*SO*</t>
-  </si>
-  <si>
     <t>ENV_SOX</t>
   </si>
   <si>
-    <t>*VO*</t>
-  </si>
-  <si>
     <t>ENV_VOC</t>
   </si>
   <si>
-    <t>VOC</t>
-  </si>
-  <si>
-    <t>___ELC</t>
-  </si>
-  <si>
     <t>FINALELC</t>
   </si>
   <si>
@@ -2451,33 +2367,18 @@
     <t>Renewable - TRA</t>
   </si>
   <si>
-    <t>ELC___,-ELCHIG*,-ELCMED,-ELCLOW</t>
-  </si>
-  <si>
     <t>FUEELC</t>
   </si>
   <si>
-    <t>ENV,NRG</t>
-  </si>
-  <si>
-    <t>FUEELC+ELC</t>
-  </si>
-  <si>
     <t>FUEELC-REN</t>
   </si>
   <si>
     <t>Ren Fuels</t>
   </si>
   <si>
-    <t>Resdential</t>
-  </si>
-  <si>
     <t>FUESUP</t>
   </si>
   <si>
-    <t>Energy Transformation</t>
-  </si>
-  <si>
     <t>I*LTH,I*HTH</t>
   </si>
   <si>
@@ -2487,64 +2388,118 @@
     <t>Industrial Heat</t>
   </si>
   <si>
-    <t>N2O</t>
-  </si>
-  <si>
-    <t>NOX</t>
-  </si>
-  <si>
-    <t>,-GASBFG</t>
-  </si>
-  <si>
-    <t>NRG-BFG</t>
-  </si>
-  <si>
-    <t>NRG no BFG</t>
-  </si>
-  <si>
-    <t>*TID*,*WAV*</t>
-  </si>
-  <si>
-    <t>OCEAN</t>
-  </si>
-  <si>
-    <t>OILHFO,OILDST,OILGSL,OILLPG,OILKER</t>
-  </si>
-  <si>
-    <t>OILRPPTRD</t>
-  </si>
-  <si>
-    <t>Traded RPP</t>
-  </si>
-  <si>
-    <t>PMX</t>
-  </si>
-  <si>
-    <t>RSD_DEM</t>
-  </si>
-  <si>
-    <t>SOX</t>
-  </si>
-  <si>
-    <t>TRAELC, TRABAT</t>
-  </si>
-  <si>
-    <t>TRAELC</t>
-  </si>
-  <si>
     <t>*TID, *WAV</t>
   </si>
   <si>
-    <t>A__</t>
-  </si>
-  <si>
-    <t>C___</t>
-  </si>
-  <si>
-    <t>I__</t>
-  </si>
-  <si>
-    <t>T__</t>
+    <t>A*</t>
+  </si>
+  <si>
+    <t>Commercial Demand</t>
+  </si>
+  <si>
+    <t>Industrial Demand</t>
+  </si>
+  <si>
+    <t>Residential Demand</t>
+  </si>
+  <si>
+    <t>I*,N*</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>CH4 Emissions</t>
+  </si>
+  <si>
+    <t>*CO2*,-*CO2S*</t>
+  </si>
+  <si>
+    <t>CO2 Emissions</t>
+  </si>
+  <si>
+    <t>N2O Emissions</t>
+  </si>
+  <si>
+    <t>*NOx*</t>
+  </si>
+  <si>
+    <t>NOx Emissions</t>
+  </si>
+  <si>
+    <t>PM2.5 Emissions</t>
+  </si>
+  <si>
+    <t>PM10 Emissions</t>
+  </si>
+  <si>
+    <t>ENV_PM10</t>
+  </si>
+  <si>
+    <t>ENV_PM2p5</t>
+  </si>
+  <si>
+    <t>*PM25*</t>
+  </si>
+  <si>
+    <t>*PM10*</t>
+  </si>
+  <si>
+    <t>*SO2*</t>
+  </si>
+  <si>
+    <t>ENV_SO2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SO2 Emissions </t>
+  </si>
+  <si>
+    <t>*VOC*</t>
+  </si>
+  <si>
+    <t>VOC Emissions</t>
+  </si>
+  <si>
+    <t>*ELC</t>
+  </si>
+  <si>
+    <t>FEC_ELC</t>
+  </si>
+  <si>
+    <t>Final consumption -  electricity</t>
+  </si>
+  <si>
+    <t>Agriculture fuels</t>
+  </si>
+  <si>
+    <t>Commercial fuels</t>
+  </si>
+  <si>
+    <t>Industrial fuels</t>
+  </si>
+  <si>
+    <t>Resdential fuels</t>
+  </si>
+  <si>
+    <t>Supply fuels</t>
+  </si>
+  <si>
+    <t>Transport fuels</t>
+  </si>
+  <si>
+    <t>ELC*,-ELCH,-ELCD,-ELCC</t>
+  </si>
+  <si>
+    <t>Electricity sector fuels</t>
+  </si>
+  <si>
+    <t>*NUC*</t>
+  </si>
+  <si>
+    <t>*COA*,*COH,*COK</t>
+  </si>
+  <si>
+    <t>*GAS*,*COG,*BFG,-BIOGAS</t>
   </si>
 </sst>
 </file>
@@ -2906,23 +2861,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C81DF5AD-B845-4EDD-A631-66C609C42342}">
-  <dimension ref="A1:N68"/>
+  <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="9" width="9.140625" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>686</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>687</v>
       </c>
@@ -2954,19 +2912,16 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>694</v>
-      </c>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>695</v>
       </c>
       <c r="D3" t="str">
-        <f>"z_"&amp;N3</f>
-        <v>z_AGR-DMD</v>
+        <f t="shared" ref="D3:D47" si="0">"z_"&amp;N3</f>
+        <v>z_ALL_STM</v>
       </c>
       <c r="E3" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="F3" t="s">
         <v>17</v>
@@ -2978,13 +2933,13 @@
         <v>696</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="D4" t="str">
-        <f t="shared" ref="D4:D67" si="0">"z_"&amp;N4</f>
-        <v>z_ALL_STM</v>
+        <f t="shared" si="0"/>
+        <v>z_ALL_TH</v>
       </c>
       <c r="E4" t="s">
         <v>699</v>
@@ -2996,43 +2951,46 @@
         <v>17</v>
       </c>
       <c r="N4" t="s">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>700</v>
+      </c>
       <c r="B5" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
-        <v>z_ALL_TH</v>
+        <v>z_ALLBIO</v>
       </c>
       <c r="E5" t="s">
+        <v>703</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+      <c r="N5" t="s">
         <v>702</v>
       </c>
-      <c r="F5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" t="s">
-        <v>17</v>
-      </c>
-      <c r="N5" t="s">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="B6" t="s">
         <v>704</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
-        <v>z_ALLBIO</v>
+        <v>z_ALLBIOGAS</v>
       </c>
       <c r="E6" t="s">
-        <v>706</v>
+        <v>148</v>
       </c>
       <c r="F6" t="s">
         <v>17</v>
@@ -3044,19 +3002,19 @@
         <v>705</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="B7" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v>z_ALLBIOGAS</v>
+        <v>z_ALLBIOLIQ</v>
       </c>
       <c r="E7" t="s">
-        <v>148</v>
+        <v>708</v>
       </c>
       <c r="F7" t="s">
         <v>17</v>
@@ -3065,16 +3023,19 @@
         <v>17</v>
       </c>
       <c r="N7" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>700</v>
+      </c>
       <c r="B8" t="s">
         <v>709</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v>z_ALLBIOLIQ</v>
+        <v>z_ALLBIOMASS</v>
       </c>
       <c r="E8" t="s">
         <v>711</v>
@@ -3089,19 +3050,18 @@
         <v>710</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="B9" t="s">
+        <v>819</v>
+      </c>
+      <c r="D9" t="s">
         <v>712</v>
       </c>
-      <c r="D9" t="str">
-        <f t="shared" si="0"/>
-        <v>z_ALLBIOMASS</v>
-      </c>
       <c r="E9" t="s">
-        <v>714</v>
+        <v>151</v>
       </c>
       <c r="F9" t="s">
         <v>17</v>
@@ -3110,22 +3070,25 @@
         <v>17</v>
       </c>
       <c r="N9" t="s">
+        <v>712</v>
+      </c>
+      <c r="P9" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>700</v>
+      </c>
+      <c r="B10" t="s">
         <v>713</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>703</v>
-      </c>
-      <c r="B10" t="s">
-        <v>715</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v>z_ALLCOAL</v>
+        <v>z_ALLELC</v>
       </c>
       <c r="E10" t="s">
-        <v>151</v>
+        <v>350</v>
       </c>
       <c r="F10" t="s">
         <v>17</v>
@@ -3134,64 +3097,74 @@
         <v>17</v>
       </c>
       <c r="N10" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>700</v>
+      </c>
+      <c r="B11" t="s">
+        <v>820</v>
+      </c>
+      <c r="D11" t="s">
+        <v>715</v>
+      </c>
+      <c r="E11" t="s">
+        <v>158</v>
+      </c>
+      <c r="F11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" t="s">
+        <v>17</v>
+      </c>
+      <c r="N11" t="s">
+        <v>715</v>
+      </c>
+      <c r="P11" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>700</v>
+      </c>
+      <c r="B12" t="s">
+        <v>370</v>
+      </c>
+      <c r="D12" t="s">
         <v>716</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="E12" t="s">
+        <v>161</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" t="s">
+        <v>17</v>
+      </c>
+      <c r="N12" t="s">
+        <v>716</v>
+      </c>
+      <c r="P12" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>700</v>
+      </c>
+      <c r="B13" t="s">
         <v>717</v>
-      </c>
-      <c r="D11" t="str">
-        <f t="shared" si="0"/>
-        <v>z_ALLELC</v>
-      </c>
-      <c r="E11" t="s">
-        <v>350</v>
-      </c>
-      <c r="F11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" t="s">
-        <v>17</v>
-      </c>
-      <c r="N11" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>719</v>
-      </c>
-      <c r="D12" t="str">
-        <f t="shared" si="0"/>
-        <v>z_ALLGAS</v>
-      </c>
-      <c r="E12" t="s">
-        <v>158</v>
-      </c>
-      <c r="F12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" t="s">
-        <v>17</v>
-      </c>
-      <c r="N12" t="s">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>703</v>
-      </c>
-      <c r="B13" t="s">
-        <v>721</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
-        <v>z_ALLGEO</v>
+        <v>z_ALLH2</v>
       </c>
       <c r="E13" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="F13" t="s">
         <v>17</v>
@@ -3200,22 +3173,22 @@
         <v>17</v>
       </c>
       <c r="N13" t="s">
-        <v>722</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="B14" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
-        <v>z_ALLH2</v>
+        <v>z_ALLHET</v>
       </c>
       <c r="E14" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="F14" t="s">
         <v>17</v>
@@ -3224,19 +3197,22 @@
         <v>17</v>
       </c>
       <c r="N14" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>700</v>
+      </c>
       <c r="B15" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
-        <v>z_ALLHET</v>
+        <v>z_ALLHETNOIND</v>
       </c>
       <c r="E15" t="s">
-        <v>729</v>
+        <v>722</v>
       </c>
       <c r="F15" t="s">
         <v>17</v>
@@ -3245,19 +3221,21 @@
         <v>17</v>
       </c>
       <c r="N15" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>700</v>
+      </c>
       <c r="B16" t="s">
-        <v>730</v>
-      </c>
-      <c r="D16" t="str">
-        <f t="shared" si="0"/>
-        <v>z_ALLHETNOIND</v>
+        <v>220</v>
+      </c>
+      <c r="D16" t="s">
+        <v>725</v>
       </c>
       <c r="E16" t="s">
-        <v>729</v>
+        <v>293</v>
       </c>
       <c r="F16" t="s">
         <v>17</v>
@@ -3266,22 +3244,24 @@
         <v>17</v>
       </c>
       <c r="N16" t="s">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+        <v>725</v>
+      </c>
+      <c r="P16" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="B17" t="s">
-        <v>291</v>
-      </c>
-      <c r="D17" t="str">
-        <f t="shared" si="0"/>
-        <v>z_ALLHYD</v>
+        <v>818</v>
+      </c>
+      <c r="D17" t="s">
+        <v>726</v>
       </c>
       <c r="E17" t="s">
-        <v>293</v>
+        <v>172</v>
       </c>
       <c r="F17" t="s">
         <v>17</v>
@@ -3290,22 +3270,25 @@
         <v>17</v>
       </c>
       <c r="N17" t="s">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+        <v>726</v>
+      </c>
+      <c r="P17" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="B18" t="s">
-        <v>733</v>
+        <v>783</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
-        <v>z_ALLNUC</v>
+        <v>z_ALLOCE</v>
       </c>
       <c r="E18" t="s">
-        <v>172</v>
+        <v>728</v>
       </c>
       <c r="F18" t="s">
         <v>17</v>
@@ -3314,19 +3297,22 @@
         <v>17</v>
       </c>
       <c r="N18" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>700</v>
+      </c>
       <c r="B19" t="s">
-        <v>831</v>
+        <v>729</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
-        <v>z_ALLOCE</v>
+        <v>z_ALLOIL</v>
       </c>
       <c r="E19" t="s">
-        <v>736</v>
+        <v>175</v>
       </c>
       <c r="F19" t="s">
         <v>17</v>
@@ -3335,22 +3321,22 @@
         <v>17</v>
       </c>
       <c r="N19" t="s">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="B20" t="s">
-        <v>737</v>
+        <v>731</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
-        <v>z_ALLOIL</v>
+        <v>z_ALLREN</v>
       </c>
       <c r="E20" t="s">
-        <v>175</v>
+        <v>516</v>
       </c>
       <c r="F20" t="s">
         <v>17</v>
@@ -3359,22 +3345,21 @@
         <v>17</v>
       </c>
       <c r="N20" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="B21" t="s">
-        <v>739</v>
-      </c>
-      <c r="D21" t="str">
-        <f t="shared" si="0"/>
-        <v>z_ALLREN</v>
+        <v>305</v>
+      </c>
+      <c r="D21" t="s">
+        <v>733</v>
       </c>
       <c r="E21" t="s">
-        <v>516</v>
+        <v>307</v>
       </c>
       <c r="F21" t="s">
         <v>17</v>
@@ -3383,19 +3368,25 @@
         <v>17</v>
       </c>
       <c r="N21" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+        <v>733</v>
+      </c>
+      <c r="P21" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>700</v>
+      </c>
       <c r="B22" t="s">
-        <v>305</v>
+        <v>734</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
-        <v>z_ALLSOL</v>
+        <v>z_ALLSYN</v>
       </c>
       <c r="E22" t="s">
-        <v>307</v>
+        <v>736</v>
       </c>
       <c r="F22" t="s">
         <v>17</v>
@@ -3404,67 +3395,73 @@
         <v>17</v>
       </c>
       <c r="N22" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>700</v>
+      </c>
+      <c r="B23" t="s">
+        <v>311</v>
+      </c>
+      <c r="D23" t="s">
+        <v>737</v>
+      </c>
+      <c r="E23" t="s">
+        <v>313</v>
+      </c>
+      <c r="F23" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" t="s">
+        <v>17</v>
+      </c>
+      <c r="N23" t="s">
+        <v>737</v>
+      </c>
+      <c r="P23" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>694</v>
+      </c>
+      <c r="B24" t="s">
+        <v>784</v>
+      </c>
+      <c r="D24" t="s">
+        <v>740</v>
+      </c>
+      <c r="E24" t="s">
         <v>741</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>703</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="F24" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" t="s">
+        <v>17</v>
+      </c>
+      <c r="N24" t="s">
+        <v>740</v>
+      </c>
+      <c r="P24" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>694</v>
+      </c>
+      <c r="B25" t="s">
+        <v>138</v>
+      </c>
+      <c r="D25" t="s">
         <v>742</v>
       </c>
-      <c r="D23" t="str">
-        <f t="shared" si="0"/>
-        <v>z_ALLSYN</v>
-      </c>
-      <c r="E23" t="s">
-        <v>744</v>
-      </c>
-      <c r="F23" t="s">
-        <v>17</v>
-      </c>
-      <c r="G23" t="s">
-        <v>17</v>
-      </c>
-      <c r="N23" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>311</v>
-      </c>
-      <c r="D24" t="str">
-        <f t="shared" si="0"/>
-        <v>z_ALLWIN</v>
-      </c>
-      <c r="E24" t="s">
-        <v>313</v>
-      </c>
-      <c r="F24" t="s">
-        <v>17</v>
-      </c>
-      <c r="G24" t="s">
-        <v>17</v>
-      </c>
-      <c r="N24" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>746</v>
-      </c>
-      <c r="B25" t="s">
-        <v>747</v>
-      </c>
-      <c r="D25" t="str">
-        <f t="shared" si="0"/>
-        <v>z_CH4</v>
-      </c>
       <c r="E25" t="s">
-        <v>748</v>
+        <v>785</v>
       </c>
       <c r="F25" t="s">
         <v>17</v>
@@ -3473,22 +3470,24 @@
         <v>17</v>
       </c>
       <c r="N25" t="s">
-        <v>748</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+        <v>742</v>
+      </c>
+      <c r="P25" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>694</v>
       </c>
       <c r="B26" t="s">
-        <v>677</v>
-      </c>
-      <c r="D26" t="str">
-        <f t="shared" si="0"/>
-        <v>z_CHX</v>
+        <v>788</v>
+      </c>
+      <c r="D26" t="s">
+        <v>743</v>
       </c>
       <c r="E26" t="s">
-        <v>749</v>
+        <v>786</v>
       </c>
       <c r="F26" t="s">
         <v>17</v>
@@ -3497,22 +3496,24 @@
         <v>17</v>
       </c>
       <c r="N26" t="s">
-        <v>749</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+        <v>743</v>
+      </c>
+      <c r="P26" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>746</v>
+        <v>694</v>
       </c>
       <c r="B27" t="s">
-        <v>750</v>
-      </c>
-      <c r="D27" t="str">
-        <f t="shared" si="0"/>
-        <v>z_CO2</v>
+        <v>496</v>
+      </c>
+      <c r="D27" t="s">
+        <v>744</v>
       </c>
       <c r="E27" t="s">
-        <v>751</v>
+        <v>787</v>
       </c>
       <c r="F27" t="s">
         <v>17</v>
@@ -3521,256 +3522,282 @@
         <v>17</v>
       </c>
       <c r="N27" t="s">
-        <v>751</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+        <v>744</v>
+      </c>
+      <c r="P27" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>694</v>
       </c>
       <c r="B28" t="s">
-        <v>832</v>
-      </c>
-      <c r="D28" t="str">
-        <f t="shared" si="0"/>
-        <v>z_DEM_AGR</v>
+        <v>575</v>
+      </c>
+      <c r="D28" t="s">
+        <v>745</v>
       </c>
       <c r="E28" t="s">
+        <v>746</v>
+      </c>
+      <c r="F28" t="s">
+        <v>17</v>
+      </c>
+      <c r="G28" t="s">
+        <v>17</v>
+      </c>
+      <c r="N28" t="s">
+        <v>745</v>
+      </c>
+      <c r="P28" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>738</v>
+      </c>
+      <c r="B29" t="s">
+        <v>739</v>
+      </c>
+      <c r="D29" t="s">
+        <v>747</v>
+      </c>
+      <c r="E29" t="s">
+        <v>790</v>
+      </c>
+      <c r="F29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G29" t="s">
+        <v>17</v>
+      </c>
+      <c r="N29" t="s">
+        <v>747</v>
+      </c>
+      <c r="P29" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>738</v>
+      </c>
+      <c r="B30" t="s">
+        <v>791</v>
+      </c>
+      <c r="D30" t="s">
+        <v>748</v>
+      </c>
+      <c r="E30" t="s">
+        <v>792</v>
+      </c>
+      <c r="F30" t="s">
+        <v>17</v>
+      </c>
+      <c r="G30" t="s">
+        <v>17</v>
+      </c>
+      <c r="N30" t="s">
+        <v>748</v>
+      </c>
+      <c r="P30" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>738</v>
+      </c>
+      <c r="B31" t="s">
+        <v>749</v>
+      </c>
+      <c r="D31" t="s">
+        <v>750</v>
+      </c>
+      <c r="E31" t="s">
+        <v>793</v>
+      </c>
+      <c r="F31" t="s">
+        <v>17</v>
+      </c>
+      <c r="G31" t="s">
+        <v>17</v>
+      </c>
+      <c r="N31" t="s">
+        <v>750</v>
+      </c>
+      <c r="P31" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>738</v>
+      </c>
+      <c r="B32" t="s">
+        <v>794</v>
+      </c>
+      <c r="D32" t="s">
+        <v>751</v>
+      </c>
+      <c r="E32" t="s">
+        <v>795</v>
+      </c>
+      <c r="F32" t="s">
+        <v>17</v>
+      </c>
+      <c r="G32" t="s">
+        <v>17</v>
+      </c>
+      <c r="N32" t="s">
+        <v>751</v>
+      </c>
+      <c r="P32" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>738</v>
+      </c>
+      <c r="B33" t="s">
+        <v>800</v>
+      </c>
+      <c r="D33" t="s">
+        <v>799</v>
+      </c>
+      <c r="E33" t="s">
+        <v>796</v>
+      </c>
+      <c r="F33" t="s">
+        <v>17</v>
+      </c>
+      <c r="G33" t="s">
+        <v>17</v>
+      </c>
+      <c r="N33" t="s">
+        <v>752</v>
+      </c>
+      <c r="P33" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>738</v>
+      </c>
+      <c r="B34" t="s">
+        <v>801</v>
+      </c>
+      <c r="D34" t="s">
+        <v>798</v>
+      </c>
+      <c r="E34" t="s">
+        <v>797</v>
+      </c>
+      <c r="F34" t="s">
+        <v>17</v>
+      </c>
+      <c r="G34" t="s">
+        <v>17</v>
+      </c>
+      <c r="P34" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>738</v>
+      </c>
+      <c r="B35" t="s">
+        <v>802</v>
+      </c>
+      <c r="D35" t="s">
+        <v>803</v>
+      </c>
+      <c r="E35" t="s">
+        <v>804</v>
+      </c>
+      <c r="F35" t="s">
+        <v>17</v>
+      </c>
+      <c r="G35" t="s">
+        <v>17</v>
+      </c>
+      <c r="N35" t="s">
         <v>753</v>
       </c>
-      <c r="F28" t="s">
-        <v>17</v>
-      </c>
-      <c r="G28" t="s">
-        <v>17</v>
-      </c>
-      <c r="N28" t="s">
-        <v>752</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>694</v>
-      </c>
-      <c r="B29" t="s">
-        <v>833</v>
-      </c>
-      <c r="D29" t="str">
-        <f t="shared" si="0"/>
-        <v>z_DEM_COM</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="P35" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>738</v>
+      </c>
+      <c r="B36" t="s">
+        <v>805</v>
+      </c>
+      <c r="D36" t="s">
+        <v>754</v>
+      </c>
+      <c r="E36" t="s">
+        <v>806</v>
+      </c>
+      <c r="F36" t="s">
+        <v>17</v>
+      </c>
+      <c r="G36" t="s">
+        <v>17</v>
+      </c>
+      <c r="N36" t="s">
+        <v>754</v>
+      </c>
+      <c r="P36" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>700</v>
+      </c>
+      <c r="B37" t="s">
+        <v>807</v>
+      </c>
+      <c r="D37" t="s">
+        <v>808</v>
+      </c>
+      <c r="E37" t="s">
+        <v>809</v>
+      </c>
+      <c r="F37" t="s">
+        <v>17</v>
+      </c>
+      <c r="G37" t="s">
+        <v>17</v>
+      </c>
+      <c r="N37" t="s">
         <v>755</v>
       </c>
-      <c r="F29" t="s">
-        <v>17</v>
-      </c>
-      <c r="G29" t="s">
-        <v>17</v>
-      </c>
-      <c r="N29" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>694</v>
-      </c>
-      <c r="B30" t="s">
-        <v>834</v>
-      </c>
-      <c r="D30" t="str">
-        <f t="shared" si="0"/>
-        <v>z_DEM_IND</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="P37" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>756</v>
+      </c>
+      <c r="B38" t="s">
         <v>757</v>
-      </c>
-      <c r="F30" t="s">
-        <v>17</v>
-      </c>
-      <c r="G30" t="s">
-        <v>17</v>
-      </c>
-      <c r="N30" t="s">
-        <v>756</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>446</v>
-      </c>
-      <c r="D31" t="str">
-        <f t="shared" si="0"/>
-        <v>z_DEM_RSD</v>
-      </c>
-      <c r="E31" t="s">
-        <v>759</v>
-      </c>
-      <c r="F31" t="s">
-        <v>17</v>
-      </c>
-      <c r="G31" t="s">
-        <v>17</v>
-      </c>
-      <c r="N31" t="s">
-        <v>758</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>694</v>
-      </c>
-      <c r="B32" t="s">
-        <v>835</v>
-      </c>
-      <c r="D32" t="str">
-        <f t="shared" si="0"/>
-        <v>z_DEM_TRA</v>
-      </c>
-      <c r="E32" t="s">
-        <v>761</v>
-      </c>
-      <c r="F32" t="s">
-        <v>17</v>
-      </c>
-      <c r="G32" t="s">
-        <v>17</v>
-      </c>
-      <c r="N32" t="s">
-        <v>760</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>694</v>
-      </c>
-      <c r="B33" t="s">
-        <v>685</v>
-      </c>
-      <c r="D33" t="str">
-        <f t="shared" si="0"/>
-        <v>z_DEMRHX</v>
-      </c>
-      <c r="E33" t="s">
-        <v>762</v>
-      </c>
-      <c r="F33" t="s">
-        <v>17</v>
-      </c>
-      <c r="G33" t="s">
-        <v>17</v>
-      </c>
-      <c r="N33" t="s">
-        <v>762</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>763</v>
-      </c>
-      <c r="D34" t="str">
-        <f t="shared" si="0"/>
-        <v>z_DM</v>
-      </c>
-      <c r="E34" t="s">
-        <v>764</v>
-      </c>
-      <c r="F34" t="s">
-        <v>17</v>
-      </c>
-      <c r="G34" t="s">
-        <v>17</v>
-      </c>
-      <c r="N34" t="s">
-        <v>764</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>746</v>
-      </c>
-      <c r="B35" t="s">
-        <v>747</v>
-      </c>
-      <c r="D35" t="str">
-        <f t="shared" si="0"/>
-        <v>z_ENV_CH4</v>
-      </c>
-      <c r="E35" t="s">
-        <v>765</v>
-      </c>
-      <c r="F35" t="s">
-        <v>17</v>
-      </c>
-      <c r="G35" t="s">
-        <v>17</v>
-      </c>
-      <c r="N35" t="s">
-        <v>765</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>746</v>
-      </c>
-      <c r="B36" t="s">
-        <v>766</v>
-      </c>
-      <c r="D36" t="str">
-        <f t="shared" si="0"/>
-        <v>z_ENV_CO2</v>
-      </c>
-      <c r="E36" t="s">
-        <v>767</v>
-      </c>
-      <c r="F36" t="s">
-        <v>17</v>
-      </c>
-      <c r="G36" t="s">
-        <v>17</v>
-      </c>
-      <c r="N36" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>746</v>
-      </c>
-      <c r="B37" t="s">
-        <v>768</v>
-      </c>
-      <c r="D37" t="str">
-        <f t="shared" si="0"/>
-        <v>z_ENV_COX</v>
-      </c>
-      <c r="E37" t="s">
-        <v>770</v>
-      </c>
-      <c r="F37" t="s">
-        <v>17</v>
-      </c>
-      <c r="G37" t="s">
-        <v>17</v>
-      </c>
-      <c r="N37" t="s">
-        <v>769</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>746</v>
-      </c>
-      <c r="B38" t="s">
-        <v>771</v>
       </c>
       <c r="D38" t="str">
         <f t="shared" si="0"/>
-        <v>z_ENV_N2O</v>
+        <v>z_FINREN</v>
       </c>
       <c r="E38" t="s">
-        <v>772</v>
+        <v>759</v>
       </c>
       <c r="F38" t="s">
         <v>17</v>
@@ -3779,22 +3806,22 @@
         <v>17</v>
       </c>
       <c r="N38" t="s">
-        <v>772</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>746</v>
+        <v>760</v>
       </c>
       <c r="B39" t="s">
-        <v>773</v>
+        <v>757</v>
       </c>
       <c r="D39" t="str">
         <f t="shared" si="0"/>
-        <v>z_ENV_NOX</v>
+        <v>z_FINREN-AGR</v>
       </c>
       <c r="E39" t="s">
-        <v>774</v>
+        <v>762</v>
       </c>
       <c r="F39" t="s">
         <v>17</v>
@@ -3803,22 +3830,22 @@
         <v>17</v>
       </c>
       <c r="N39" t="s">
-        <v>774</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>746</v>
+        <v>763</v>
       </c>
       <c r="B40" t="s">
-        <v>775</v>
+        <v>757</v>
       </c>
       <c r="D40" t="str">
         <f t="shared" si="0"/>
-        <v>z_ENV_PMX</v>
+        <v>z_FINREN-COM</v>
       </c>
       <c r="E40" t="s">
-        <v>776</v>
+        <v>765</v>
       </c>
       <c r="F40" t="s">
         <v>17</v>
@@ -3827,22 +3854,22 @@
         <v>17</v>
       </c>
       <c r="N40" t="s">
-        <v>776</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>746</v>
+        <v>766</v>
       </c>
       <c r="B41" t="s">
-        <v>777</v>
+        <v>767</v>
       </c>
       <c r="D41" t="str">
         <f t="shared" si="0"/>
-        <v>z_ENV_SOX</v>
+        <v>z_FINREN-IND</v>
       </c>
       <c r="E41" t="s">
-        <v>778</v>
+        <v>769</v>
       </c>
       <c r="F41" t="s">
         <v>17</v>
@@ -3851,22 +3878,22 @@
         <v>17</v>
       </c>
       <c r="N41" t="s">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>746</v>
+        <v>770</v>
       </c>
       <c r="B42" t="s">
-        <v>779</v>
+        <v>757</v>
       </c>
       <c r="D42" t="str">
         <f t="shared" si="0"/>
-        <v>z_ENV_VOC</v>
+        <v>z_FINREN-RSD</v>
       </c>
       <c r="E42" t="s">
-        <v>781</v>
+        <v>772</v>
       </c>
       <c r="F42" t="s">
         <v>17</v>
@@ -3875,19 +3902,22 @@
         <v>17</v>
       </c>
       <c r="N42" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>773</v>
+      </c>
       <c r="B43" t="s">
-        <v>782</v>
+        <v>757</v>
       </c>
       <c r="D43" t="str">
         <f t="shared" si="0"/>
-        <v>z_FINALELC</v>
+        <v>z_FINREN-TRA</v>
       </c>
       <c r="E43" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="F43" t="s">
         <v>17</v>
@@ -3896,22 +3926,21 @@
         <v>17</v>
       </c>
       <c r="N43" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>784</v>
+        <v>700</v>
       </c>
       <c r="B44" t="s">
-        <v>785</v>
-      </c>
-      <c r="D44" t="str">
-        <f t="shared" si="0"/>
-        <v>z_FINREN</v>
+        <v>74</v>
+      </c>
+      <c r="D44" t="s">
+        <v>760</v>
       </c>
       <c r="E44" t="s">
-        <v>787</v>
+        <v>810</v>
       </c>
       <c r="F44" t="s">
         <v>17</v>
@@ -3920,22 +3949,24 @@
         <v>17</v>
       </c>
       <c r="N44" t="s">
-        <v>786</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+        <v>760</v>
+      </c>
+      <c r="P44" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>788</v>
+        <v>700</v>
       </c>
       <c r="B45" t="s">
-        <v>785</v>
-      </c>
-      <c r="D45" t="str">
-        <f t="shared" si="0"/>
-        <v>z_FINREN-AGR</v>
+        <v>216</v>
+      </c>
+      <c r="D45" t="s">
+        <v>763</v>
       </c>
       <c r="E45" t="s">
-        <v>790</v>
+        <v>811</v>
       </c>
       <c r="F45" t="s">
         <v>17</v>
@@ -3944,22 +3975,24 @@
         <v>17</v>
       </c>
       <c r="N45" t="s">
+        <v>763</v>
+      </c>
+      <c r="P45" t="s">
         <v>789</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>791</v>
+        <v>700</v>
       </c>
       <c r="B46" t="s">
-        <v>785</v>
-      </c>
-      <c r="D46" t="str">
-        <f t="shared" si="0"/>
-        <v>z_FINREN-COM</v>
+        <v>816</v>
+      </c>
+      <c r="D46" t="s">
+        <v>776</v>
       </c>
       <c r="E46" t="s">
-        <v>793</v>
+        <v>817</v>
       </c>
       <c r="F46" t="s">
         <v>17</v>
@@ -3968,22 +4001,25 @@
         <v>17</v>
       </c>
       <c r="N46" t="s">
-        <v>792</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+        <v>776</v>
+      </c>
+      <c r="P46" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>794</v>
+        <v>732</v>
       </c>
       <c r="B47" t="s">
-        <v>795</v>
+        <v>556</v>
       </c>
       <c r="D47" t="str">
         <f t="shared" si="0"/>
-        <v>z_FINREN-IND</v>
+        <v>z_FUEELC-REN</v>
       </c>
       <c r="E47" t="s">
-        <v>797</v>
+        <v>778</v>
       </c>
       <c r="F47" t="s">
         <v>17</v>
@@ -3992,22 +4028,21 @@
         <v>17</v>
       </c>
       <c r="N47" t="s">
-        <v>796</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>798</v>
+        <v>700</v>
       </c>
       <c r="B48" t="s">
-        <v>785</v>
-      </c>
-      <c r="D48" t="str">
-        <f t="shared" si="0"/>
-        <v>z_FINREN-RSD</v>
+        <v>88</v>
+      </c>
+      <c r="D48" t="s">
+        <v>766</v>
       </c>
       <c r="E48" t="s">
-        <v>800</v>
+        <v>812</v>
       </c>
       <c r="F48" t="s">
         <v>17</v>
@@ -4016,22 +4051,24 @@
         <v>17</v>
       </c>
       <c r="N48" t="s">
-        <v>799</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+        <v>766</v>
+      </c>
+      <c r="P48" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>801</v>
+        <v>700</v>
       </c>
       <c r="B49" t="s">
-        <v>785</v>
-      </c>
-      <c r="D49" t="str">
-        <f t="shared" si="0"/>
-        <v>z_FINREN-TRA</v>
+        <v>237</v>
+      </c>
+      <c r="D49" t="s">
+        <v>770</v>
       </c>
       <c r="E49" t="s">
-        <v>803</v>
+        <v>813</v>
       </c>
       <c r="F49" t="s">
         <v>17</v>
@@ -4040,22 +4077,24 @@
         <v>17</v>
       </c>
       <c r="N49" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+        <v>770</v>
+      </c>
+      <c r="P49" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="B50" t="s">
-        <v>74</v>
-      </c>
-      <c r="D50" t="str">
-        <f t="shared" si="0"/>
-        <v>z_FUEAGR</v>
+        <v>243</v>
+      </c>
+      <c r="D50" t="s">
+        <v>779</v>
       </c>
       <c r="E50" t="s">
-        <v>68</v>
+        <v>814</v>
       </c>
       <c r="F50" t="s">
         <v>17</v>
@@ -4064,22 +4103,24 @@
         <v>17</v>
       </c>
       <c r="N50" t="s">
-        <v>788</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+        <v>779</v>
+      </c>
+      <c r="P50" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="B51" t="s">
-        <v>216</v>
-      </c>
-      <c r="D51" t="str">
-        <f t="shared" si="0"/>
-        <v>z_FUECOM</v>
+        <v>655</v>
+      </c>
+      <c r="D51" t="s">
+        <v>773</v>
       </c>
       <c r="E51" t="s">
-        <v>215</v>
+        <v>815</v>
       </c>
       <c r="F51" t="s">
         <v>17</v>
@@ -4088,22 +4129,24 @@
         <v>17</v>
       </c>
       <c r="N51" t="s">
-        <v>791</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+        <v>773</v>
+      </c>
+      <c r="P51" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="B52" t="s">
-        <v>804</v>
-      </c>
-      <c r="D52" t="str">
-        <f t="shared" si="0"/>
-        <v>z_FUEELC</v>
+        <v>780</v>
+      </c>
+      <c r="D52" t="s">
+        <v>781</v>
       </c>
       <c r="E52" t="s">
-        <v>350</v>
+        <v>782</v>
       </c>
       <c r="F52" t="s">
         <v>17</v>
@@ -4112,376 +4155,10 @@
         <v>17</v>
       </c>
       <c r="N52" t="s">
-        <v>805</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>806</v>
-      </c>
-      <c r="B53" t="s">
-        <v>142</v>
-      </c>
-      <c r="D53" t="str">
-        <f t="shared" si="0"/>
-        <v>z_FUEELC+ELC</v>
-      </c>
-      <c r="E53" t="s">
-        <v>350</v>
-      </c>
-      <c r="F53" t="s">
-        <v>17</v>
-      </c>
-      <c r="G53" t="s">
-        <v>17</v>
-      </c>
-      <c r="N53" t="s">
-        <v>807</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>740</v>
-      </c>
-      <c r="B54" t="s">
-        <v>556</v>
-      </c>
-      <c r="D54" t="str">
-        <f t="shared" si="0"/>
-        <v>z_FUEELC-REN</v>
-      </c>
-      <c r="E54" t="s">
-        <v>809</v>
-      </c>
-      <c r="F54" t="s">
-        <v>17</v>
-      </c>
-      <c r="G54" t="s">
-        <v>17</v>
-      </c>
-      <c r="N54" t="s">
-        <v>808</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>703</v>
-      </c>
-      <c r="B55" t="s">
-        <v>88</v>
-      </c>
-      <c r="D55" t="str">
-        <f t="shared" si="0"/>
-        <v>z_FUEIND</v>
-      </c>
-      <c r="E55" t="s">
-        <v>232</v>
-      </c>
-      <c r="F55" t="s">
-        <v>17</v>
-      </c>
-      <c r="G55" t="s">
-        <v>17</v>
-      </c>
-      <c r="N55" t="s">
-        <v>794</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>703</v>
-      </c>
-      <c r="B56" t="s">
-        <v>237</v>
-      </c>
-      <c r="D56" t="str">
-        <f t="shared" si="0"/>
-        <v>z_FUERSD</v>
-      </c>
-      <c r="E56" t="s">
-        <v>810</v>
-      </c>
-      <c r="F56" t="s">
-        <v>17</v>
-      </c>
-      <c r="G56" t="s">
-        <v>17</v>
-      </c>
-      <c r="N56" t="s">
-        <v>798</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>703</v>
-      </c>
-      <c r="B57" t="s">
-        <v>243</v>
-      </c>
-      <c r="D57" t="str">
-        <f t="shared" si="0"/>
-        <v>z_FUESUP</v>
-      </c>
-      <c r="E57" t="s">
-        <v>812</v>
-      </c>
-      <c r="F57" t="s">
-        <v>17</v>
-      </c>
-      <c r="G57" t="s">
-        <v>17</v>
-      </c>
-      <c r="N57" t="s">
-        <v>811</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>703</v>
-      </c>
-      <c r="B58" t="s">
-        <v>655</v>
-      </c>
-      <c r="D58" t="str">
-        <f t="shared" si="0"/>
-        <v>z_FUETRA</v>
-      </c>
-      <c r="E58" t="s">
-        <v>249</v>
-      </c>
-      <c r="F58" t="s">
-        <v>17</v>
-      </c>
-      <c r="G58" t="s">
-        <v>17</v>
-      </c>
-      <c r="N58" t="s">
-        <v>801</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
-        <v>813</v>
-      </c>
-      <c r="D59" t="str">
-        <f t="shared" si="0"/>
-        <v>z_INDHEAT</v>
-      </c>
-      <c r="E59" t="s">
-        <v>815</v>
-      </c>
-      <c r="F59" t="s">
-        <v>17</v>
-      </c>
-      <c r="G59" t="s">
-        <v>17</v>
-      </c>
-      <c r="N59" t="s">
-        <v>814</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>746</v>
-      </c>
-      <c r="B60" t="s">
-        <v>771</v>
-      </c>
-      <c r="D60" t="str">
-        <f t="shared" si="0"/>
-        <v>z_N2O</v>
-      </c>
-      <c r="E60" t="s">
-        <v>816</v>
-      </c>
-      <c r="F60" t="s">
-        <v>17</v>
-      </c>
-      <c r="G60" t="s">
-        <v>17</v>
-      </c>
-      <c r="N60" t="s">
-        <v>816</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>746</v>
-      </c>
-      <c r="B61" t="s">
-        <v>773</v>
-      </c>
-      <c r="D61" t="str">
-        <f t="shared" si="0"/>
-        <v>z_NOX</v>
-      </c>
-      <c r="E61" t="s">
-        <v>817</v>
-      </c>
-      <c r="F61" t="s">
-        <v>17</v>
-      </c>
-      <c r="G61" t="s">
-        <v>17</v>
-      </c>
-      <c r="N61" t="s">
-        <v>817</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>703</v>
-      </c>
-      <c r="B62" t="s">
-        <v>818</v>
-      </c>
-      <c r="D62" t="str">
-        <f t="shared" si="0"/>
-        <v>z_NRG-BFG</v>
-      </c>
-      <c r="E62" t="s">
-        <v>820</v>
-      </c>
-      <c r="F62" t="s">
-        <v>17</v>
-      </c>
-      <c r="G62" t="s">
-        <v>17</v>
-      </c>
-      <c r="N62" t="s">
-        <v>819</v>
-      </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>821</v>
-      </c>
-      <c r="D63" t="str">
-        <f t="shared" si="0"/>
-        <v>z_OCEAN</v>
-      </c>
-      <c r="E63" t="s">
-        <v>822</v>
-      </c>
-      <c r="F63" t="s">
-        <v>17</v>
-      </c>
-      <c r="G63" t="s">
-        <v>17</v>
-      </c>
-      <c r="N63" t="s">
-        <v>822</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
-        <v>823</v>
-      </c>
-      <c r="D64" t="str">
-        <f t="shared" si="0"/>
-        <v>z_OILRPPTRD</v>
-      </c>
-      <c r="E64" t="s">
-        <v>825</v>
-      </c>
-      <c r="F64" t="s">
-        <v>17</v>
-      </c>
-      <c r="G64" t="s">
-        <v>17</v>
-      </c>
-      <c r="N64" t="s">
-        <v>824</v>
-      </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>746</v>
-      </c>
-      <c r="B65" t="s">
-        <v>775</v>
-      </c>
-      <c r="D65" t="str">
-        <f t="shared" si="0"/>
-        <v>z_PMX</v>
-      </c>
-      <c r="E65" t="s">
-        <v>826</v>
-      </c>
-      <c r="F65" t="s">
-        <v>17</v>
-      </c>
-      <c r="G65" t="s">
-        <v>17</v>
-      </c>
-      <c r="N65" t="s">
-        <v>826</v>
-      </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
-        <v>446</v>
-      </c>
-      <c r="D66" t="str">
-        <f t="shared" si="0"/>
-        <v>z_RSD_DEM</v>
-      </c>
-      <c r="E66" t="s">
-        <v>759</v>
-      </c>
-      <c r="F66" t="s">
-        <v>17</v>
-      </c>
-      <c r="G66" t="s">
-        <v>17</v>
-      </c>
-      <c r="N66" t="s">
-        <v>827</v>
-      </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>746</v>
-      </c>
-      <c r="B67" t="s">
-        <v>777</v>
-      </c>
-      <c r="D67" t="str">
-        <f t="shared" si="0"/>
-        <v>z_SOX</v>
-      </c>
-      <c r="E67" t="s">
-        <v>828</v>
-      </c>
-      <c r="F67" t="s">
-        <v>17</v>
-      </c>
-      <c r="G67" t="s">
-        <v>17</v>
-      </c>
-      <c r="N67" t="s">
-        <v>828</v>
-      </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
-        <v>829</v>
-      </c>
-      <c r="D68" t="str">
-        <f t="shared" ref="D68" si="1">"z_"&amp;N68</f>
-        <v>z_TRAELC</v>
-      </c>
-      <c r="E68" t="s">
-        <v>350</v>
-      </c>
-      <c r="F68" t="s">
-        <v>17</v>
-      </c>
-      <c r="G68" t="s">
-        <v>17</v>
-      </c>
-      <c r="N68" t="s">
-        <v>830</v>
+        <v>781</v>
+      </c>
+      <c r="P52" t="s">
+        <v>789</v>
       </c>
     </row>
   </sheetData>
@@ -7537,7 +7214,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="130" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>681</v>
       </c>

</xml_diff>

<commit_message>
Add a few RSD sets and tables
</commit_message>
<xml_diff>
--- a/SetRules.xlsx
+++ b/SetRules.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E51E5B-8246-48E4-BEB3-898E07FF35C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14CE1F4A-4506-4B48-ADD5-C39B270BB1C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{69765015-6AAF-4B94-8956-691CCC759B47}"/>
   </bookViews>
   <sheets>
-    <sheet name="VEDA_Sets-Comm" sheetId="2" r:id="rId1"/>
+    <sheet name="VEDA_Sets-Comm" sheetId="5" r:id="rId1"/>
     <sheet name="extra_Sets-Comm" sheetId="3" r:id="rId2"/>
-    <sheet name="VEDA_Sets-Proc" sheetId="1" r:id="rId3"/>
+    <sheet name="VEDA_Sets-Proc" sheetId="6" r:id="rId3"/>
     <sheet name="extra_Sets-Proc" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2666" uniqueCount="1070">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2750" uniqueCount="1103">
   <si>
     <t>~TFM_Psets</t>
   </si>
@@ -3249,6 +3249,105 @@
   </si>
   <si>
     <t>Transport Train Long Distance</t>
+  </si>
+  <si>
+    <t>Residential Water Heating</t>
+  </si>
+  <si>
+    <t>RSD_NRGSRV-WH</t>
+  </si>
+  <si>
+    <t>R-WH*</t>
+  </si>
+  <si>
+    <t>Residential Space Heating</t>
+  </si>
+  <si>
+    <t>RSD_NRGSRV-SH</t>
+  </si>
+  <si>
+    <t>R-SH*</t>
+  </si>
+  <si>
+    <t>Residential Space Cooling</t>
+  </si>
+  <si>
+    <t>RSD_NRGSRV-SC</t>
+  </si>
+  <si>
+    <t>R-SC*</t>
+  </si>
+  <si>
+    <t>Residential Refrigeration</t>
+  </si>
+  <si>
+    <t>RSD_NRGSRV-RF</t>
+  </si>
+  <si>
+    <t>R-RSDRF*</t>
+  </si>
+  <si>
+    <t>Residential Pump and Fans</t>
+  </si>
+  <si>
+    <t>RSD_NRGSRV-PF</t>
+  </si>
+  <si>
+    <t>R-PF*</t>
+  </si>
+  <si>
+    <t>Residential Electric Appliances</t>
+  </si>
+  <si>
+    <t>RSD_NRGSRV-OE</t>
+  </si>
+  <si>
+    <t>R-RSDOE*</t>
+  </si>
+  <si>
+    <t>Residential Other Applications</t>
+  </si>
+  <si>
+    <t>RSD_NRGSRV-OA</t>
+  </si>
+  <si>
+    <t>R-RSDOA*</t>
+  </si>
+  <si>
+    <t>RSD_NRGSRV-LT</t>
+  </si>
+  <si>
+    <t>R-LT*</t>
+  </si>
+  <si>
+    <t>RSD_NRGSRV-DW</t>
+  </si>
+  <si>
+    <t>R-RSDDW*</t>
+  </si>
+  <si>
+    <t>Residential Cloth Washing</t>
+  </si>
+  <si>
+    <t>RSD_NRGSRV-CW</t>
+  </si>
+  <si>
+    <t>R-RSDCW*</t>
+  </si>
+  <si>
+    <t>RSD_NRGSRV-CK</t>
+  </si>
+  <si>
+    <t>R-RSDCK*</t>
+  </si>
+  <si>
+    <t>Residential Cloth Drying</t>
+  </si>
+  <si>
+    <t>RSD_NRGSRV-CD</t>
+  </si>
+  <si>
+    <t>R-RSDCD*</t>
   </si>
 </sst>
 </file>
@@ -3609,27 +3708,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9CE0C8F-B7C1-486F-ABA3-B5D6FFB88B6D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92FCDF15-1442-474A-ACC7-D199AB8A1E18}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -3670,16 +3759,16 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>242</v>
+        <v>278</v>
       </c>
       <c r="B3" t="s">
-        <v>243</v>
+        <v>279</v>
       </c>
       <c r="D3" t="s">
-        <v>116</v>
+        <v>184</v>
       </c>
       <c r="E3" t="s">
-        <v>117</v>
+        <v>185</v>
       </c>
       <c r="F3" t="s">
         <v>15</v>
@@ -3696,22 +3785,22 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>242</v>
+        <v>278</v>
       </c>
       <c r="B4" t="s">
-        <v>244</v>
+        <v>280</v>
       </c>
       <c r="D4" t="s">
-        <v>118</v>
+        <v>186</v>
       </c>
       <c r="E4" t="s">
-        <v>119</v>
+        <v>187</v>
       </c>
       <c r="F4" t="s">
         <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H4" t="s">
         <v>15</v>
@@ -3722,22 +3811,22 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>242</v>
+        <v>278</v>
       </c>
       <c r="B5" t="s">
-        <v>245</v>
+        <v>281</v>
       </c>
       <c r="D5" t="s">
-        <v>120</v>
+        <v>188</v>
       </c>
       <c r="E5" t="s">
-        <v>121</v>
+        <v>189</v>
       </c>
       <c r="F5" t="s">
         <v>15</v>
       </c>
       <c r="G5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H5" t="s">
         <v>15</v>
@@ -3748,22 +3837,22 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>242</v>
+        <v>278</v>
       </c>
       <c r="B6" t="s">
-        <v>246</v>
+        <v>282</v>
       </c>
       <c r="D6" t="s">
-        <v>122</v>
+        <v>190</v>
       </c>
       <c r="E6" t="s">
-        <v>123</v>
+        <v>191</v>
       </c>
       <c r="F6" t="s">
         <v>15</v>
       </c>
       <c r="G6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H6" t="s">
         <v>15</v>
@@ -3774,22 +3863,22 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>242</v>
+        <v>278</v>
       </c>
       <c r="B7" t="s">
-        <v>247</v>
+        <v>283</v>
       </c>
       <c r="D7" t="s">
-        <v>124</v>
+        <v>192</v>
       </c>
       <c r="E7" t="s">
-        <v>125</v>
+        <v>193</v>
       </c>
       <c r="F7" t="s">
         <v>15</v>
       </c>
       <c r="G7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H7" t="s">
         <v>15</v>
@@ -3803,19 +3892,19 @@
         <v>242</v>
       </c>
       <c r="B8" t="s">
-        <v>248</v>
+        <v>284</v>
       </c>
       <c r="D8" t="s">
-        <v>126</v>
+        <v>194</v>
       </c>
       <c r="E8" t="s">
-        <v>127</v>
+        <v>195</v>
       </c>
       <c r="F8" t="s">
         <v>15</v>
       </c>
       <c r="G8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H8" t="s">
         <v>15</v>
@@ -3829,13 +3918,13 @@
         <v>242</v>
       </c>
       <c r="B9" t="s">
-        <v>249</v>
+        <v>285</v>
       </c>
       <c r="D9" t="s">
-        <v>128</v>
+        <v>196</v>
       </c>
       <c r="E9" t="s">
-        <v>129</v>
+        <v>197</v>
       </c>
       <c r="F9" t="s">
         <v>15</v>
@@ -3855,13 +3944,13 @@
         <v>242</v>
       </c>
       <c r="B10" t="s">
-        <v>250</v>
+        <v>286</v>
       </c>
       <c r="D10" t="s">
-        <v>130</v>
+        <v>198</v>
       </c>
       <c r="E10" t="s">
-        <v>131</v>
+        <v>199</v>
       </c>
       <c r="F10" t="s">
         <v>15</v>
@@ -3881,19 +3970,19 @@
         <v>242</v>
       </c>
       <c r="B11" t="s">
-        <v>251</v>
+        <v>287</v>
       </c>
       <c r="D11" t="s">
-        <v>132</v>
+        <v>200</v>
       </c>
       <c r="E11" t="s">
-        <v>133</v>
+        <v>201</v>
       </c>
       <c r="F11" t="s">
         <v>15</v>
       </c>
       <c r="G11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H11" t="s">
         <v>15</v>
@@ -3907,13 +3996,13 @@
         <v>242</v>
       </c>
       <c r="B12" t="s">
-        <v>252</v>
+        <v>288</v>
       </c>
       <c r="D12" t="s">
-        <v>134</v>
+        <v>202</v>
       </c>
       <c r="E12" t="s">
-        <v>135</v>
+        <v>203</v>
       </c>
       <c r="F12" t="s">
         <v>15</v>
@@ -3933,13 +4022,13 @@
         <v>242</v>
       </c>
       <c r="B13" t="s">
-        <v>253</v>
+        <v>289</v>
       </c>
       <c r="D13" t="s">
-        <v>136</v>
+        <v>204</v>
       </c>
       <c r="E13" t="s">
-        <v>137</v>
+        <v>205</v>
       </c>
       <c r="F13" t="s">
         <v>15</v>
@@ -3959,13 +4048,13 @@
         <v>242</v>
       </c>
       <c r="B14" t="s">
-        <v>254</v>
+        <v>290</v>
       </c>
       <c r="D14" t="s">
-        <v>138</v>
+        <v>206</v>
       </c>
       <c r="E14" t="s">
-        <v>139</v>
+        <v>207</v>
       </c>
       <c r="F14" t="s">
         <v>15</v>
@@ -3985,13 +4074,13 @@
         <v>242</v>
       </c>
       <c r="B15" t="s">
-        <v>255</v>
+        <v>291</v>
       </c>
       <c r="D15" t="s">
-        <v>140</v>
+        <v>208</v>
       </c>
       <c r="E15" t="s">
-        <v>141</v>
+        <v>209</v>
       </c>
       <c r="F15" t="s">
         <v>15</v>
@@ -4011,19 +4100,19 @@
         <v>242</v>
       </c>
       <c r="B16" t="s">
-        <v>256</v>
+        <v>292</v>
       </c>
       <c r="D16" t="s">
-        <v>142</v>
+        <v>210</v>
       </c>
       <c r="E16" t="s">
-        <v>143</v>
+        <v>211</v>
       </c>
       <c r="F16" t="s">
         <v>15</v>
       </c>
       <c r="G16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H16" t="s">
         <v>15</v>
@@ -4037,13 +4126,13 @@
         <v>242</v>
       </c>
       <c r="B17" t="s">
-        <v>257</v>
+        <v>293</v>
       </c>
       <c r="D17" t="s">
-        <v>144</v>
+        <v>212</v>
       </c>
       <c r="E17" t="s">
-        <v>145</v>
+        <v>213</v>
       </c>
       <c r="F17" t="s">
         <v>15</v>
@@ -4063,13 +4152,13 @@
         <v>242</v>
       </c>
       <c r="B18" t="s">
-        <v>258</v>
+        <v>294</v>
       </c>
       <c r="D18" t="s">
-        <v>146</v>
+        <v>214</v>
       </c>
       <c r="E18" t="s">
-        <v>147</v>
+        <v>215</v>
       </c>
       <c r="F18" t="s">
         <v>15</v>
@@ -4089,19 +4178,19 @@
         <v>242</v>
       </c>
       <c r="B19" t="s">
-        <v>259</v>
+        <v>295</v>
       </c>
       <c r="D19" t="s">
-        <v>148</v>
+        <v>216</v>
       </c>
       <c r="E19" t="s">
-        <v>149</v>
+        <v>217</v>
       </c>
       <c r="F19" t="s">
         <v>15</v>
       </c>
       <c r="G19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H19" t="s">
         <v>15</v>
@@ -4115,13 +4204,13 @@
         <v>242</v>
       </c>
       <c r="B20" t="s">
-        <v>260</v>
+        <v>296</v>
       </c>
       <c r="D20" t="s">
-        <v>150</v>
+        <v>218</v>
       </c>
       <c r="E20" t="s">
-        <v>151</v>
+        <v>219</v>
       </c>
       <c r="F20" t="s">
         <v>15</v>
@@ -4141,13 +4230,13 @@
         <v>242</v>
       </c>
       <c r="B21" t="s">
-        <v>261</v>
+        <v>297</v>
       </c>
       <c r="D21" t="s">
-        <v>152</v>
+        <v>220</v>
       </c>
       <c r="E21" t="s">
-        <v>153</v>
+        <v>221</v>
       </c>
       <c r="F21" t="s">
         <v>15</v>
@@ -4167,13 +4256,13 @@
         <v>242</v>
       </c>
       <c r="B22" t="s">
-        <v>262</v>
+        <v>298</v>
       </c>
       <c r="D22" t="s">
-        <v>154</v>
+        <v>222</v>
       </c>
       <c r="E22" t="s">
-        <v>155</v>
+        <v>223</v>
       </c>
       <c r="F22" t="s">
         <v>15</v>
@@ -4193,13 +4282,13 @@
         <v>242</v>
       </c>
       <c r="B23" t="s">
-        <v>263</v>
+        <v>299</v>
       </c>
       <c r="D23" t="s">
-        <v>156</v>
+        <v>224</v>
       </c>
       <c r="E23" t="s">
-        <v>157</v>
+        <v>225</v>
       </c>
       <c r="F23" t="s">
         <v>15</v>
@@ -4219,19 +4308,19 @@
         <v>242</v>
       </c>
       <c r="B24" t="s">
-        <v>264</v>
+        <v>300</v>
       </c>
       <c r="D24" t="s">
-        <v>158</v>
+        <v>226</v>
       </c>
       <c r="E24" t="s">
-        <v>159</v>
+        <v>227</v>
       </c>
       <c r="F24" t="s">
         <v>15</v>
       </c>
       <c r="G24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H24" t="s">
         <v>15</v>
@@ -4245,13 +4334,13 @@
         <v>242</v>
       </c>
       <c r="B25" t="s">
-        <v>265</v>
+        <v>301</v>
       </c>
       <c r="D25" t="s">
-        <v>160</v>
+        <v>228</v>
       </c>
       <c r="E25" t="s">
-        <v>161</v>
+        <v>229</v>
       </c>
       <c r="F25" t="s">
         <v>15</v>
@@ -4271,13 +4360,13 @@
         <v>242</v>
       </c>
       <c r="B26" t="s">
-        <v>266</v>
+        <v>302</v>
       </c>
       <c r="D26" t="s">
-        <v>162</v>
+        <v>230</v>
       </c>
       <c r="E26" t="s">
-        <v>163</v>
+        <v>231</v>
       </c>
       <c r="F26" t="s">
         <v>15</v>
@@ -4297,19 +4386,19 @@
         <v>242</v>
       </c>
       <c r="B27" t="s">
-        <v>267</v>
+        <v>303</v>
       </c>
       <c r="D27" t="s">
-        <v>164</v>
+        <v>232</v>
       </c>
       <c r="E27" t="s">
-        <v>165</v>
+        <v>233</v>
       </c>
       <c r="F27" t="s">
         <v>15</v>
       </c>
       <c r="G27" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H27" t="s">
         <v>15</v>
@@ -4323,13 +4412,13 @@
         <v>242</v>
       </c>
       <c r="B28" t="s">
-        <v>268</v>
+        <v>304</v>
       </c>
       <c r="D28" t="s">
-        <v>166</v>
+        <v>234</v>
       </c>
       <c r="E28" t="s">
-        <v>167</v>
+        <v>235</v>
       </c>
       <c r="F28" t="s">
         <v>15</v>
@@ -4349,13 +4438,13 @@
         <v>242</v>
       </c>
       <c r="B29" t="s">
-        <v>269</v>
+        <v>305</v>
       </c>
       <c r="D29" t="s">
-        <v>168</v>
+        <v>236</v>
       </c>
       <c r="E29" t="s">
-        <v>169</v>
+        <v>237</v>
       </c>
       <c r="F29" t="s">
         <v>15</v>
@@ -4375,13 +4464,13 @@
         <v>242</v>
       </c>
       <c r="B30" t="s">
-        <v>270</v>
+        <v>306</v>
       </c>
       <c r="D30" t="s">
-        <v>170</v>
+        <v>238</v>
       </c>
       <c r="E30" t="s">
-        <v>171</v>
+        <v>239</v>
       </c>
       <c r="F30" t="s">
         <v>15</v>
@@ -4401,13 +4490,13 @@
         <v>242</v>
       </c>
       <c r="B31" t="s">
-        <v>271</v>
+        <v>307</v>
       </c>
       <c r="D31" t="s">
-        <v>172</v>
+        <v>240</v>
       </c>
       <c r="E31" t="s">
-        <v>173</v>
+        <v>241</v>
       </c>
       <c r="F31" t="s">
         <v>15</v>
@@ -4427,19 +4516,19 @@
         <v>242</v>
       </c>
       <c r="B32" t="s">
-        <v>272</v>
+        <v>243</v>
       </c>
       <c r="D32" t="s">
-        <v>174</v>
+        <v>116</v>
       </c>
       <c r="E32" t="s">
-        <v>175</v>
+        <v>117</v>
       </c>
       <c r="F32" t="s">
         <v>15</v>
       </c>
       <c r="G32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H32" t="s">
         <v>15</v>
@@ -4453,13 +4542,13 @@
         <v>242</v>
       </c>
       <c r="B33" t="s">
-        <v>273</v>
+        <v>244</v>
       </c>
       <c r="D33" t="s">
-        <v>176</v>
+        <v>118</v>
       </c>
       <c r="E33" t="s">
-        <v>177</v>
+        <v>119</v>
       </c>
       <c r="F33" t="s">
         <v>15</v>
@@ -4479,13 +4568,13 @@
         <v>242</v>
       </c>
       <c r="B34" t="s">
-        <v>274</v>
+        <v>245</v>
       </c>
       <c r="D34" t="s">
-        <v>178</v>
+        <v>120</v>
       </c>
       <c r="E34" t="s">
-        <v>179</v>
+        <v>121</v>
       </c>
       <c r="F34" t="s">
         <v>15</v>
@@ -4505,19 +4594,19 @@
         <v>242</v>
       </c>
       <c r="B35" t="s">
-        <v>275</v>
+        <v>246</v>
       </c>
       <c r="D35" t="s">
-        <v>180</v>
+        <v>122</v>
       </c>
       <c r="E35" t="s">
-        <v>181</v>
+        <v>123</v>
       </c>
       <c r="F35" t="s">
         <v>15</v>
       </c>
       <c r="G35" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H35" t="s">
         <v>15</v>
@@ -4528,16 +4617,16 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>276</v>
+        <v>242</v>
       </c>
       <c r="B36" t="s">
-        <v>277</v>
+        <v>247</v>
       </c>
       <c r="D36" t="s">
-        <v>182</v>
+        <v>124</v>
       </c>
       <c r="E36" t="s">
-        <v>183</v>
+        <v>125</v>
       </c>
       <c r="F36" t="s">
         <v>15</v>
@@ -4554,22 +4643,22 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>278</v>
+        <v>242</v>
       </c>
       <c r="B37" t="s">
-        <v>279</v>
+        <v>248</v>
       </c>
       <c r="D37" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
       <c r="E37" t="s">
-        <v>185</v>
+        <v>127</v>
       </c>
       <c r="F37" t="s">
         <v>15</v>
       </c>
       <c r="G37" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H37" t="s">
         <v>15</v>
@@ -4580,22 +4669,22 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>278</v>
+        <v>242</v>
       </c>
       <c r="B38" t="s">
-        <v>280</v>
+        <v>249</v>
       </c>
       <c r="D38" t="s">
-        <v>186</v>
+        <v>128</v>
       </c>
       <c r="E38" t="s">
-        <v>187</v>
+        <v>129</v>
       </c>
       <c r="F38" t="s">
         <v>15</v>
       </c>
       <c r="G38" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H38" t="s">
         <v>15</v>
@@ -4606,22 +4695,22 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>278</v>
+        <v>242</v>
       </c>
       <c r="B39" t="s">
-        <v>281</v>
+        <v>250</v>
       </c>
       <c r="D39" t="s">
-        <v>188</v>
+        <v>130</v>
       </c>
       <c r="E39" t="s">
-        <v>189</v>
+        <v>131</v>
       </c>
       <c r="F39" t="s">
         <v>15</v>
       </c>
       <c r="G39" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H39" t="s">
         <v>15</v>
@@ -4632,16 +4721,16 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>278</v>
+        <v>242</v>
       </c>
       <c r="B40" t="s">
-        <v>282</v>
+        <v>251</v>
       </c>
       <c r="D40" t="s">
-        <v>190</v>
+        <v>132</v>
       </c>
       <c r="E40" t="s">
-        <v>191</v>
+        <v>133</v>
       </c>
       <c r="F40" t="s">
         <v>15</v>
@@ -4658,22 +4747,22 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>278</v>
+        <v>242</v>
       </c>
       <c r="B41" t="s">
-        <v>283</v>
+        <v>252</v>
       </c>
       <c r="D41" t="s">
-        <v>192</v>
+        <v>134</v>
       </c>
       <c r="E41" t="s">
-        <v>193</v>
+        <v>135</v>
       </c>
       <c r="F41" t="s">
         <v>15</v>
       </c>
       <c r="G41" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H41" t="s">
         <v>15</v>
@@ -4687,19 +4776,19 @@
         <v>242</v>
       </c>
       <c r="B42" t="s">
-        <v>284</v>
+        <v>253</v>
       </c>
       <c r="D42" t="s">
-        <v>194</v>
+        <v>136</v>
       </c>
       <c r="E42" t="s">
-        <v>195</v>
+        <v>137</v>
       </c>
       <c r="F42" t="s">
         <v>15</v>
       </c>
       <c r="G42" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H42" t="s">
         <v>15</v>
@@ -4713,13 +4802,13 @@
         <v>242</v>
       </c>
       <c r="B43" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="D43" t="s">
-        <v>196</v>
+        <v>138</v>
       </c>
       <c r="E43" t="s">
-        <v>197</v>
+        <v>139</v>
       </c>
       <c r="F43" t="s">
         <v>15</v>
@@ -4739,13 +4828,13 @@
         <v>242</v>
       </c>
       <c r="B44" t="s">
-        <v>286</v>
+        <v>255</v>
       </c>
       <c r="D44" t="s">
-        <v>198</v>
+        <v>140</v>
       </c>
       <c r="E44" t="s">
-        <v>199</v>
+        <v>141</v>
       </c>
       <c r="F44" t="s">
         <v>15</v>
@@ -4765,13 +4854,13 @@
         <v>242</v>
       </c>
       <c r="B45" t="s">
-        <v>287</v>
+        <v>256</v>
       </c>
       <c r="D45" t="s">
-        <v>200</v>
+        <v>142</v>
       </c>
       <c r="E45" t="s">
-        <v>201</v>
+        <v>143</v>
       </c>
       <c r="F45" t="s">
         <v>15</v>
@@ -4791,13 +4880,13 @@
         <v>242</v>
       </c>
       <c r="B46" t="s">
-        <v>288</v>
+        <v>257</v>
       </c>
       <c r="D46" t="s">
-        <v>202</v>
+        <v>144</v>
       </c>
       <c r="E46" t="s">
-        <v>203</v>
+        <v>145</v>
       </c>
       <c r="F46" t="s">
         <v>15</v>
@@ -4817,13 +4906,13 @@
         <v>242</v>
       </c>
       <c r="B47" t="s">
-        <v>289</v>
+        <v>258</v>
       </c>
       <c r="D47" t="s">
-        <v>204</v>
+        <v>146</v>
       </c>
       <c r="E47" t="s">
-        <v>205</v>
+        <v>147</v>
       </c>
       <c r="F47" t="s">
         <v>15</v>
@@ -4843,19 +4932,19 @@
         <v>242</v>
       </c>
       <c r="B48" t="s">
-        <v>290</v>
+        <v>259</v>
       </c>
       <c r="D48" t="s">
-        <v>206</v>
+        <v>148</v>
       </c>
       <c r="E48" t="s">
-        <v>207</v>
+        <v>149</v>
       </c>
       <c r="F48" t="s">
         <v>15</v>
       </c>
       <c r="G48" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H48" t="s">
         <v>15</v>
@@ -4869,13 +4958,13 @@
         <v>242</v>
       </c>
       <c r="B49" t="s">
-        <v>291</v>
+        <v>260</v>
       </c>
       <c r="D49" t="s">
-        <v>208</v>
+        <v>150</v>
       </c>
       <c r="E49" t="s">
-        <v>209</v>
+        <v>151</v>
       </c>
       <c r="F49" t="s">
         <v>15</v>
@@ -4895,19 +4984,19 @@
         <v>242</v>
       </c>
       <c r="B50" t="s">
-        <v>292</v>
+        <v>261</v>
       </c>
       <c r="D50" t="s">
-        <v>210</v>
+        <v>152</v>
       </c>
       <c r="E50" t="s">
-        <v>211</v>
+        <v>153</v>
       </c>
       <c r="F50" t="s">
         <v>15</v>
       </c>
       <c r="G50" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H50" t="s">
         <v>15</v>
@@ -4921,13 +5010,13 @@
         <v>242</v>
       </c>
       <c r="B51" t="s">
-        <v>293</v>
+        <v>262</v>
       </c>
       <c r="D51" t="s">
-        <v>212</v>
+        <v>154</v>
       </c>
       <c r="E51" t="s">
-        <v>213</v>
+        <v>155</v>
       </c>
       <c r="F51" t="s">
         <v>15</v>
@@ -4947,13 +5036,13 @@
         <v>242</v>
       </c>
       <c r="B52" t="s">
-        <v>294</v>
+        <v>263</v>
       </c>
       <c r="D52" t="s">
-        <v>214</v>
+        <v>156</v>
       </c>
       <c r="E52" t="s">
-        <v>215</v>
+        <v>157</v>
       </c>
       <c r="F52" t="s">
         <v>15</v>
@@ -4973,13 +5062,13 @@
         <v>242</v>
       </c>
       <c r="B53" t="s">
-        <v>295</v>
+        <v>264</v>
       </c>
       <c r="D53" t="s">
-        <v>216</v>
+        <v>158</v>
       </c>
       <c r="E53" t="s">
-        <v>217</v>
+        <v>159</v>
       </c>
       <c r="F53" t="s">
         <v>15</v>
@@ -4999,13 +5088,13 @@
         <v>242</v>
       </c>
       <c r="B54" t="s">
-        <v>296</v>
+        <v>265</v>
       </c>
       <c r="D54" t="s">
-        <v>218</v>
+        <v>160</v>
       </c>
       <c r="E54" t="s">
-        <v>219</v>
+        <v>161</v>
       </c>
       <c r="F54" t="s">
         <v>15</v>
@@ -5025,13 +5114,13 @@
         <v>242</v>
       </c>
       <c r="B55" t="s">
-        <v>297</v>
+        <v>266</v>
       </c>
       <c r="D55" t="s">
-        <v>220</v>
+        <v>162</v>
       </c>
       <c r="E55" t="s">
-        <v>221</v>
+        <v>163</v>
       </c>
       <c r="F55" t="s">
         <v>15</v>
@@ -5051,19 +5140,19 @@
         <v>242</v>
       </c>
       <c r="B56" t="s">
-        <v>298</v>
+        <v>267</v>
       </c>
       <c r="D56" t="s">
-        <v>222</v>
+        <v>164</v>
       </c>
       <c r="E56" t="s">
-        <v>223</v>
+        <v>165</v>
       </c>
       <c r="F56" t="s">
         <v>15</v>
       </c>
       <c r="G56" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H56" t="s">
         <v>15</v>
@@ -5077,13 +5166,13 @@
         <v>242</v>
       </c>
       <c r="B57" t="s">
-        <v>299</v>
+        <v>268</v>
       </c>
       <c r="D57" t="s">
-        <v>224</v>
+        <v>166</v>
       </c>
       <c r="E57" t="s">
-        <v>225</v>
+        <v>167</v>
       </c>
       <c r="F57" t="s">
         <v>15</v>
@@ -5103,19 +5192,19 @@
         <v>242</v>
       </c>
       <c r="B58" t="s">
-        <v>300</v>
+        <v>269</v>
       </c>
       <c r="D58" t="s">
-        <v>226</v>
+        <v>168</v>
       </c>
       <c r="E58" t="s">
-        <v>227</v>
+        <v>169</v>
       </c>
       <c r="F58" t="s">
         <v>15</v>
       </c>
       <c r="G58" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H58" t="s">
         <v>15</v>
@@ -5129,13 +5218,13 @@
         <v>242</v>
       </c>
       <c r="B59" t="s">
-        <v>301</v>
+        <v>270</v>
       </c>
       <c r="D59" t="s">
-        <v>228</v>
+        <v>170</v>
       </c>
       <c r="E59" t="s">
-        <v>229</v>
+        <v>171</v>
       </c>
       <c r="F59" t="s">
         <v>15</v>
@@ -5155,13 +5244,13 @@
         <v>242</v>
       </c>
       <c r="B60" t="s">
-        <v>302</v>
+        <v>271</v>
       </c>
       <c r="D60" t="s">
-        <v>230</v>
+        <v>172</v>
       </c>
       <c r="E60" t="s">
-        <v>231</v>
+        <v>173</v>
       </c>
       <c r="F60" t="s">
         <v>15</v>
@@ -5181,13 +5270,13 @@
         <v>242</v>
       </c>
       <c r="B61" t="s">
-        <v>303</v>
+        <v>272</v>
       </c>
       <c r="D61" t="s">
-        <v>232</v>
+        <v>174</v>
       </c>
       <c r="E61" t="s">
-        <v>233</v>
+        <v>175</v>
       </c>
       <c r="F61" t="s">
         <v>15</v>
@@ -5207,13 +5296,13 @@
         <v>242</v>
       </c>
       <c r="B62" t="s">
-        <v>304</v>
+        <v>273</v>
       </c>
       <c r="D62" t="s">
-        <v>234</v>
+        <v>176</v>
       </c>
       <c r="E62" t="s">
-        <v>235</v>
+        <v>177</v>
       </c>
       <c r="F62" t="s">
         <v>15</v>
@@ -5233,13 +5322,13 @@
         <v>242</v>
       </c>
       <c r="B63" t="s">
-        <v>305</v>
+        <v>274</v>
       </c>
       <c r="D63" t="s">
-        <v>236</v>
+        <v>178</v>
       </c>
       <c r="E63" t="s">
-        <v>237</v>
+        <v>179</v>
       </c>
       <c r="F63" t="s">
         <v>15</v>
@@ -5259,19 +5348,19 @@
         <v>242</v>
       </c>
       <c r="B64" t="s">
-        <v>306</v>
+        <v>275</v>
       </c>
       <c r="D64" t="s">
-        <v>238</v>
+        <v>180</v>
       </c>
       <c r="E64" t="s">
-        <v>239</v>
+        <v>181</v>
       </c>
       <c r="F64" t="s">
         <v>15</v>
       </c>
       <c r="G64" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H64" t="s">
         <v>15</v>
@@ -5282,16 +5371,16 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>242</v>
+        <v>276</v>
       </c>
       <c r="B65" t="s">
-        <v>307</v>
+        <v>277</v>
       </c>
       <c r="D65" t="s">
-        <v>240</v>
+        <v>182</v>
       </c>
       <c r="E65" t="s">
-        <v>241</v>
+        <v>183</v>
       </c>
       <c r="F65" t="s">
         <v>15</v>
@@ -5315,8 +5404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0CB6C28-EC74-4923-AA3E-E780416BCEAF}">
   <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6660,30 +6749,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA82158A-CD0E-4DF6-A2AF-F14CC1280C79}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24231217-6A54-4B12-AA31-B59CB94B1CCE}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="41" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.85546875" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -7463,7 +7539,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>104</v>
       </c>
@@ -7480,7 +7556,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>105</v>
       </c>
@@ -7497,7 +7573,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>106</v>
       </c>
@@ -7514,7 +7590,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>107</v>
       </c>
@@ -7528,6 +7604,282 @@
         <v>15</v>
       </c>
       <c r="I36" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>1102</v>
+      </c>
+      <c r="F37" t="s">
+        <v>1101</v>
+      </c>
+      <c r="G37" t="s">
+        <v>1100</v>
+      </c>
+      <c r="H37" t="s">
+        <v>15</v>
+      </c>
+      <c r="I37" t="s">
+        <v>16</v>
+      </c>
+      <c r="J37" t="s">
+        <v>15</v>
+      </c>
+      <c r="K37" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>1099</v>
+      </c>
+      <c r="F38" t="s">
+        <v>1098</v>
+      </c>
+      <c r="G38" t="s">
+        <v>878</v>
+      </c>
+      <c r="H38" t="s">
+        <v>15</v>
+      </c>
+      <c r="I38" t="s">
+        <v>16</v>
+      </c>
+      <c r="J38" t="s">
+        <v>15</v>
+      </c>
+      <c r="K38" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>1097</v>
+      </c>
+      <c r="F39" t="s">
+        <v>1096</v>
+      </c>
+      <c r="G39" t="s">
+        <v>1095</v>
+      </c>
+      <c r="H39" t="s">
+        <v>15</v>
+      </c>
+      <c r="I39" t="s">
+        <v>16</v>
+      </c>
+      <c r="J39" t="s">
+        <v>15</v>
+      </c>
+      <c r="K39" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>1094</v>
+      </c>
+      <c r="F40" t="s">
+        <v>1093</v>
+      </c>
+      <c r="G40" t="s">
+        <v>883</v>
+      </c>
+      <c r="H40" t="s">
+        <v>15</v>
+      </c>
+      <c r="I40" t="s">
+        <v>16</v>
+      </c>
+      <c r="J40" t="s">
+        <v>15</v>
+      </c>
+      <c r="K40" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>1092</v>
+      </c>
+      <c r="F41" t="s">
+        <v>1091</v>
+      </c>
+      <c r="G41" t="s">
+        <v>919</v>
+      </c>
+      <c r="H41" t="s">
+        <v>15</v>
+      </c>
+      <c r="I41" t="s">
+        <v>16</v>
+      </c>
+      <c r="J41" t="s">
+        <v>15</v>
+      </c>
+      <c r="K41" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>1090</v>
+      </c>
+      <c r="F42" t="s">
+        <v>1089</v>
+      </c>
+      <c r="G42" t="s">
+        <v>1088</v>
+      </c>
+      <c r="H42" t="s">
+        <v>15</v>
+      </c>
+      <c r="I42" t="s">
+        <v>16</v>
+      </c>
+      <c r="J42" t="s">
+        <v>15</v>
+      </c>
+      <c r="K42" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F43" t="s">
+        <v>1086</v>
+      </c>
+      <c r="G43" t="s">
+        <v>1085</v>
+      </c>
+      <c r="H43" t="s">
+        <v>15</v>
+      </c>
+      <c r="I43" t="s">
+        <v>16</v>
+      </c>
+      <c r="J43" t="s">
+        <v>15</v>
+      </c>
+      <c r="K43" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>1084</v>
+      </c>
+      <c r="F44" t="s">
+        <v>1083</v>
+      </c>
+      <c r="G44" t="s">
+        <v>1082</v>
+      </c>
+      <c r="H44" t="s">
+        <v>15</v>
+      </c>
+      <c r="I44" t="s">
+        <v>16</v>
+      </c>
+      <c r="J44" t="s">
+        <v>15</v>
+      </c>
+      <c r="K44" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>1081</v>
+      </c>
+      <c r="F45" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G45" t="s">
+        <v>1079</v>
+      </c>
+      <c r="H45" t="s">
+        <v>15</v>
+      </c>
+      <c r="I45" t="s">
+        <v>16</v>
+      </c>
+      <c r="J45" t="s">
+        <v>15</v>
+      </c>
+      <c r="K45" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>1078</v>
+      </c>
+      <c r="F46" t="s">
+        <v>1077</v>
+      </c>
+      <c r="G46" t="s">
+        <v>1076</v>
+      </c>
+      <c r="H46" t="s">
+        <v>15</v>
+      </c>
+      <c r="I46" t="s">
+        <v>16</v>
+      </c>
+      <c r="J46" t="s">
+        <v>15</v>
+      </c>
+      <c r="K46" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>1075</v>
+      </c>
+      <c r="F47" t="s">
+        <v>1074</v>
+      </c>
+      <c r="G47" t="s">
+        <v>1073</v>
+      </c>
+      <c r="H47" t="s">
+        <v>15</v>
+      </c>
+      <c r="I47" t="s">
+        <v>16</v>
+      </c>
+      <c r="J47" t="s">
+        <v>15</v>
+      </c>
+      <c r="K47" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>1072</v>
+      </c>
+      <c r="F48" t="s">
+        <v>1071</v>
+      </c>
+      <c r="G48" t="s">
+        <v>1070</v>
+      </c>
+      <c r="H48" t="s">
+        <v>15</v>
+      </c>
+      <c r="I48" t="s">
+        <v>16</v>
+      </c>
+      <c r="J48" t="s">
+        <v>15</v>
+      </c>
+      <c r="K48" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update sets and tables
</commit_message>
<xml_diff>
--- a/SetRules.xlsx
+++ b/SetRules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFCDA325-BD6E-4C46-8565-B993B8AF904B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8290EA1A-A870-47CB-AB10-933367BDC2B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="870" windowWidth="20670" windowHeight="11385" activeTab="2" xr2:uid="{69765015-6AAF-4B94-8956-691CCC759B47}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{69765015-6AAF-4B94-8956-691CCC759B47}"/>
   </bookViews>
   <sheets>
     <sheet name="VEDA_Sets-Comm" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2750" uniqueCount="1103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2759" uniqueCount="1106">
   <si>
     <t>~TFM_Psets</t>
   </si>
@@ -3348,6 +3348,15 @@
   </si>
   <si>
     <t>TRAF*</t>
+  </si>
+  <si>
+    <t>T-MGT*</t>
+  </si>
+  <si>
+    <t>DMD_TRA-F-MTRUCK</t>
+  </si>
+  <si>
+    <t>Freight transport - medium goods truck</t>
   </si>
 </sst>
 </file>
@@ -6753,10 +6762,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:L48"/>
+  <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6900,16 +6909,16 @@
         <v>73</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>1103</v>
       </c>
       <c r="E6" t="s">
         <v>1102</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>1104</v>
       </c>
       <c r="G6" t="s">
-        <v>22</v>
+        <v>1105</v>
       </c>
       <c r="H6" t="s">
         <v>15</v>
@@ -6929,16 +6938,16 @@
         <v>73</v>
       </c>
       <c r="B7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E7" t="s">
-        <v>79</v>
+        <v>1102</v>
       </c>
       <c r="F7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H7" t="s">
         <v>15</v>
@@ -6958,16 +6967,16 @@
         <v>73</v>
       </c>
       <c r="B8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E8" t="s">
         <v>79</v>
       </c>
       <c r="F8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H8" t="s">
         <v>15</v>
@@ -6987,16 +6996,16 @@
         <v>73</v>
       </c>
       <c r="B9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E9" t="s">
         <v>79</v>
       </c>
       <c r="F9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H9" t="s">
         <v>15</v>
@@ -7016,16 +7025,16 @@
         <v>73</v>
       </c>
       <c r="B10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E10" t="s">
         <v>79</v>
       </c>
       <c r="F10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H10" t="s">
         <v>15</v>
@@ -7045,16 +7054,16 @@
         <v>73</v>
       </c>
       <c r="B11" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="E11" t="s">
         <v>79</v>
       </c>
       <c r="F11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H11" t="s">
         <v>15</v>
@@ -7074,16 +7083,16 @@
         <v>73</v>
       </c>
       <c r="B12" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="E12" t="s">
         <v>79</v>
       </c>
       <c r="F12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H12" t="s">
         <v>15</v>
@@ -7103,16 +7112,16 @@
         <v>73</v>
       </c>
       <c r="B13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E13" t="s">
         <v>79</v>
       </c>
       <c r="F13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H13" t="s">
         <v>15</v>
@@ -7132,16 +7141,16 @@
         <v>73</v>
       </c>
       <c r="B14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E14" t="s">
         <v>79</v>
       </c>
       <c r="F14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H14" t="s">
         <v>15</v>
@@ -7158,45 +7167,51 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" t="s">
+        <v>79</v>
+      </c>
+      <c r="F15" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" t="s">
+        <v>15</v>
+      </c>
+      <c r="J15" t="s">
+        <v>15</v>
+      </c>
+      <c r="K15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>39</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>75</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F16" t="s">
         <v>40</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G16" t="s">
         <v>41</v>
       </c>
-      <c r="H15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I15" t="s">
-        <v>15</v>
-      </c>
-      <c r="J15" t="s">
-        <v>15</v>
-      </c>
-      <c r="K15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>86</v>
-      </c>
-      <c r="F16" t="s">
-        <v>42</v>
-      </c>
-      <c r="G16" t="s">
-        <v>43</v>
-      </c>
       <c r="H16" t="s">
         <v>15</v>
       </c>
       <c r="I16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J16" t="s">
         <v>15</v>
@@ -7207,13 +7222,13 @@
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H17" t="s">
         <v>15</v>
@@ -7230,13 +7245,13 @@
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H18" t="s">
         <v>15</v>
@@ -7253,13 +7268,13 @@
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H19" t="s">
         <v>15</v>
@@ -7276,13 +7291,13 @@
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H20" t="s">
         <v>15</v>
@@ -7299,13 +7314,13 @@
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H21" t="s">
         <v>15</v>
@@ -7322,13 +7337,13 @@
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G22" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H22" t="s">
         <v>15</v>
@@ -7345,13 +7360,13 @@
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F23" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H23" t="s">
         <v>15</v>
@@ -7368,13 +7383,13 @@
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F24" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G24" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H24" t="s">
         <v>15</v>
@@ -7391,13 +7406,13 @@
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F25" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G25" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H25" t="s">
         <v>15</v>
@@ -7414,70 +7429,76 @@
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F26" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H26" t="s">
         <v>15</v>
       </c>
       <c r="I26" t="s">
+        <v>16</v>
+      </c>
+      <c r="J26" t="s">
+        <v>15</v>
+      </c>
+      <c r="K26" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H27" t="s">
         <v>15</v>
       </c>
       <c r="I27" t="s">
-        <v>16</v>
-      </c>
-      <c r="J27" t="s">
-        <v>15</v>
-      </c>
-      <c r="K27" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H28" t="s">
         <v>15</v>
       </c>
       <c r="I28" t="s">
+        <v>16</v>
+      </c>
+      <c r="J28" t="s">
+        <v>15</v>
+      </c>
+      <c r="K28" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H29" t="s">
         <v>15</v>
@@ -7488,53 +7509,53 @@
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H30" t="s">
         <v>15</v>
       </c>
       <c r="I30" t="s">
-        <v>16</v>
-      </c>
-      <c r="J30" t="s">
-        <v>15</v>
-      </c>
-      <c r="K30" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H31" t="s">
         <v>15</v>
       </c>
       <c r="I31" t="s">
+        <v>16</v>
+      </c>
+      <c r="J31" t="s">
+        <v>15</v>
+      </c>
+      <c r="K31" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H32" t="s">
         <v>15</v>
@@ -7545,13 +7566,13 @@
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H33" t="s">
         <v>15</v>
@@ -7562,13 +7583,13 @@
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H34" t="s">
         <v>15</v>
@@ -7579,13 +7600,13 @@
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F35" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G35" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H35" t="s">
         <v>15</v>
@@ -7596,13 +7617,13 @@
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F36" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G36" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H36" t="s">
         <v>15</v>
@@ -7613,36 +7634,30 @@
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>1101</v>
+        <v>106</v>
       </c>
       <c r="F37" t="s">
-        <v>1100</v>
+        <v>72</v>
       </c>
       <c r="G37" t="s">
-        <v>1099</v>
+        <v>72</v>
       </c>
       <c r="H37" t="s">
         <v>15</v>
       </c>
       <c r="I37" t="s">
-        <v>16</v>
-      </c>
-      <c r="J37" t="s">
-        <v>15</v>
-      </c>
-      <c r="K37" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>1098</v>
+        <v>1101</v>
       </c>
       <c r="F38" t="s">
-        <v>1097</v>
+        <v>1100</v>
       </c>
       <c r="G38" t="s">
-        <v>877</v>
+        <v>1099</v>
       </c>
       <c r="H38" t="s">
         <v>15</v>
@@ -7659,13 +7674,13 @@
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>1096</v>
+        <v>1098</v>
       </c>
       <c r="F39" t="s">
-        <v>1095</v>
+        <v>1097</v>
       </c>
       <c r="G39" t="s">
-        <v>1094</v>
+        <v>877</v>
       </c>
       <c r="H39" t="s">
         <v>15</v>
@@ -7682,13 +7697,13 @@
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>1093</v>
+        <v>1096</v>
       </c>
       <c r="F40" t="s">
-        <v>1092</v>
+        <v>1095</v>
       </c>
       <c r="G40" t="s">
-        <v>882</v>
+        <v>1094</v>
       </c>
       <c r="H40" t="s">
         <v>15</v>
@@ -7705,13 +7720,13 @@
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>1091</v>
+        <v>1093</v>
       </c>
       <c r="F41" t="s">
-        <v>1090</v>
+        <v>1092</v>
       </c>
       <c r="G41" t="s">
-        <v>918</v>
+        <v>882</v>
       </c>
       <c r="H41" t="s">
         <v>15</v>
@@ -7728,13 +7743,13 @@
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>1089</v>
+        <v>1091</v>
       </c>
       <c r="F42" t="s">
-        <v>1088</v>
+        <v>1090</v>
       </c>
       <c r="G42" t="s">
-        <v>1087</v>
+        <v>918</v>
       </c>
       <c r="H42" t="s">
         <v>15</v>
@@ -7751,13 +7766,13 @@
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>1086</v>
+        <v>1089</v>
       </c>
       <c r="F43" t="s">
-        <v>1085</v>
+        <v>1088</v>
       </c>
       <c r="G43" t="s">
-        <v>1084</v>
+        <v>1087</v>
       </c>
       <c r="H43" t="s">
         <v>15</v>
@@ -7774,13 +7789,13 @@
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="F44" t="s">
-        <v>1082</v>
+        <v>1085</v>
       </c>
       <c r="G44" t="s">
-        <v>1081</v>
+        <v>1084</v>
       </c>
       <c r="H44" t="s">
         <v>15</v>
@@ -7797,13 +7812,13 @@
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>1080</v>
+        <v>1083</v>
       </c>
       <c r="F45" t="s">
-        <v>1079</v>
+        <v>1082</v>
       </c>
       <c r="G45" t="s">
-        <v>1078</v>
+        <v>1081</v>
       </c>
       <c r="H45" t="s">
         <v>15</v>
@@ -7820,13 +7835,13 @@
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>1077</v>
+        <v>1080</v>
       </c>
       <c r="F46" t="s">
-        <v>1076</v>
+        <v>1079</v>
       </c>
       <c r="G46" t="s">
-        <v>1075</v>
+        <v>1078</v>
       </c>
       <c r="H46" t="s">
         <v>15</v>
@@ -7843,13 +7858,13 @@
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>1074</v>
+        <v>1077</v>
       </c>
       <c r="F47" t="s">
-        <v>1073</v>
+        <v>1076</v>
       </c>
       <c r="G47" t="s">
-        <v>1072</v>
+        <v>1075</v>
       </c>
       <c r="H47" t="s">
         <v>15</v>
@@ -7866,24 +7881,47 @@
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
+        <v>1074</v>
+      </c>
+      <c r="F48" t="s">
+        <v>1073</v>
+      </c>
+      <c r="G48" t="s">
+        <v>1072</v>
+      </c>
+      <c r="H48" t="s">
+        <v>15</v>
+      </c>
+      <c r="I48" t="s">
+        <v>16</v>
+      </c>
+      <c r="J48" t="s">
+        <v>15</v>
+      </c>
+      <c r="K48" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
         <v>1071</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F49" t="s">
         <v>1070</v>
       </c>
-      <c r="G48" t="s">
+      <c r="G49" t="s">
         <v>1069</v>
       </c>
-      <c r="H48" t="s">
-        <v>15</v>
-      </c>
-      <c r="I48" t="s">
-        <v>16</v>
-      </c>
-      <c r="J48" t="s">
-        <v>15</v>
-      </c>
-      <c r="K48" t="s">
+      <c r="H49" t="s">
+        <v>15</v>
+      </c>
+      <c r="I49" t="s">
+        <v>16</v>
+      </c>
+      <c r="J49" t="s">
+        <v>15</v>
+      </c>
+      <c r="K49" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Naming and Sets?
</commit_message>
<xml_diff>
--- a/SetRules.xlsx
+++ b/SetRules.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr backupFile="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8290EA1A-A870-47CB-AB10-933367BDC2B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A6AE0DD-6680-4E08-A7A0-A37459DFC57D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{69765015-6AAF-4B94-8956-691CCC759B47}"/>
   </bookViews>
@@ -29,7 +29,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -3254,27 +3253,18 @@
     <t>RSD_NRGSRV-WH</t>
   </si>
   <si>
-    <t>R-WH*</t>
-  </si>
-  <si>
     <t>Residential Space Heating</t>
   </si>
   <si>
     <t>RSD_NRGSRV-SH</t>
   </si>
   <si>
-    <t>R-SH*</t>
-  </si>
-  <si>
     <t>Residential Space Cooling</t>
   </si>
   <si>
     <t>RSD_NRGSRV-SC</t>
   </si>
   <si>
-    <t>R-SC*</t>
-  </si>
-  <si>
     <t>Residential Refrigeration</t>
   </si>
   <si>
@@ -3357,6 +3347,15 @@
   </si>
   <si>
     <t>Freight transport - medium goods truck</t>
+  </si>
+  <si>
+    <t>R-WH*,R-H*</t>
+  </si>
+  <si>
+    <t>R-SC*,R-HC*</t>
+  </si>
+  <si>
+    <t>R-SH*,R-H*,R-HC*</t>
   </si>
 </sst>
 </file>
@@ -6764,8 +6763,8 @@
   </sheetPr>
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6825,7 +6824,7 @@
         <v>74</v>
       </c>
       <c r="E3" t="s">
-        <v>1102</v>
+        <v>1099</v>
       </c>
       <c r="F3" t="s">
         <v>13</v>
@@ -6854,7 +6853,7 @@
         <v>75</v>
       </c>
       <c r="E4" t="s">
-        <v>1102</v>
+        <v>1099</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
@@ -6883,7 +6882,7 @@
         <v>76</v>
       </c>
       <c r="E5" t="s">
-        <v>1102</v>
+        <v>1099</v>
       </c>
       <c r="F5" t="s">
         <v>19</v>
@@ -6909,16 +6908,16 @@
         <v>73</v>
       </c>
       <c r="B6" t="s">
-        <v>1103</v>
+        <v>1100</v>
       </c>
       <c r="E6" t="s">
+        <v>1099</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1101</v>
+      </c>
+      <c r="G6" t="s">
         <v>1102</v>
-      </c>
-      <c r="F6" t="s">
-        <v>1104</v>
-      </c>
-      <c r="G6" t="s">
-        <v>1105</v>
       </c>
       <c r="H6" t="s">
         <v>15</v>
@@ -6941,7 +6940,7 @@
         <v>77</v>
       </c>
       <c r="E7" t="s">
-        <v>1102</v>
+        <v>1099</v>
       </c>
       <c r="F7" t="s">
         <v>21</v>
@@ -7651,13 +7650,13 @@
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>1101</v>
+        <v>1098</v>
       </c>
       <c r="F38" t="s">
-        <v>1100</v>
+        <v>1097</v>
       </c>
       <c r="G38" t="s">
-        <v>1099</v>
+        <v>1096</v>
       </c>
       <c r="H38" t="s">
         <v>15</v>
@@ -7674,10 +7673,10 @@
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>1098</v>
+        <v>1095</v>
       </c>
       <c r="F39" t="s">
-        <v>1097</v>
+        <v>1094</v>
       </c>
       <c r="G39" t="s">
         <v>877</v>
@@ -7697,13 +7696,13 @@
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>1096</v>
+        <v>1093</v>
       </c>
       <c r="F40" t="s">
-        <v>1095</v>
+        <v>1092</v>
       </c>
       <c r="G40" t="s">
-        <v>1094</v>
+        <v>1091</v>
       </c>
       <c r="H40" t="s">
         <v>15</v>
@@ -7720,10 +7719,10 @@
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>1093</v>
+        <v>1090</v>
       </c>
       <c r="F41" t="s">
-        <v>1092</v>
+        <v>1089</v>
       </c>
       <c r="G41" t="s">
         <v>882</v>
@@ -7743,10 +7742,10 @@
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>1091</v>
+        <v>1088</v>
       </c>
       <c r="F42" t="s">
-        <v>1090</v>
+        <v>1087</v>
       </c>
       <c r="G42" t="s">
         <v>918</v>
@@ -7766,13 +7765,13 @@
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>1089</v>
+        <v>1086</v>
       </c>
       <c r="F43" t="s">
-        <v>1088</v>
+        <v>1085</v>
       </c>
       <c r="G43" t="s">
-        <v>1087</v>
+        <v>1084</v>
       </c>
       <c r="H43" t="s">
         <v>15</v>
@@ -7789,13 +7788,13 @@
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>1086</v>
+        <v>1083</v>
       </c>
       <c r="F44" t="s">
-        <v>1085</v>
+        <v>1082</v>
       </c>
       <c r="G44" t="s">
-        <v>1084</v>
+        <v>1081</v>
       </c>
       <c r="H44" t="s">
         <v>15</v>
@@ -7812,13 +7811,13 @@
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>1083</v>
+        <v>1080</v>
       </c>
       <c r="F45" t="s">
-        <v>1082</v>
+        <v>1079</v>
       </c>
       <c r="G45" t="s">
-        <v>1081</v>
+        <v>1078</v>
       </c>
       <c r="H45" t="s">
         <v>15</v>
@@ -7835,13 +7834,13 @@
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>1080</v>
+        <v>1077</v>
       </c>
       <c r="F46" t="s">
-        <v>1079</v>
+        <v>1076</v>
       </c>
       <c r="G46" t="s">
-        <v>1078</v>
+        <v>1075</v>
       </c>
       <c r="H46" t="s">
         <v>15</v>
@@ -7858,13 +7857,13 @@
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>1077</v>
+        <v>1104</v>
       </c>
       <c r="F47" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="G47" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="H47" t="s">
         <v>15</v>
@@ -7881,13 +7880,13 @@
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>1074</v>
+        <v>1105</v>
       </c>
       <c r="F48" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="G48" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="H48" t="s">
         <v>15</v>
@@ -7904,7 +7903,7 @@
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>1071</v>
+        <v>1103</v>
       </c>
       <c r="F49" t="s">
         <v>1070</v>

</xml_diff>

<commit_message>
Add some industry sets and tables
</commit_message>
<xml_diff>
--- a/SetRules.xlsx
+++ b/SetRules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr backupFile="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_TIMES-IE\ind-redevelopment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8290EA1A-A870-47CB-AB10-933367BDC2B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F436B8A-D943-4097-AA14-85D1F1EB0E92}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{69765015-6AAF-4B94-8956-691CCC759B47}"/>
+    <workbookView xWindow="9330" yWindow="915" windowWidth="10425" windowHeight="14355" activeTab="2" xr2:uid="{69765015-6AAF-4B94-8956-691CCC759B47}"/>
   </bookViews>
   <sheets>
     <sheet name="VEDA_Sets-Comm" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2759" uniqueCount="1106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2863" uniqueCount="1145">
   <si>
     <t>~TFM_Psets</t>
   </si>
@@ -3357,6 +3357,123 @@
   </si>
   <si>
     <t>Freight transport - medium goods truck</t>
+  </si>
+  <si>
+    <t>I*CAF*</t>
+  </si>
+  <si>
+    <t>DMD_IND-CAF</t>
+  </si>
+  <si>
+    <t>Industry - Chemicals and man-made fibers</t>
+  </si>
+  <si>
+    <t>I*EOE*</t>
+  </si>
+  <si>
+    <t>DMD_IND-EOE</t>
+  </si>
+  <si>
+    <t>Industry - Electrical and optical equipment</t>
+  </si>
+  <si>
+    <t>I*FAB*</t>
+  </si>
+  <si>
+    <t>DMD_IND-FAB</t>
+  </si>
+  <si>
+    <t>Industry - Food and beverages</t>
+  </si>
+  <si>
+    <t>I*MAE*</t>
+  </si>
+  <si>
+    <t>DMD_IND-MAE</t>
+  </si>
+  <si>
+    <t>Industry - Machinery and equipment n.e.c.</t>
+  </si>
+  <si>
+    <t>I*MAP*</t>
+  </si>
+  <si>
+    <t>DMD_IND-MAP</t>
+  </si>
+  <si>
+    <t>Industry - Basic metals and fabricated metal prod.</t>
+  </si>
+  <si>
+    <t>I*NEM*</t>
+  </si>
+  <si>
+    <t>DMD_IND-NEM</t>
+  </si>
+  <si>
+    <t>Industry - Non-energy mining</t>
+  </si>
+  <si>
+    <t>I*OMA*</t>
+  </si>
+  <si>
+    <t>DMD_IND-OMA</t>
+  </si>
+  <si>
+    <t>Industry - Other manufacturing</t>
+  </si>
+  <si>
+    <t>I*ONM*</t>
+  </si>
+  <si>
+    <t>DMD_IND-ONM</t>
+  </si>
+  <si>
+    <t>Industry - Other non-metalic mineral products</t>
+  </si>
+  <si>
+    <t>I*PX4*</t>
+  </si>
+  <si>
+    <t>DMD_IND-PX4</t>
+  </si>
+  <si>
+    <t>Industry - Pulp, paper, publishing and printing</t>
+  </si>
+  <si>
+    <t>I*RAP*</t>
+  </si>
+  <si>
+    <t>DMD_IND-RAP</t>
+  </si>
+  <si>
+    <t>Industry - Rubber and plastic products</t>
+  </si>
+  <si>
+    <t>I*TAP*</t>
+  </si>
+  <si>
+    <t>DMD_IND-TAP</t>
+  </si>
+  <si>
+    <t>Industry - Textiles and textile products</t>
+  </si>
+  <si>
+    <t>I*TEM*</t>
+  </si>
+  <si>
+    <t>DMD_IND-TEM</t>
+  </si>
+  <si>
+    <t>Industry - Transport equipment manufacture</t>
+  </si>
+  <si>
+    <t>I*WAP*</t>
+  </si>
+  <si>
+    <t>DMD_IND-WAP</t>
+  </si>
+  <si>
+    <t>Industry - Wood and wood products</t>
   </si>
 </sst>
 </file>
@@ -3723,8 +3840,8 @@
   </sheetPr>
   <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6762,10 +6879,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:L49"/>
+  <dimension ref="A1:L62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7902,7 +8019,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>1071</v>
       </c>
@@ -7922,6 +8039,344 @@
         <v>15</v>
       </c>
       <c r="K49" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>73</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1106</v>
+      </c>
+      <c r="F50" t="s">
+        <v>1107</v>
+      </c>
+      <c r="G50" t="s">
+        <v>1108</v>
+      </c>
+      <c r="H50" t="s">
+        <v>15</v>
+      </c>
+      <c r="I50" t="s">
+        <v>16</v>
+      </c>
+      <c r="J50" t="s">
+        <v>15</v>
+      </c>
+      <c r="K50" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>73</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1109</v>
+      </c>
+      <c r="F51" t="s">
+        <v>1110</v>
+      </c>
+      <c r="G51" t="s">
+        <v>1111</v>
+      </c>
+      <c r="H51" t="s">
+        <v>15</v>
+      </c>
+      <c r="I51" t="s">
+        <v>16</v>
+      </c>
+      <c r="J51" t="s">
+        <v>15</v>
+      </c>
+      <c r="K51" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>73</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1112</v>
+      </c>
+      <c r="F52" t="s">
+        <v>1113</v>
+      </c>
+      <c r="G52" t="s">
+        <v>1114</v>
+      </c>
+      <c r="H52" t="s">
+        <v>15</v>
+      </c>
+      <c r="I52" t="s">
+        <v>16</v>
+      </c>
+      <c r="J52" t="s">
+        <v>15</v>
+      </c>
+      <c r="K52" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>73</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1115</v>
+      </c>
+      <c r="F53" t="s">
+        <v>1116</v>
+      </c>
+      <c r="G53" t="s">
+        <v>1117</v>
+      </c>
+      <c r="H53" t="s">
+        <v>15</v>
+      </c>
+      <c r="I53" t="s">
+        <v>16</v>
+      </c>
+      <c r="J53" t="s">
+        <v>15</v>
+      </c>
+      <c r="K53" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>73</v>
+      </c>
+      <c r="B54" t="s">
+        <v>1118</v>
+      </c>
+      <c r="F54" t="s">
+        <v>1119</v>
+      </c>
+      <c r="G54" t="s">
+        <v>1120</v>
+      </c>
+      <c r="H54" t="s">
+        <v>15</v>
+      </c>
+      <c r="I54" t="s">
+        <v>16</v>
+      </c>
+      <c r="J54" t="s">
+        <v>15</v>
+      </c>
+      <c r="K54" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>73</v>
+      </c>
+      <c r="B55" t="s">
+        <v>1121</v>
+      </c>
+      <c r="F55" t="s">
+        <v>1122</v>
+      </c>
+      <c r="G55" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H55" t="s">
+        <v>15</v>
+      </c>
+      <c r="I55" t="s">
+        <v>16</v>
+      </c>
+      <c r="J55" t="s">
+        <v>15</v>
+      </c>
+      <c r="K55" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>73</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1124</v>
+      </c>
+      <c r="F56" t="s">
+        <v>1125</v>
+      </c>
+      <c r="G56" t="s">
+        <v>1126</v>
+      </c>
+      <c r="H56" t="s">
+        <v>15</v>
+      </c>
+      <c r="I56" t="s">
+        <v>16</v>
+      </c>
+      <c r="J56" t="s">
+        <v>15</v>
+      </c>
+      <c r="K56" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>73</v>
+      </c>
+      <c r="B57" t="s">
+        <v>1127</v>
+      </c>
+      <c r="F57" t="s">
+        <v>1128</v>
+      </c>
+      <c r="G57" t="s">
+        <v>1129</v>
+      </c>
+      <c r="H57" t="s">
+        <v>15</v>
+      </c>
+      <c r="I57" t="s">
+        <v>16</v>
+      </c>
+      <c r="J57" t="s">
+        <v>15</v>
+      </c>
+      <c r="K57" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>73</v>
+      </c>
+      <c r="B58" t="s">
+        <v>1130</v>
+      </c>
+      <c r="F58" t="s">
+        <v>1131</v>
+      </c>
+      <c r="G58" t="s">
+        <v>1132</v>
+      </c>
+      <c r="H58" t="s">
+        <v>15</v>
+      </c>
+      <c r="I58" t="s">
+        <v>16</v>
+      </c>
+      <c r="J58" t="s">
+        <v>15</v>
+      </c>
+      <c r="K58" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>73</v>
+      </c>
+      <c r="B59" t="s">
+        <v>1133</v>
+      </c>
+      <c r="F59" t="s">
+        <v>1134</v>
+      </c>
+      <c r="G59" t="s">
+        <v>1135</v>
+      </c>
+      <c r="H59" t="s">
+        <v>15</v>
+      </c>
+      <c r="I59" t="s">
+        <v>16</v>
+      </c>
+      <c r="J59" t="s">
+        <v>15</v>
+      </c>
+      <c r="K59" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>73</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1136</v>
+      </c>
+      <c r="F60" t="s">
+        <v>1137</v>
+      </c>
+      <c r="G60" t="s">
+        <v>1138</v>
+      </c>
+      <c r="H60" t="s">
+        <v>15</v>
+      </c>
+      <c r="I60" t="s">
+        <v>16</v>
+      </c>
+      <c r="J60" t="s">
+        <v>15</v>
+      </c>
+      <c r="K60" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>73</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1139</v>
+      </c>
+      <c r="F61" t="s">
+        <v>1140</v>
+      </c>
+      <c r="G61" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H61" t="s">
+        <v>15</v>
+      </c>
+      <c r="I61" t="s">
+        <v>16</v>
+      </c>
+      <c r="J61" t="s">
+        <v>15</v>
+      </c>
+      <c r="K61" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>73</v>
+      </c>
+      <c r="B62" t="s">
+        <v>1142</v>
+      </c>
+      <c r="F62" t="s">
+        <v>1143</v>
+      </c>
+      <c r="G62" t="s">
+        <v>1144</v>
+      </c>
+      <c r="H62" t="s">
+        <v>15</v>
+      </c>
+      <c r="I62" t="s">
+        <v>16</v>
+      </c>
+      <c r="J62" t="s">
+        <v>15</v>
+      </c>
+      <c r="K62" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update sets and tables for RSD
- single set for hot water, space heating and space cooling
- commodity sets for sectoral energy carriers
- tables with marginal costs for sectoral energy carriers
</commit_message>
<xml_diff>
--- a/SetRules.xlsx
+++ b/SetRules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8C5E45-2483-4970-A359-5F116FC062A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB225BC-9D44-4A6C-9E19-646A7C0619DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" activeTab="4" xr2:uid="{69765015-6AAF-4B94-8956-691CCC759B47}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{69765015-6AAF-4B94-8956-691CCC759B47}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets-Comm" sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2917" uniqueCount="1163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2944" uniqueCount="1170">
   <si>
     <t>~TFM_Psets</t>
   </si>
@@ -3027,24 +3027,6 @@
     <t>Transport Train Long Distance</t>
   </si>
   <si>
-    <t>Residential Water Heating</t>
-  </si>
-  <si>
-    <t>RSD_NRGSRV-WH</t>
-  </si>
-  <si>
-    <t>Residential Space Heating</t>
-  </si>
-  <si>
-    <t>RSD_NRGSRV-SH</t>
-  </si>
-  <si>
-    <t>Residential Space Cooling</t>
-  </si>
-  <si>
-    <t>RSD_NRGSRV-SC</t>
-  </si>
-  <si>
     <t>Residential Refrigeration</t>
   </si>
   <si>
@@ -3525,13 +3507,52 @@
     <t>T-CAR*BEV*</t>
   </si>
   <si>
-    <t>R-SC*,R-HC*</t>
-  </si>
-  <si>
-    <t>R-SH*,R-H*,R-HC*</t>
-  </si>
-  <si>
-    <t>R-WH*,R-H*</t>
+    <t>RSDWH*,RSDSH*,RSDSC*</t>
+  </si>
+  <si>
+    <t>Residential Hot Water and Space Heating and Cooling</t>
+  </si>
+  <si>
+    <t>RSD_NRGSRV-WS</t>
+  </si>
+  <si>
+    <t>-IRE</t>
+  </si>
+  <si>
+    <t>DUMMY_IMPORT</t>
+  </si>
+  <si>
+    <t>Dummy import processes</t>
+  </si>
+  <si>
+    <t>IMP*Z</t>
+  </si>
+  <si>
+    <t>NGR-FUELS_RSD</t>
+  </si>
+  <si>
+    <t>Residential energy carriers</t>
+  </si>
+  <si>
+    <t>NGR-FUELS_COM</t>
+  </si>
+  <si>
+    <t>Commercial energy carriers</t>
+  </si>
+  <si>
+    <t>NGR-FUELS_IND</t>
+  </si>
+  <si>
+    <t>Industry energy carriers</t>
+  </si>
+  <si>
+    <t>NGR-FUELS_AGR</t>
+  </si>
+  <si>
+    <t>Agriculture energy carriers</t>
+  </si>
+  <si>
+    <t>RSD*,-*_*t</t>
   </si>
 </sst>
 </file>
@@ -3573,12 +3594,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3896,10 +3918,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:J65"/>
+  <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4083,7 +4105,7 @@
         <v>208</v>
       </c>
       <c r="D8" t="s">
-        <v>1068</v>
+        <v>1062</v>
       </c>
       <c r="E8" t="s">
         <v>140</v>
@@ -4109,7 +4131,7 @@
         <v>209</v>
       </c>
       <c r="D9" t="s">
-        <v>1069</v>
+        <v>1063</v>
       </c>
       <c r="E9" t="s">
         <v>141</v>
@@ -4135,7 +4157,7 @@
         <v>210</v>
       </c>
       <c r="D10" t="s">
-        <v>1070</v>
+        <v>1064</v>
       </c>
       <c r="E10" t="s">
         <v>142</v>
@@ -4161,7 +4183,7 @@
         <v>211</v>
       </c>
       <c r="D11" t="s">
-        <v>1071</v>
+        <v>1065</v>
       </c>
       <c r="E11" t="s">
         <v>143</v>
@@ -4187,7 +4209,7 @@
         <v>212</v>
       </c>
       <c r="D12" t="s">
-        <v>1072</v>
+        <v>1066</v>
       </c>
       <c r="E12" t="s">
         <v>144</v>
@@ -4213,7 +4235,7 @@
         <v>213</v>
       </c>
       <c r="D13" t="s">
-        <v>1073</v>
+        <v>1067</v>
       </c>
       <c r="E13" t="s">
         <v>145</v>
@@ -4239,7 +4261,7 @@
         <v>214</v>
       </c>
       <c r="D14" t="s">
-        <v>1074</v>
+        <v>1068</v>
       </c>
       <c r="E14" t="s">
         <v>146</v>
@@ -4265,7 +4287,7 @@
         <v>215</v>
       </c>
       <c r="D15" t="s">
-        <v>1075</v>
+        <v>1069</v>
       </c>
       <c r="E15" t="s">
         <v>147</v>
@@ -4291,7 +4313,7 @@
         <v>216</v>
       </c>
       <c r="D16" t="s">
-        <v>1076</v>
+        <v>1070</v>
       </c>
       <c r="E16" t="s">
         <v>149</v>
@@ -4317,7 +4339,7 @@
         <v>217</v>
       </c>
       <c r="D17" t="s">
-        <v>1077</v>
+        <v>1071</v>
       </c>
       <c r="E17" t="s">
         <v>150</v>
@@ -4343,7 +4365,7 @@
         <v>218</v>
       </c>
       <c r="D18" t="s">
-        <v>1078</v>
+        <v>1072</v>
       </c>
       <c r="E18" t="s">
         <v>151</v>
@@ -4369,7 +4391,7 @@
         <v>219</v>
       </c>
       <c r="D19" t="s">
-        <v>1079</v>
+        <v>1073</v>
       </c>
       <c r="E19" t="s">
         <v>152</v>
@@ -4395,7 +4417,7 @@
         <v>220</v>
       </c>
       <c r="D20" t="s">
-        <v>1080</v>
+        <v>1074</v>
       </c>
       <c r="E20" t="s">
         <v>153</v>
@@ -4421,7 +4443,7 @@
         <v>221</v>
       </c>
       <c r="D21" t="s">
-        <v>1081</v>
+        <v>1075</v>
       </c>
       <c r="E21" t="s">
         <v>154</v>
@@ -4447,7 +4469,7 @@
         <v>222</v>
       </c>
       <c r="D22" t="s">
-        <v>1082</v>
+        <v>1076</v>
       </c>
       <c r="E22" t="s">
         <v>155</v>
@@ -4473,7 +4495,7 @@
         <v>223</v>
       </c>
       <c r="D23" t="s">
-        <v>1083</v>
+        <v>1077</v>
       </c>
       <c r="E23" t="s">
         <v>156</v>
@@ -4499,7 +4521,7 @@
         <v>224</v>
       </c>
       <c r="D24" t="s">
-        <v>1084</v>
+        <v>1078</v>
       </c>
       <c r="E24" t="s">
         <v>158</v>
@@ -4525,7 +4547,7 @@
         <v>225</v>
       </c>
       <c r="D25" t="s">
-        <v>1085</v>
+        <v>1079</v>
       </c>
       <c r="E25" t="s">
         <v>159</v>
@@ -4551,7 +4573,7 @@
         <v>226</v>
       </c>
       <c r="D26" t="s">
-        <v>1086</v>
+        <v>1080</v>
       </c>
       <c r="E26" t="s">
         <v>160</v>
@@ -4577,7 +4599,7 @@
         <v>227</v>
       </c>
       <c r="D27" t="s">
-        <v>1087</v>
+        <v>1081</v>
       </c>
       <c r="E27" t="s">
         <v>161</v>
@@ -4603,7 +4625,7 @@
         <v>228</v>
       </c>
       <c r="D28" t="s">
-        <v>1088</v>
+        <v>1082</v>
       </c>
       <c r="E28" t="s">
         <v>162</v>
@@ -4629,7 +4651,7 @@
         <v>229</v>
       </c>
       <c r="D29" t="s">
-        <v>1089</v>
+        <v>1083</v>
       </c>
       <c r="E29" t="s">
         <v>163</v>
@@ -4655,7 +4677,7 @@
         <v>230</v>
       </c>
       <c r="D30" t="s">
-        <v>1090</v>
+        <v>1084</v>
       </c>
       <c r="E30" t="s">
         <v>164</v>
@@ -4681,7 +4703,7 @@
         <v>231</v>
       </c>
       <c r="D31" t="s">
-        <v>1091</v>
+        <v>1085</v>
       </c>
       <c r="E31" t="s">
         <v>165</v>
@@ -4707,7 +4729,7 @@
         <v>167</v>
       </c>
       <c r="D32" t="s">
-        <v>1092</v>
+        <v>1086</v>
       </c>
       <c r="E32" t="s">
         <v>92</v>
@@ -4733,7 +4755,7 @@
         <v>168</v>
       </c>
       <c r="D33" t="s">
-        <v>1093</v>
+        <v>1087</v>
       </c>
       <c r="E33" t="s">
         <v>93</v>
@@ -4759,7 +4781,7 @@
         <v>169</v>
       </c>
       <c r="D34" t="s">
-        <v>1094</v>
+        <v>1088</v>
       </c>
       <c r="E34" t="s">
         <v>94</v>
@@ -4785,7 +4807,7 @@
         <v>170</v>
       </c>
       <c r="D35" t="s">
-        <v>1095</v>
+        <v>1089</v>
       </c>
       <c r="E35" t="s">
         <v>95</v>
@@ -4811,7 +4833,7 @@
         <v>171</v>
       </c>
       <c r="D36" t="s">
-        <v>1096</v>
+        <v>1090</v>
       </c>
       <c r="E36" t="s">
         <v>96</v>
@@ -4837,7 +4859,7 @@
         <v>172</v>
       </c>
       <c r="D37" t="s">
-        <v>1097</v>
+        <v>1091</v>
       </c>
       <c r="E37" t="s">
         <v>97</v>
@@ -4863,7 +4885,7 @@
         <v>173</v>
       </c>
       <c r="D38" t="s">
-        <v>1098</v>
+        <v>1092</v>
       </c>
       <c r="E38" t="s">
         <v>98</v>
@@ -4889,7 +4911,7 @@
         <v>174</v>
       </c>
       <c r="D39" t="s">
-        <v>1099</v>
+        <v>1093</v>
       </c>
       <c r="E39" t="s">
         <v>99</v>
@@ -4915,7 +4937,7 @@
         <v>175</v>
       </c>
       <c r="D40" t="s">
-        <v>1100</v>
+        <v>1094</v>
       </c>
       <c r="E40" t="s">
         <v>101</v>
@@ -4941,7 +4963,7 @@
         <v>176</v>
       </c>
       <c r="D41" t="s">
-        <v>1101</v>
+        <v>1095</v>
       </c>
       <c r="E41" t="s">
         <v>102</v>
@@ -4967,7 +4989,7 @@
         <v>177</v>
       </c>
       <c r="D42" t="s">
-        <v>1102</v>
+        <v>1096</v>
       </c>
       <c r="E42" t="s">
         <v>103</v>
@@ -4993,7 +5015,7 @@
         <v>178</v>
       </c>
       <c r="D43" t="s">
-        <v>1103</v>
+        <v>1097</v>
       </c>
       <c r="E43" t="s">
         <v>104</v>
@@ -5019,7 +5041,7 @@
         <v>179</v>
       </c>
       <c r="D44" t="s">
-        <v>1104</v>
+        <v>1098</v>
       </c>
       <c r="E44" t="s">
         <v>105</v>
@@ -5045,7 +5067,7 @@
         <v>180</v>
       </c>
       <c r="D45" t="s">
-        <v>1105</v>
+        <v>1099</v>
       </c>
       <c r="E45" t="s">
         <v>106</v>
@@ -5071,7 +5093,7 @@
         <v>181</v>
       </c>
       <c r="D46" t="s">
-        <v>1106</v>
+        <v>1100</v>
       </c>
       <c r="E46" t="s">
         <v>107</v>
@@ -5097,7 +5119,7 @@
         <v>182</v>
       </c>
       <c r="D47" t="s">
-        <v>1107</v>
+        <v>1101</v>
       </c>
       <c r="E47" t="s">
         <v>108</v>
@@ -5123,7 +5145,7 @@
         <v>183</v>
       </c>
       <c r="D48" t="s">
-        <v>1108</v>
+        <v>1102</v>
       </c>
       <c r="E48" t="s">
         <v>109</v>
@@ -5149,7 +5171,7 @@
         <v>184</v>
       </c>
       <c r="D49" t="s">
-        <v>1109</v>
+        <v>1103</v>
       </c>
       <c r="E49" t="s">
         <v>110</v>
@@ -5175,7 +5197,7 @@
         <v>185</v>
       </c>
       <c r="D50" t="s">
-        <v>1110</v>
+        <v>1104</v>
       </c>
       <c r="E50" t="s">
         <v>111</v>
@@ -5201,7 +5223,7 @@
         <v>186</v>
       </c>
       <c r="D51" t="s">
-        <v>1111</v>
+        <v>1105</v>
       </c>
       <c r="E51" t="s">
         <v>112</v>
@@ -5227,7 +5249,7 @@
         <v>187</v>
       </c>
       <c r="D52" t="s">
-        <v>1112</v>
+        <v>1106</v>
       </c>
       <c r="E52" t="s">
         <v>113</v>
@@ -5253,7 +5275,7 @@
         <v>188</v>
       </c>
       <c r="D53" t="s">
-        <v>1113</v>
+        <v>1107</v>
       </c>
       <c r="E53" t="s">
         <v>114</v>
@@ -5279,7 +5301,7 @@
         <v>189</v>
       </c>
       <c r="D54" t="s">
-        <v>1114</v>
+        <v>1108</v>
       </c>
       <c r="E54" t="s">
         <v>115</v>
@@ -5305,7 +5327,7 @@
         <v>190</v>
       </c>
       <c r="D55" t="s">
-        <v>1115</v>
+        <v>1109</v>
       </c>
       <c r="E55" t="s">
         <v>116</v>
@@ -5331,7 +5353,7 @@
         <v>191</v>
       </c>
       <c r="D56" t="s">
-        <v>1116</v>
+        <v>1110</v>
       </c>
       <c r="E56" t="s">
         <v>118</v>
@@ -5357,7 +5379,7 @@
         <v>192</v>
       </c>
       <c r="D57" t="s">
-        <v>1117</v>
+        <v>1111</v>
       </c>
       <c r="E57" t="s">
         <v>119</v>
@@ -5383,7 +5405,7 @@
         <v>193</v>
       </c>
       <c r="D58" t="s">
-        <v>1118</v>
+        <v>1112</v>
       </c>
       <c r="E58" t="s">
         <v>120</v>
@@ -5409,7 +5431,7 @@
         <v>194</v>
       </c>
       <c r="D59" t="s">
-        <v>1119</v>
+        <v>1113</v>
       </c>
       <c r="E59" t="s">
         <v>121</v>
@@ -5435,7 +5457,7 @@
         <v>195</v>
       </c>
       <c r="D60" t="s">
-        <v>1120</v>
+        <v>1114</v>
       </c>
       <c r="E60" t="s">
         <v>122</v>
@@ -5461,7 +5483,7 @@
         <v>196</v>
       </c>
       <c r="D61" t="s">
-        <v>1121</v>
+        <v>1115</v>
       </c>
       <c r="E61" t="s">
         <v>123</v>
@@ -5487,7 +5509,7 @@
         <v>197</v>
       </c>
       <c r="D62" t="s">
-        <v>1122</v>
+        <v>1116</v>
       </c>
       <c r="E62" t="s">
         <v>124</v>
@@ -5513,7 +5535,7 @@
         <v>198</v>
       </c>
       <c r="D63" t="s">
-        <v>1123</v>
+        <v>1117</v>
       </c>
       <c r="E63" t="s">
         <v>125</v>
@@ -5539,7 +5561,7 @@
         <v>199</v>
       </c>
       <c r="D64" t="s">
-        <v>1124</v>
+        <v>1118</v>
       </c>
       <c r="E64" t="s">
         <v>127</v>
@@ -5565,7 +5587,7 @@
         <v>201</v>
       </c>
       <c r="D65" t="s">
-        <v>1125</v>
+        <v>1119</v>
       </c>
       <c r="E65" t="s">
         <v>128</v>
@@ -5580,6 +5602,110 @@
         <v>15</v>
       </c>
       <c r="I65" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>200</v>
+      </c>
+      <c r="B66" t="s">
+        <v>1169</v>
+      </c>
+      <c r="D66" t="s">
+        <v>1161</v>
+      </c>
+      <c r="E66" t="s">
+        <v>1162</v>
+      </c>
+      <c r="F66" t="s">
+        <v>15</v>
+      </c>
+      <c r="G66" t="s">
+        <v>16</v>
+      </c>
+      <c r="H66" t="s">
+        <v>15</v>
+      </c>
+      <c r="I66" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>200</v>
+      </c>
+      <c r="B67" t="s">
+        <v>328</v>
+      </c>
+      <c r="D67" t="s">
+        <v>1163</v>
+      </c>
+      <c r="E67" t="s">
+        <v>1164</v>
+      </c>
+      <c r="F67" t="s">
+        <v>15</v>
+      </c>
+      <c r="G67" t="s">
+        <v>16</v>
+      </c>
+      <c r="H67" t="s">
+        <v>15</v>
+      </c>
+      <c r="I67" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>200</v>
+      </c>
+      <c r="B68" t="s">
+        <v>336</v>
+      </c>
+      <c r="D68" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E68" t="s">
+        <v>1166</v>
+      </c>
+      <c r="F68" t="s">
+        <v>15</v>
+      </c>
+      <c r="G68" t="s">
+        <v>16</v>
+      </c>
+      <c r="H68" t="s">
+        <v>15</v>
+      </c>
+      <c r="I68" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>200</v>
+      </c>
+      <c r="B69" t="s">
+        <v>326</v>
+      </c>
+      <c r="D69" t="s">
+        <v>1167</v>
+      </c>
+      <c r="E69" t="s">
+        <v>1168</v>
+      </c>
+      <c r="F69" t="s">
+        <v>15</v>
+      </c>
+      <c r="G69" t="s">
+        <v>16</v>
+      </c>
+      <c r="H69" t="s">
+        <v>15</v>
+      </c>
+      <c r="I69" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6941,10 +7067,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6997,14 +7123,17 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>881</v>
+      </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>1160</v>
       </c>
       <c r="F3" t="s">
-        <v>1126</v>
+        <v>1158</v>
       </c>
       <c r="G3" t="s">
-        <v>42</v>
+        <v>1159</v>
       </c>
       <c r="H3" t="s">
         <v>15</v>
@@ -7021,13 +7150,13 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F4" t="s">
-        <v>1127</v>
+        <v>1120</v>
       </c>
       <c r="G4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H4" t="s">
         <v>15</v>
@@ -7044,13 +7173,13 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F5" t="s">
-        <v>1128</v>
+        <v>1121</v>
       </c>
       <c r="G5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H5" t="s">
         <v>15</v>
@@ -7067,13 +7196,13 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F6" t="s">
-        <v>1129</v>
+        <v>1122</v>
       </c>
       <c r="G6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H6" t="s">
         <v>15</v>
@@ -7090,13 +7219,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>1067</v>
+        <v>67</v>
       </c>
       <c r="F7" t="s">
-        <v>1130</v>
+        <v>1123</v>
       </c>
       <c r="G7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H7" t="s">
         <v>15</v>
@@ -7113,13 +7242,13 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>68</v>
+        <v>1061</v>
       </c>
       <c r="F8" t="s">
-        <v>1131</v>
+        <v>1124</v>
       </c>
       <c r="G8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H8" t="s">
         <v>15</v>
@@ -7136,13 +7265,13 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F9" t="s">
-        <v>1132</v>
+        <v>1125</v>
       </c>
       <c r="G9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H9" t="s">
         <v>15</v>
@@ -7159,13 +7288,13 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F10" t="s">
-        <v>1133</v>
+        <v>1126</v>
       </c>
       <c r="G10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H10" t="s">
         <v>15</v>
@@ -7182,24 +7311,47 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1127</v>
+      </c>
+      <c r="G11" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>71</v>
       </c>
-      <c r="F11" t="s">
-        <v>1134</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="F12" t="s">
+        <v>1128</v>
+      </c>
+      <c r="G12" t="s">
         <v>50</v>
       </c>
-      <c r="H11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I11" t="s">
-        <v>16</v>
-      </c>
-      <c r="J11" t="s">
-        <v>15</v>
-      </c>
-      <c r="K11" t="s">
+      <c r="H12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12" t="s">
         <v>16</v>
       </c>
     </row>
@@ -7273,13 +7425,13 @@
         <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>1028</v>
+        <v>1022</v>
       </c>
       <c r="F3" t="s">
-        <v>1029</v>
+        <v>1023</v>
       </c>
       <c r="G3" t="s">
-        <v>1030</v>
+        <v>1024</v>
       </c>
       <c r="H3" t="s">
         <v>15</v>
@@ -7299,13 +7451,13 @@
         <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>1031</v>
+        <v>1025</v>
       </c>
       <c r="F4" t="s">
-        <v>1032</v>
+        <v>1026</v>
       </c>
       <c r="G4" t="s">
-        <v>1033</v>
+        <v>1027</v>
       </c>
       <c r="H4" t="s">
         <v>15</v>
@@ -7325,13 +7477,13 @@
         <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>1034</v>
+        <v>1028</v>
       </c>
       <c r="F5" t="s">
-        <v>1035</v>
+        <v>1029</v>
       </c>
       <c r="G5" t="s">
-        <v>1036</v>
+        <v>1030</v>
       </c>
       <c r="H5" t="s">
         <v>15</v>
@@ -7351,13 +7503,13 @@
         <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>1037</v>
+        <v>1031</v>
       </c>
       <c r="F6" t="s">
-        <v>1038</v>
+        <v>1032</v>
       </c>
       <c r="G6" t="s">
-        <v>1039</v>
+        <v>1033</v>
       </c>
       <c r="H6" t="s">
         <v>15</v>
@@ -7377,13 +7529,13 @@
         <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>1040</v>
+        <v>1034</v>
       </c>
       <c r="F7" t="s">
-        <v>1041</v>
+        <v>1035</v>
       </c>
       <c r="G7" t="s">
-        <v>1042</v>
+        <v>1036</v>
       </c>
       <c r="H7" t="s">
         <v>15</v>
@@ -7403,13 +7555,13 @@
         <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>1043</v>
+        <v>1037</v>
       </c>
       <c r="F8" t="s">
-        <v>1044</v>
+        <v>1038</v>
       </c>
       <c r="G8" t="s">
-        <v>1045</v>
+        <v>1039</v>
       </c>
       <c r="H8" t="s">
         <v>15</v>
@@ -7429,13 +7581,13 @@
         <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>1046</v>
+        <v>1040</v>
       </c>
       <c r="F9" t="s">
-        <v>1047</v>
+        <v>1041</v>
       </c>
       <c r="G9" t="s">
-        <v>1048</v>
+        <v>1042</v>
       </c>
       <c r="H9" t="s">
         <v>15</v>
@@ -7455,13 +7607,13 @@
         <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>1049</v>
+        <v>1043</v>
       </c>
       <c r="F10" t="s">
-        <v>1050</v>
+        <v>1044</v>
       </c>
       <c r="G10" t="s">
-        <v>1051</v>
+        <v>1045</v>
       </c>
       <c r="H10" t="s">
         <v>15</v>
@@ -7481,13 +7633,13 @@
         <v>51</v>
       </c>
       <c r="B11" t="s">
-        <v>1052</v>
+        <v>1046</v>
       </c>
       <c r="F11" t="s">
-        <v>1053</v>
+        <v>1047</v>
       </c>
       <c r="G11" t="s">
-        <v>1054</v>
+        <v>1048</v>
       </c>
       <c r="H11" t="s">
         <v>15</v>
@@ -7507,13 +7659,13 @@
         <v>51</v>
       </c>
       <c r="B12" t="s">
-        <v>1055</v>
+        <v>1049</v>
       </c>
       <c r="F12" t="s">
-        <v>1056</v>
+        <v>1050</v>
       </c>
       <c r="G12" t="s">
-        <v>1057</v>
+        <v>1051</v>
       </c>
       <c r="H12" t="s">
         <v>15</v>
@@ -7533,13 +7685,13 @@
         <v>51</v>
       </c>
       <c r="B13" t="s">
-        <v>1058</v>
+        <v>1052</v>
       </c>
       <c r="F13" t="s">
-        <v>1059</v>
+        <v>1053</v>
       </c>
       <c r="G13" t="s">
-        <v>1060</v>
+        <v>1054</v>
       </c>
       <c r="H13" t="s">
         <v>15</v>
@@ -7559,13 +7711,13 @@
         <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>1061</v>
+        <v>1055</v>
       </c>
       <c r="F14" t="s">
-        <v>1062</v>
+        <v>1056</v>
       </c>
       <c r="G14" t="s">
-        <v>1063</v>
+        <v>1057</v>
       </c>
       <c r="H14" t="s">
         <v>15</v>
@@ -7585,13 +7737,13 @@
         <v>51</v>
       </c>
       <c r="B15" t="s">
-        <v>1064</v>
+        <v>1058</v>
       </c>
       <c r="F15" t="s">
-        <v>1065</v>
+        <v>1059</v>
       </c>
       <c r="G15" t="s">
-        <v>1066</v>
+        <v>1060</v>
       </c>
       <c r="H15" t="s">
         <v>15</v>
@@ -7616,10 +7768,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7673,13 +7825,13 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>1023</v>
+        <v>1017</v>
       </c>
       <c r="F3" t="s">
-        <v>1022</v>
+        <v>1016</v>
       </c>
       <c r="G3" t="s">
-        <v>1021</v>
+        <v>1015</v>
       </c>
       <c r="H3" t="s">
         <v>15</v>
@@ -7696,10 +7848,10 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>1020</v>
+        <v>1014</v>
       </c>
       <c r="F4" t="s">
-        <v>1019</v>
+        <v>1013</v>
       </c>
       <c r="G4" t="s">
         <v>802</v>
@@ -7719,13 +7871,13 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>1018</v>
+        <v>1012</v>
       </c>
       <c r="F5" t="s">
-        <v>1017</v>
+        <v>1011</v>
       </c>
       <c r="G5" t="s">
-        <v>1016</v>
+        <v>1010</v>
       </c>
       <c r="H5" t="s">
         <v>15</v>
@@ -7742,10 +7894,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>1015</v>
+        <v>1009</v>
       </c>
       <c r="F6" t="s">
-        <v>1014</v>
+        <v>1008</v>
       </c>
       <c r="G6" t="s">
         <v>807</v>
@@ -7765,10 +7917,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>1013</v>
+        <v>1007</v>
       </c>
       <c r="F7" t="s">
-        <v>1012</v>
+        <v>1006</v>
       </c>
       <c r="G7" t="s">
         <v>843</v>
@@ -7788,13 +7940,13 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>1011</v>
+        <v>1005</v>
       </c>
       <c r="F8" t="s">
-        <v>1010</v>
+        <v>1004</v>
       </c>
       <c r="G8" t="s">
-        <v>1009</v>
+        <v>1003</v>
       </c>
       <c r="H8" t="s">
         <v>15</v>
@@ -7811,13 +7963,13 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>1008</v>
+        <v>1002</v>
       </c>
       <c r="F9" t="s">
-        <v>1007</v>
+        <v>1001</v>
       </c>
       <c r="G9" t="s">
-        <v>1006</v>
+        <v>1000</v>
       </c>
       <c r="H9" t="s">
         <v>15</v>
@@ -7834,13 +7986,13 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>1005</v>
+        <v>999</v>
       </c>
       <c r="F10" t="s">
-        <v>1004</v>
+        <v>998</v>
       </c>
       <c r="G10" t="s">
-        <v>1003</v>
+        <v>997</v>
       </c>
       <c r="H10" t="s">
         <v>15</v>
@@ -7857,13 +8009,13 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>1002</v>
+        <v>996</v>
       </c>
       <c r="F11" t="s">
-        <v>1001</v>
+        <v>995</v>
       </c>
       <c r="G11" t="s">
-        <v>1000</v>
+        <v>994</v>
       </c>
       <c r="H11" t="s">
         <v>15</v>
@@ -7879,71 +8031,28 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>1160</v>
+      <c r="A12" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1154</v>
       </c>
       <c r="F12" t="s">
-        <v>999</v>
+        <v>1156</v>
       </c>
       <c r="G12" t="s">
-        <v>998</v>
+        <v>1155</v>
       </c>
       <c r="H12" t="s">
         <v>15</v>
       </c>
       <c r="I12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J12" t="s">
         <v>15</v>
       </c>
       <c r="K12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>1161</v>
-      </c>
-      <c r="F13" t="s">
-        <v>997</v>
-      </c>
-      <c r="G13" t="s">
-        <v>996</v>
-      </c>
-      <c r="H13" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" t="s">
-        <v>16</v>
-      </c>
-      <c r="J13" t="s">
-        <v>15</v>
-      </c>
-      <c r="K13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>1162</v>
-      </c>
-      <c r="F14" t="s">
-        <v>995</v>
-      </c>
-      <c r="G14" t="s">
-        <v>994</v>
-      </c>
-      <c r="H14" t="s">
-        <v>15</v>
-      </c>
-      <c r="I14" t="s">
-        <v>16</v>
-      </c>
-      <c r="J14" t="s">
-        <v>15</v>
-      </c>
-      <c r="K14" t="s">
         <v>16</v>
       </c>
     </row>
@@ -7960,7 +8069,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8020,7 +8129,7 @@
         <v>52</v>
       </c>
       <c r="E3" t="s">
-        <v>1024</v>
+        <v>1018</v>
       </c>
       <c r="F3" t="s">
         <v>13</v>
@@ -8049,7 +8158,7 @@
         <v>53</v>
       </c>
       <c r="E4" t="s">
-        <v>1024</v>
+        <v>1018</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
@@ -8078,7 +8187,7 @@
         <v>54</v>
       </c>
       <c r="E5" t="s">
-        <v>1024</v>
+        <v>1018</v>
       </c>
       <c r="F5" t="s">
         <v>19</v>
@@ -8104,16 +8213,16 @@
         <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>1025</v>
+        <v>1019</v>
       </c>
       <c r="E6" t="s">
-        <v>1024</v>
+        <v>1018</v>
       </c>
       <c r="F6" t="s">
-        <v>1026</v>
+        <v>1020</v>
       </c>
       <c r="G6" t="s">
-        <v>1027</v>
+        <v>1021</v>
       </c>
       <c r="H6" t="s">
         <v>15</v>
@@ -8136,7 +8245,7 @@
         <v>55</v>
       </c>
       <c r="E7" t="s">
-        <v>1024</v>
+        <v>1018</v>
       </c>
       <c r="F7" t="s">
         <v>21</v>
@@ -8420,16 +8529,16 @@
         <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>1159</v>
+        <v>1153</v>
       </c>
       <c r="E17" t="s">
         <v>57</v>
       </c>
       <c r="F17" t="s">
-        <v>1157</v>
+        <v>1151</v>
       </c>
       <c r="G17" t="s">
-        <v>1158</v>
+        <v>1152</v>
       </c>
       <c r="H17" t="s">
         <v>15</v>
@@ -8514,10 +8623,10 @@
         <v>72</v>
       </c>
       <c r="F3" t="s">
-        <v>1135</v>
+        <v>1129</v>
       </c>
       <c r="G3" t="s">
-        <v>1156</v>
+        <v>1150</v>
       </c>
       <c r="H3" t="s">
         <v>15</v>
@@ -8531,10 +8640,10 @@
         <v>73</v>
       </c>
       <c r="F4" t="s">
-        <v>1136</v>
+        <v>1130</v>
       </c>
       <c r="G4" t="s">
-        <v>1155</v>
+        <v>1149</v>
       </c>
       <c r="H4" t="s">
         <v>15</v>
@@ -8554,10 +8663,10 @@
         <v>74</v>
       </c>
       <c r="F5" t="s">
-        <v>1137</v>
+        <v>1131</v>
       </c>
       <c r="G5" t="s">
-        <v>1154</v>
+        <v>1148</v>
       </c>
       <c r="H5" t="s">
         <v>15</v>
@@ -8571,10 +8680,10 @@
         <v>75</v>
       </c>
       <c r="F6" t="s">
-        <v>1138</v>
+        <v>1132</v>
       </c>
       <c r="G6" t="s">
-        <v>1153</v>
+        <v>1147</v>
       </c>
       <c r="H6" t="s">
         <v>15</v>
@@ -8588,10 +8697,10 @@
         <v>76</v>
       </c>
       <c r="F7" t="s">
-        <v>1139</v>
+        <v>1133</v>
       </c>
       <c r="G7" t="s">
-        <v>1152</v>
+        <v>1146</v>
       </c>
       <c r="H7" t="s">
         <v>15</v>
@@ -8611,10 +8720,10 @@
         <v>77</v>
       </c>
       <c r="F8" t="s">
-        <v>1140</v>
+        <v>1134</v>
       </c>
       <c r="G8" t="s">
-        <v>1151</v>
+        <v>1145</v>
       </c>
       <c r="H8" t="s">
         <v>15</v>
@@ -8628,10 +8737,10 @@
         <v>78</v>
       </c>
       <c r="F9" t="s">
-        <v>1141</v>
+        <v>1135</v>
       </c>
       <c r="G9" t="s">
-        <v>1150</v>
+        <v>1144</v>
       </c>
       <c r="H9" t="s">
         <v>15</v>
@@ -8645,10 +8754,10 @@
         <v>79</v>
       </c>
       <c r="F10" t="s">
-        <v>1142</v>
+        <v>1136</v>
       </c>
       <c r="G10" t="s">
-        <v>1149</v>
+        <v>1143</v>
       </c>
       <c r="H10" t="s">
         <v>15</v>
@@ -8662,10 +8771,10 @@
         <v>80</v>
       </c>
       <c r="F11" t="s">
-        <v>1143</v>
+        <v>1137</v>
       </c>
       <c r="G11" t="s">
-        <v>1146</v>
+        <v>1140</v>
       </c>
       <c r="H11" t="s">
         <v>15</v>
@@ -8679,10 +8788,10 @@
         <v>81</v>
       </c>
       <c r="F12" t="s">
-        <v>1144</v>
+        <v>1138</v>
       </c>
       <c r="G12" t="s">
-        <v>1147</v>
+        <v>1141</v>
       </c>
       <c r="H12" t="s">
         <v>15</v>
@@ -8696,10 +8805,10 @@
         <v>82</v>
       </c>
       <c r="F13" t="s">
-        <v>1145</v>
+        <v>1139</v>
       </c>
       <c r="G13" t="s">
-        <v>1148</v>
+        <v>1142</v>
       </c>
       <c r="H13" t="s">
         <v>15</v>
@@ -8717,8 +8826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493D947D-D359-42F9-887E-EA748C65C63F}">
   <dimension ref="A1:N255"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView topLeftCell="A152" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C182" sqref="C182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Expand RSD process sets and tables
- buildings (apartments, attached, detached)
- space heating/cooling and hot water supply
</commit_message>
<xml_diff>
--- a/SetRules.xlsx
+++ b/SetRules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB225BC-9D44-4A6C-9E19-646A7C0619DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758CE543-923A-4EAF-A22B-E138F362EBBF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{69765015-6AAF-4B94-8956-691CCC759B47}"/>
+    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" activeTab="4" xr2:uid="{69765015-6AAF-4B94-8956-691CCC759B47}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets-Comm" sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2944" uniqueCount="1170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3045" uniqueCount="1212">
   <si>
     <t>~TFM_Psets</t>
   </si>
@@ -3553,6 +3553,132 @@
   </si>
   <si>
     <t>RSD*,-*_*t</t>
+  </si>
+  <si>
+    <t>Residential - Buildings - Apartments</t>
+  </si>
+  <si>
+    <t>Residential - Buildings - Attached</t>
+  </si>
+  <si>
+    <t>Residential - Buildings - Detached</t>
+  </si>
+  <si>
+    <t>DMD_RSD-BLD-APT</t>
+  </si>
+  <si>
+    <t>DMD_RSD-BLD-ATT</t>
+  </si>
+  <si>
+    <t>DMD_RSD-BLD-DET</t>
+  </si>
+  <si>
+    <t>R*BLD*APT*</t>
+  </si>
+  <si>
+    <t>R*BLD*ATT*</t>
+  </si>
+  <si>
+    <t>R*BLD*DET*</t>
+  </si>
+  <si>
+    <t>R*SW*N*,-R*HP*,-R*HET*</t>
+  </si>
+  <si>
+    <t>R*SW*HP*N*</t>
+  </si>
+  <si>
+    <t>R*SW*HET*N*</t>
+  </si>
+  <si>
+    <t>R*SH*N*,-R*HP*</t>
+  </si>
+  <si>
+    <t>R*HC*HP*N*</t>
+  </si>
+  <si>
+    <t>R*SC*N*</t>
+  </si>
+  <si>
+    <t>R*WH*N*,-R*WH*SOL*</t>
+  </si>
+  <si>
+    <t>R*WH*SOL*N*</t>
+  </si>
+  <si>
+    <t>R*SH*X*</t>
+  </si>
+  <si>
+    <t>R*WH*X*</t>
+  </si>
+  <si>
+    <t>Residential - Space and Water Heating - New Boilers</t>
+  </si>
+  <si>
+    <t>Residential - Space and Water Heating - New Heat Pumps</t>
+  </si>
+  <si>
+    <t>Residential - Space and Water Heating - New District Heating</t>
+  </si>
+  <si>
+    <t>Residential - Space Heating - New Boilers</t>
+  </si>
+  <si>
+    <t>Residential - Space Heating - New Heat Pumps</t>
+  </si>
+  <si>
+    <t>Residential - Space Heating and Cooling - New Heat Pumps</t>
+  </si>
+  <si>
+    <t>Residential - Space Cooling - New Air Conditioners</t>
+  </si>
+  <si>
+    <t>Residential - Water Heating - New Boilers</t>
+  </si>
+  <si>
+    <t>Residential - Water Heating - New Solar</t>
+  </si>
+  <si>
+    <t>RSD_TECH-SW-N-BOILERS</t>
+  </si>
+  <si>
+    <t>RSD_TECH-SW-N-HP</t>
+  </si>
+  <si>
+    <t>RSD_TECH-SW-N-DH</t>
+  </si>
+  <si>
+    <t>RSD_TECH-SH-N-BOILERS</t>
+  </si>
+  <si>
+    <t>RSD_TECH-SH-N-HP</t>
+  </si>
+  <si>
+    <t>RSD_TECH-HC-N-HP</t>
+  </si>
+  <si>
+    <t>RSD_TECH-SC-N-AC</t>
+  </si>
+  <si>
+    <t>RSD_TECH-WH-N-BOILERS</t>
+  </si>
+  <si>
+    <t>RSD_TECH-WH-N-SOLAR</t>
+  </si>
+  <si>
+    <t>RSD_TECH-SH-E</t>
+  </si>
+  <si>
+    <t>RSD_TECH-WH-E</t>
+  </si>
+  <si>
+    <t>Residential - Water Heating - Existing</t>
+  </si>
+  <si>
+    <t>Residential - Space Heating - Existing</t>
+  </si>
+  <si>
+    <t>R*SH*HP*N*</t>
   </si>
 </sst>
 </file>
@@ -3920,7 +4046,7 @@
   </sheetPr>
   <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A42" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
@@ -7368,7 +7494,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="H15" sqref="H15:K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7768,15 +7894,15 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="40.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8053,6 +8179,337 @@
         <v>15</v>
       </c>
       <c r="K12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1176</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1173</v>
+      </c>
+      <c r="G13" t="s">
+        <v>1170</v>
+      </c>
+      <c r="H13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1177</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1174</v>
+      </c>
+      <c r="G14" t="s">
+        <v>1171</v>
+      </c>
+      <c r="H14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" t="s">
+        <v>16</v>
+      </c>
+      <c r="J14" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1178</v>
+      </c>
+      <c r="F15" t="s">
+        <v>1175</v>
+      </c>
+      <c r="G15" t="s">
+        <v>1172</v>
+      </c>
+      <c r="H15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J15" t="s">
+        <v>15</v>
+      </c>
+      <c r="K15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>1179</v>
+      </c>
+      <c r="F16" t="s">
+        <v>1198</v>
+      </c>
+      <c r="G16" t="s">
+        <v>1189</v>
+      </c>
+      <c r="H16" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" t="s">
+        <v>16</v>
+      </c>
+      <c r="J16" t="s">
+        <v>15</v>
+      </c>
+      <c r="K16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>1180</v>
+      </c>
+      <c r="F17" t="s">
+        <v>1199</v>
+      </c>
+      <c r="G17" t="s">
+        <v>1190</v>
+      </c>
+      <c r="H17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" t="s">
+        <v>16</v>
+      </c>
+      <c r="J17" t="s">
+        <v>15</v>
+      </c>
+      <c r="K17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>1181</v>
+      </c>
+      <c r="F18" t="s">
+        <v>1200</v>
+      </c>
+      <c r="G18" t="s">
+        <v>1191</v>
+      </c>
+      <c r="H18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" t="s">
+        <v>16</v>
+      </c>
+      <c r="J18" t="s">
+        <v>15</v>
+      </c>
+      <c r="K18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>1182</v>
+      </c>
+      <c r="F19" t="s">
+        <v>1201</v>
+      </c>
+      <c r="G19" t="s">
+        <v>1192</v>
+      </c>
+      <c r="H19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" t="s">
+        <v>16</v>
+      </c>
+      <c r="J19" t="s">
+        <v>15</v>
+      </c>
+      <c r="K19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>1211</v>
+      </c>
+      <c r="F20" t="s">
+        <v>1202</v>
+      </c>
+      <c r="G20" t="s">
+        <v>1193</v>
+      </c>
+      <c r="H20" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" t="s">
+        <v>16</v>
+      </c>
+      <c r="J20" t="s">
+        <v>15</v>
+      </c>
+      <c r="K20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>1183</v>
+      </c>
+      <c r="F21" t="s">
+        <v>1203</v>
+      </c>
+      <c r="G21" t="s">
+        <v>1194</v>
+      </c>
+      <c r="H21" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" t="s">
+        <v>16</v>
+      </c>
+      <c r="J21" t="s">
+        <v>15</v>
+      </c>
+      <c r="K21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>1184</v>
+      </c>
+      <c r="F22" t="s">
+        <v>1204</v>
+      </c>
+      <c r="G22" t="s">
+        <v>1195</v>
+      </c>
+      <c r="H22" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" t="s">
+        <v>16</v>
+      </c>
+      <c r="J22" t="s">
+        <v>15</v>
+      </c>
+      <c r="K22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>1185</v>
+      </c>
+      <c r="F23" t="s">
+        <v>1205</v>
+      </c>
+      <c r="G23" t="s">
+        <v>1196</v>
+      </c>
+      <c r="H23" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" t="s">
+        <v>16</v>
+      </c>
+      <c r="J23" t="s">
+        <v>15</v>
+      </c>
+      <c r="K23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F24" t="s">
+        <v>1206</v>
+      </c>
+      <c r="G24" t="s">
+        <v>1197</v>
+      </c>
+      <c r="H24" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" t="s">
+        <v>16</v>
+      </c>
+      <c r="J24" t="s">
+        <v>15</v>
+      </c>
+      <c r="K24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>1187</v>
+      </c>
+      <c r="F25" t="s">
+        <v>1207</v>
+      </c>
+      <c r="G25" t="s">
+        <v>1210</v>
+      </c>
+      <c r="H25" t="s">
+        <v>15</v>
+      </c>
+      <c r="I25" t="s">
+        <v>16</v>
+      </c>
+      <c r="J25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>1188</v>
+      </c>
+      <c r="F26" t="s">
+        <v>1208</v>
+      </c>
+      <c r="G26" t="s">
+        <v>1209</v>
+      </c>
+      <c r="H26" t="s">
+        <v>15</v>
+      </c>
+      <c r="I26" t="s">
+        <v>16</v>
+      </c>
+      <c r="J26" t="s">
+        <v>15</v>
+      </c>
+      <c r="K26" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add a process set and a FEC table for Construction IND
</commit_message>
<xml_diff>
--- a/SetRules.xlsx
+++ b/SetRules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758CE543-923A-4EAF-A22B-E138F362EBBF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDF54747-F701-4C65-B551-C9418E8D70AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" activeTab="4" xr2:uid="{69765015-6AAF-4B94-8956-691CCC759B47}"/>
+    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" xr2:uid="{69765015-6AAF-4B94-8956-691CCC759B47}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets-Comm" sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3045" uniqueCount="1212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3053" uniqueCount="1215">
   <si>
     <t>~TFM_Psets</t>
   </si>
@@ -3679,6 +3679,15 @@
   </si>
   <si>
     <t>R*SH*HP*N*</t>
+  </si>
+  <si>
+    <t>I*CON*</t>
+  </si>
+  <si>
+    <t>DMD_IND-CON</t>
+  </si>
+  <si>
+    <t>Industry - Construction</t>
   </si>
 </sst>
 </file>
@@ -4046,8 +4055,8 @@
   </sheetPr>
   <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7491,10 +7500,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15:K15"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7881,6 +7890,32 @@
         <v>15</v>
       </c>
       <c r="K15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1212</v>
+      </c>
+      <c r="F16" t="s">
+        <v>1213</v>
+      </c>
+      <c r="G16" t="s">
+        <v>1214</v>
+      </c>
+      <c r="H16" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" t="s">
+        <v>16</v>
+      </c>
+      <c r="J16" t="s">
+        <v>15</v>
+      </c>
+      <c r="K16" t="s">
         <v>16</v>
       </c>
     </row>
@@ -7896,7 +7931,7 @@
   </sheetPr>
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add a table on hydrogen supply
</commit_message>
<xml_diff>
--- a/SetRules.xlsx
+++ b/SetRules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80ACB2AD-3FDA-4401-B394-DA92864953DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF740041-D1B2-4216-8DB7-0D83311FAF19}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" firstSheet="2" activeTab="5" xr2:uid="{69765015-6AAF-4B94-8956-691CCC759B47}"/>
+    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" firstSheet="2" activeTab="7" xr2:uid="{69765015-6AAF-4B94-8956-691CCC759B47}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets-Comm" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,8 @@
     <sheet name="RSD_Sets-Proc" sheetId="9" r:id="rId5"/>
     <sheet name="TRA_Sets-Proc" sheetId="10" r:id="rId6"/>
     <sheet name="PWR_Sets-Proc" sheetId="8" r:id="rId7"/>
-    <sheet name="extra_Sets-Proc" sheetId="4" r:id="rId8"/>
+    <sheet name="SUP_Sets-Proc" sheetId="12" r:id="rId8"/>
+    <sheet name="extra_Sets-Proc" sheetId="4" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3406" uniqueCount="1348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3426" uniqueCount="1351">
   <si>
     <t>~TFM_Psets</t>
   </si>
@@ -4087,6 +4088,15 @@
   </si>
   <si>
     <t xml:space="preserve">Passenger transport - light goods truck - plugin hybrid electric </t>
+  </si>
+  <si>
+    <t>SH2P*ELC*</t>
+  </si>
+  <si>
+    <t>SUP-H2-Electrolysis</t>
+  </si>
+  <si>
+    <t>Hydrogen Generation - Electrolysis</t>
   </si>
 </sst>
 </file>
@@ -9398,7 +9408,7 @@
   </sheetPr>
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
@@ -10867,6 +10877,94 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B790B4BC-8607-4508-A698-E46A5EB98EA7}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="53.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>1348</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1349</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1350</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493D947D-D359-42F9-887E-EA748C65C63F}">
   <dimension ref="A1:N255"/>
   <sheetViews>

</xml_diff>

<commit_message>
Update tables and sets for RSD
</commit_message>
<xml_diff>
--- a/SetRules.xlsx
+++ b/SetRules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr backupFile="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A641A5E6-E400-490B-8AC0-C4C159B2A547}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D667FB43-5CF1-41D1-8B1E-D348AE4B4C94}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="9" xr2:uid="{69765015-6AAF-4B94-8956-691CCC759B47}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="4" xr2:uid="{69765015-6AAF-4B94-8956-691CCC759B47}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets-Comm" sheetId="5" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3518" uniqueCount="1370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3390" uniqueCount="1319">
   <si>
     <t>~TFM_Psets</t>
   </si>
@@ -2970,75 +2970,30 @@
     <t>Transport Train Long Distance</t>
   </si>
   <si>
-    <t>Residential Refrigeration</t>
-  </si>
-  <si>
-    <t>RSD_NRGSRV-RF</t>
-  </si>
-  <si>
     <t>R-RSDRF*</t>
   </si>
   <si>
-    <t>Residential Pump and Fans</t>
-  </si>
-  <si>
-    <t>RSD_NRGSRV-PF</t>
-  </si>
-  <si>
     <t>R-PF*</t>
   </si>
   <si>
-    <t>Residential Electric Appliances</t>
-  </si>
-  <si>
-    <t>RSD_NRGSRV-OE</t>
-  </si>
-  <si>
     <t>R-RSDOE*</t>
   </si>
   <si>
-    <t>Residential Other Applications</t>
-  </si>
-  <si>
-    <t>RSD_NRGSRV-OA</t>
-  </si>
-  <si>
     <t>R-RSDOA*</t>
   </si>
   <si>
-    <t>RSD_NRGSRV-LT</t>
-  </si>
-  <si>
     <t>R-LT*</t>
   </si>
   <si>
-    <t>RSD_NRGSRV-DW</t>
-  </si>
-  <si>
     <t>R-RSDDW*</t>
   </si>
   <si>
-    <t>Residential Cloth Washing</t>
-  </si>
-  <si>
-    <t>RSD_NRGSRV-CW</t>
-  </si>
-  <si>
     <t>R-RSDCW*</t>
   </si>
   <si>
-    <t>RSD_NRGSRV-CK</t>
-  </si>
-  <si>
     <t>R-RSDCK*</t>
   </si>
   <si>
-    <t>Residential Cloth Drying</t>
-  </si>
-  <si>
-    <t>RSD_NRGSRV-CD</t>
-  </si>
-  <si>
     <t>R-RSDCD*</t>
   </si>
   <si>
@@ -3414,12 +3369,6 @@
     <t>RSDWH*,RSDSH*,RSDSC*</t>
   </si>
   <si>
-    <t>Residential Hot Water and Space Heating and Cooling</t>
-  </si>
-  <si>
-    <t>RSD_NRGSRV-WS</t>
-  </si>
-  <si>
     <t>-IRE</t>
   </si>
   <si>
@@ -3480,105 +3429,6 @@
     <t>R*BLD*DET*</t>
   </si>
   <si>
-    <t>R*SW*N*,-R*HP*,-R*HET*</t>
-  </si>
-  <si>
-    <t>R*SW*HP*N*</t>
-  </si>
-  <si>
-    <t>R*SW*HET*N*</t>
-  </si>
-  <si>
-    <t>R*SH*N*,-R*HP*</t>
-  </si>
-  <si>
-    <t>R*HC*HP*N*</t>
-  </si>
-  <si>
-    <t>R*SC*N*</t>
-  </si>
-  <si>
-    <t>R*WH*N*,-R*WH*SOL*</t>
-  </si>
-  <si>
-    <t>R*WH*SOL*N*</t>
-  </si>
-  <si>
-    <t>R*SH*X*</t>
-  </si>
-  <si>
-    <t>R*WH*X*</t>
-  </si>
-  <si>
-    <t>Residential - Space and Water Heating - New Boilers</t>
-  </si>
-  <si>
-    <t>Residential - Space and Water Heating - New Heat Pumps</t>
-  </si>
-  <si>
-    <t>Residential - Space and Water Heating - New District Heating</t>
-  </si>
-  <si>
-    <t>Residential - Space Heating - New Boilers</t>
-  </si>
-  <si>
-    <t>Residential - Space Heating - New Heat Pumps</t>
-  </si>
-  <si>
-    <t>Residential - Space Heating and Cooling - New Heat Pumps</t>
-  </si>
-  <si>
-    <t>Residential - Space Cooling - New Air Conditioners</t>
-  </si>
-  <si>
-    <t>Residential - Water Heating - New Boilers</t>
-  </si>
-  <si>
-    <t>Residential - Water Heating - New Solar</t>
-  </si>
-  <si>
-    <t>RSD_TECH-SW-N-BOILERS</t>
-  </si>
-  <si>
-    <t>RSD_TECH-SW-N-HP</t>
-  </si>
-  <si>
-    <t>RSD_TECH-SW-N-DH</t>
-  </si>
-  <si>
-    <t>RSD_TECH-SH-N-BOILERS</t>
-  </si>
-  <si>
-    <t>RSD_TECH-SH-N-HP</t>
-  </si>
-  <si>
-    <t>RSD_TECH-HC-N-HP</t>
-  </si>
-  <si>
-    <t>RSD_TECH-SC-N-AC</t>
-  </si>
-  <si>
-    <t>RSD_TECH-WH-N-BOILERS</t>
-  </si>
-  <si>
-    <t>RSD_TECH-WH-N-SOLAR</t>
-  </si>
-  <si>
-    <t>RSD_TECH-SH-E</t>
-  </si>
-  <si>
-    <t>RSD_TECH-WH-E</t>
-  </si>
-  <si>
-    <t>Residential - Water Heating - Existing</t>
-  </si>
-  <si>
-    <t>Residential - Space Heating - Existing</t>
-  </si>
-  <si>
-    <t>R*SH*HP*N*</t>
-  </si>
-  <si>
     <t>I*CON*</t>
   </si>
   <si>
@@ -3699,126 +3549,6 @@
     <t>MIN*,-*WLK,-*CYC</t>
   </si>
   <si>
-    <t>RSD_TECH-HP</t>
-  </si>
-  <si>
-    <t>RSD_TECH-AC</t>
-  </si>
-  <si>
-    <t>RSD_TECH-DH</t>
-  </si>
-  <si>
-    <t>RSD_TECH-BOILERS</t>
-  </si>
-  <si>
-    <t>Residential - Heat Pumps</t>
-  </si>
-  <si>
-    <t>Residential - Boiler</t>
-  </si>
-  <si>
-    <t>Residential - Air Conditioners</t>
-  </si>
-  <si>
-    <t>Residential - Heat Exchangers</t>
-  </si>
-  <si>
-    <t>R*HP*,R*ELC_X1</t>
-  </si>
-  <si>
-    <t>R*SC*ELC_N*</t>
-  </si>
-  <si>
-    <t>R*t_het*</t>
-  </si>
-  <si>
-    <t>R*t_*</t>
-  </si>
-  <si>
-    <t>RSDSH*,RSDWH*</t>
-  </si>
-  <si>
-    <t>RSD_TECH-SH-APT</t>
-  </si>
-  <si>
-    <t>RSD_TECH-SH-ATT</t>
-  </si>
-  <si>
-    <t>RSD_TECH-SH-DET</t>
-  </si>
-  <si>
-    <t>RSD_TECH-WH-APT</t>
-  </si>
-  <si>
-    <t>RSD_TECH-WH-ATT</t>
-  </si>
-  <si>
-    <t>RSD_TECH-WH-DET</t>
-  </si>
-  <si>
-    <t>RSD_TECH-SC-APT</t>
-  </si>
-  <si>
-    <t>RSD_TECH-SC-ATT</t>
-  </si>
-  <si>
-    <t>RSD_TECH-SC-DET</t>
-  </si>
-  <si>
-    <t>RSDSH_APT</t>
-  </si>
-  <si>
-    <t>RSDSH_ATT</t>
-  </si>
-  <si>
-    <t>RSDSH_DET</t>
-  </si>
-  <si>
-    <t>RSDWH_APT</t>
-  </si>
-  <si>
-    <t>RSDWH_ATT</t>
-  </si>
-  <si>
-    <t>RSDWH_DET</t>
-  </si>
-  <si>
-    <t>RSDSC_DET</t>
-  </si>
-  <si>
-    <t>RSDSC_APT</t>
-  </si>
-  <si>
-    <t>RSDSC_ATT</t>
-  </si>
-  <si>
-    <t>Residential - Space Heating - Apartments</t>
-  </si>
-  <si>
-    <t>Residential - Space Heating - Attached</t>
-  </si>
-  <si>
-    <t>Residential - Space Heating - Detached</t>
-  </si>
-  <si>
-    <t>Residential - Water Heating - Apartments</t>
-  </si>
-  <si>
-    <t>Residential - Water Heating - Attached</t>
-  </si>
-  <si>
-    <t>Residential - Water Heating - Detached</t>
-  </si>
-  <si>
-    <t>Residential - Space Cooling - Apartments</t>
-  </si>
-  <si>
-    <t>Residential - Space Cooling - Attached</t>
-  </si>
-  <si>
-    <t>Residential - Space Cooling - Detached</t>
-  </si>
-  <si>
     <t>TAVIDOM</t>
   </si>
   <si>
@@ -4156,6 +3886,123 @@
   </si>
   <si>
     <t>Services energy carriers</t>
+  </si>
+  <si>
+    <t>RSD_BLD-XXX_NRGSRV-CD</t>
+  </si>
+  <si>
+    <t>RSD_BLD-XXX_NRGSRV-CK</t>
+  </si>
+  <si>
+    <t>RSD_BLD-XXX_NRGSRV-CW</t>
+  </si>
+  <si>
+    <t>RSD_BLD-XXX_NRGSRV-DW</t>
+  </si>
+  <si>
+    <t>RSD_BLD-XXX_NRGSRV-LT</t>
+  </si>
+  <si>
+    <t>RSD_BLD-XXX_NRGSRV-OA</t>
+  </si>
+  <si>
+    <t>RSD_BLD-XXX_NRGSRV-OE</t>
+  </si>
+  <si>
+    <t>RSD_BLD-XXX_NRGSRV-PF</t>
+  </si>
+  <si>
+    <t>RSD_BLD-XXX_NRGSRV-RF</t>
+  </si>
+  <si>
+    <t>RSD_BLD-XXX_NRGSRV-WS</t>
+  </si>
+  <si>
+    <t>Residential - All Buildings - Cloth Drying</t>
+  </si>
+  <si>
+    <t>Residential  - All Buildings - Cooking</t>
+  </si>
+  <si>
+    <t>Residential - All Buildings - Cloth Washing</t>
+  </si>
+  <si>
+    <t>Residential - All Buildings - Dish Washing</t>
+  </si>
+  <si>
+    <t>Residential - All Buildings - Lighting</t>
+  </si>
+  <si>
+    <t>Residential - All Buildings - Other Applications</t>
+  </si>
+  <si>
+    <t>Residential - All Buildings - Electric Appliances</t>
+  </si>
+  <si>
+    <t>Residential - All Buildings - Pump and Fans</t>
+  </si>
+  <si>
+    <t>Residential - All Buildings - Refrigeration</t>
+  </si>
+  <si>
+    <t>Residential - All Buildings - Hot Water and Space Heating and Cooling</t>
+  </si>
+  <si>
+    <t>Residential - Apartments - Hot Water and Space Heating and Cooling</t>
+  </si>
+  <si>
+    <t>Residential - Attached - Hot Water and Space Heating and Cooling</t>
+  </si>
+  <si>
+    <t>Residential - Detached - Hot Water and Space Heating and Cooling</t>
+  </si>
+  <si>
+    <t>RSD_BLD-APT_NRGSRV-WS</t>
+  </si>
+  <si>
+    <t>RSD_BLD-ATT_NRGSRV-WS</t>
+  </si>
+  <si>
+    <t>RSD_BLD-DET_NRGSRV-WS</t>
+  </si>
+  <si>
+    <t>R*,-R-RTFT*</t>
+  </si>
+  <si>
+    <t>R-RTFT*</t>
+  </si>
+  <si>
+    <t>RSD_BLD-XXX_RTFT</t>
+  </si>
+  <si>
+    <t>Residential - All Buildings - Retrofits</t>
+  </si>
+  <si>
+    <t>Residential - Apartments - Retrofits</t>
+  </si>
+  <si>
+    <t>Residential - Attached - Retrofits</t>
+  </si>
+  <si>
+    <t>Residential - Detached - Retrofits</t>
+  </si>
+  <si>
+    <t>R*APT*</t>
+  </si>
+  <si>
+    <t>R*ATT*</t>
+  </si>
+  <si>
+    <t>R*DET*</t>
+  </si>
+  <si>
+    <t>RSD_BLD-APT_RTFT</t>
+  </si>
+  <si>
+    <t>RSD_BLD-ATT_RTFT</t>
+  </si>
+  <si>
+    <t>RSD_BLD-DET_RTFT</t>
   </si>
 </sst>
 </file>
@@ -4604,10 +4451,10 @@
         <v>184</v>
       </c>
       <c r="D4" t="s">
-        <v>1352</v>
+        <v>1262</v>
       </c>
       <c r="E4" t="s">
-        <v>1361</v>
+        <v>1271</v>
       </c>
       <c r="F4" t="s">
         <v>15</v>
@@ -4708,7 +4555,7 @@
         <v>188</v>
       </c>
       <c r="D8" t="s">
-        <v>1042</v>
+        <v>1027</v>
       </c>
       <c r="E8" t="s">
         <v>123</v>
@@ -4734,7 +4581,7 @@
         <v>189</v>
       </c>
       <c r="D9" t="s">
-        <v>1043</v>
+        <v>1028</v>
       </c>
       <c r="E9" t="s">
         <v>124</v>
@@ -4760,10 +4607,10 @@
         <v>190</v>
       </c>
       <c r="D10" t="s">
-        <v>1353</v>
+        <v>1263</v>
       </c>
       <c r="E10" t="s">
-        <v>1362</v>
+        <v>1272</v>
       </c>
       <c r="F10" t="s">
         <v>15</v>
@@ -4786,7 +4633,7 @@
         <v>191</v>
       </c>
       <c r="D11" t="s">
-        <v>1044</v>
+        <v>1029</v>
       </c>
       <c r="E11" t="s">
         <v>125</v>
@@ -4812,7 +4659,7 @@
         <v>192</v>
       </c>
       <c r="D12" t="s">
-        <v>1045</v>
+        <v>1030</v>
       </c>
       <c r="E12" t="s">
         <v>126</v>
@@ -4838,7 +4685,7 @@
         <v>193</v>
       </c>
       <c r="D13" t="s">
-        <v>1046</v>
+        <v>1031</v>
       </c>
       <c r="E13" t="s">
         <v>127</v>
@@ -4864,7 +4711,7 @@
         <v>194</v>
       </c>
       <c r="D14" t="s">
-        <v>1047</v>
+        <v>1032</v>
       </c>
       <c r="E14" t="s">
         <v>128</v>
@@ -4890,7 +4737,7 @@
         <v>195</v>
       </c>
       <c r="D15" t="s">
-        <v>1048</v>
+        <v>1033</v>
       </c>
       <c r="E15" t="s">
         <v>129</v>
@@ -4916,7 +4763,7 @@
         <v>196</v>
       </c>
       <c r="D16" t="s">
-        <v>1049</v>
+        <v>1034</v>
       </c>
       <c r="E16" t="s">
         <v>131</v>
@@ -4942,7 +4789,7 @@
         <v>197</v>
       </c>
       <c r="D17" t="s">
-        <v>1050</v>
+        <v>1035</v>
       </c>
       <c r="E17" t="s">
         <v>132</v>
@@ -4968,10 +4815,10 @@
         <v>198</v>
       </c>
       <c r="D18" t="s">
-        <v>1354</v>
+        <v>1264</v>
       </c>
       <c r="E18" t="s">
-        <v>1363</v>
+        <v>1273</v>
       </c>
       <c r="F18" t="s">
         <v>15</v>
@@ -4994,7 +4841,7 @@
         <v>199</v>
       </c>
       <c r="D19" t="s">
-        <v>1051</v>
+        <v>1036</v>
       </c>
       <c r="E19" t="s">
         <v>133</v>
@@ -5020,7 +4867,7 @@
         <v>200</v>
       </c>
       <c r="D20" t="s">
-        <v>1052</v>
+        <v>1037</v>
       </c>
       <c r="E20" t="s">
         <v>134</v>
@@ -5046,7 +4893,7 @@
         <v>201</v>
       </c>
       <c r="D21" t="s">
-        <v>1053</v>
+        <v>1038</v>
       </c>
       <c r="E21" t="s">
         <v>135</v>
@@ -5072,7 +4919,7 @@
         <v>202</v>
       </c>
       <c r="D22" t="s">
-        <v>1054</v>
+        <v>1039</v>
       </c>
       <c r="E22" t="s">
         <v>136</v>
@@ -5098,7 +4945,7 @@
         <v>203</v>
       </c>
       <c r="D23" t="s">
-        <v>1055</v>
+        <v>1040</v>
       </c>
       <c r="E23" t="s">
         <v>137</v>
@@ -5124,7 +4971,7 @@
         <v>204</v>
       </c>
       <c r="D24" t="s">
-        <v>1056</v>
+        <v>1041</v>
       </c>
       <c r="E24" t="s">
         <v>139</v>
@@ -5150,7 +4997,7 @@
         <v>205</v>
       </c>
       <c r="D25" t="s">
-        <v>1057</v>
+        <v>1042</v>
       </c>
       <c r="E25" t="s">
         <v>140</v>
@@ -5176,10 +5023,10 @@
         <v>206</v>
       </c>
       <c r="D26" t="s">
-        <v>1355</v>
+        <v>1265</v>
       </c>
       <c r="E26" t="s">
-        <v>1364</v>
+        <v>1274</v>
       </c>
       <c r="F26" t="s">
         <v>15</v>
@@ -5202,7 +5049,7 @@
         <v>207</v>
       </c>
       <c r="D27" t="s">
-        <v>1058</v>
+        <v>1043</v>
       </c>
       <c r="E27" t="s">
         <v>141</v>
@@ -5228,7 +5075,7 @@
         <v>208</v>
       </c>
       <c r="D28" t="s">
-        <v>1059</v>
+        <v>1044</v>
       </c>
       <c r="E28" t="s">
         <v>142</v>
@@ -5254,7 +5101,7 @@
         <v>209</v>
       </c>
       <c r="D29" t="s">
-        <v>1060</v>
+        <v>1045</v>
       </c>
       <c r="E29" t="s">
         <v>143</v>
@@ -5280,7 +5127,7 @@
         <v>210</v>
       </c>
       <c r="D30" t="s">
-        <v>1061</v>
+        <v>1046</v>
       </c>
       <c r="E30" t="s">
         <v>144</v>
@@ -5306,7 +5153,7 @@
         <v>211</v>
       </c>
       <c r="D31" t="s">
-        <v>1062</v>
+        <v>1047</v>
       </c>
       <c r="E31" t="s">
         <v>145</v>
@@ -5332,7 +5179,7 @@
         <v>147</v>
       </c>
       <c r="D32" t="s">
-        <v>1063</v>
+        <v>1048</v>
       </c>
       <c r="E32" t="s">
         <v>79</v>
@@ -5358,7 +5205,7 @@
         <v>148</v>
       </c>
       <c r="D33" t="s">
-        <v>1064</v>
+        <v>1049</v>
       </c>
       <c r="E33" t="s">
         <v>80</v>
@@ -5384,10 +5231,10 @@
         <v>149</v>
       </c>
       <c r="D34" t="s">
-        <v>1356</v>
+        <v>1266</v>
       </c>
       <c r="E34" t="s">
-        <v>1365</v>
+        <v>1275</v>
       </c>
       <c r="F34" t="s">
         <v>15</v>
@@ -5410,7 +5257,7 @@
         <v>150</v>
       </c>
       <c r="D35" t="s">
-        <v>1065</v>
+        <v>1050</v>
       </c>
       <c r="E35" t="s">
         <v>81</v>
@@ -5436,7 +5283,7 @@
         <v>151</v>
       </c>
       <c r="D36" t="s">
-        <v>1066</v>
+        <v>1051</v>
       </c>
       <c r="E36" t="s">
         <v>82</v>
@@ -5462,7 +5309,7 @@
         <v>152</v>
       </c>
       <c r="D37" t="s">
-        <v>1067</v>
+        <v>1052</v>
       </c>
       <c r="E37" t="s">
         <v>83</v>
@@ -5488,7 +5335,7 @@
         <v>153</v>
       </c>
       <c r="D38" t="s">
-        <v>1068</v>
+        <v>1053</v>
       </c>
       <c r="E38" t="s">
         <v>84</v>
@@ -5514,7 +5361,7 @@
         <v>154</v>
       </c>
       <c r="D39" t="s">
-        <v>1069</v>
+        <v>1054</v>
       </c>
       <c r="E39" t="s">
         <v>85</v>
@@ -5540,7 +5387,7 @@
         <v>155</v>
       </c>
       <c r="D40" t="s">
-        <v>1070</v>
+        <v>1055</v>
       </c>
       <c r="E40" t="s">
         <v>87</v>
@@ -5566,7 +5413,7 @@
         <v>156</v>
       </c>
       <c r="D41" t="s">
-        <v>1071</v>
+        <v>1056</v>
       </c>
       <c r="E41" t="s">
         <v>88</v>
@@ -5592,10 +5439,10 @@
         <v>157</v>
       </c>
       <c r="D42" t="s">
-        <v>1357</v>
+        <v>1267</v>
       </c>
       <c r="E42" t="s">
-        <v>1366</v>
+        <v>1276</v>
       </c>
       <c r="F42" t="s">
         <v>15</v>
@@ -5618,7 +5465,7 @@
         <v>158</v>
       </c>
       <c r="D43" t="s">
-        <v>1072</v>
+        <v>1057</v>
       </c>
       <c r="E43" t="s">
         <v>89</v>
@@ -5644,7 +5491,7 @@
         <v>159</v>
       </c>
       <c r="D44" t="s">
-        <v>1073</v>
+        <v>1058</v>
       </c>
       <c r="E44" t="s">
         <v>90</v>
@@ -5670,7 +5517,7 @@
         <v>160</v>
       </c>
       <c r="D45" t="s">
-        <v>1074</v>
+        <v>1059</v>
       </c>
       <c r="E45" t="s">
         <v>91</v>
@@ -5696,7 +5543,7 @@
         <v>161</v>
       </c>
       <c r="D46" t="s">
-        <v>1075</v>
+        <v>1060</v>
       </c>
       <c r="E46" t="s">
         <v>92</v>
@@ -5722,7 +5569,7 @@
         <v>162</v>
       </c>
       <c r="D47" t="s">
-        <v>1076</v>
+        <v>1061</v>
       </c>
       <c r="E47" t="s">
         <v>93</v>
@@ -5748,7 +5595,7 @@
         <v>163</v>
       </c>
       <c r="D48" t="s">
-        <v>1077</v>
+        <v>1062</v>
       </c>
       <c r="E48" t="s">
         <v>94</v>
@@ -5774,7 +5621,7 @@
         <v>164</v>
       </c>
       <c r="D49" t="s">
-        <v>1078</v>
+        <v>1063</v>
       </c>
       <c r="E49" t="s">
         <v>95</v>
@@ -5800,10 +5647,10 @@
         <v>165</v>
       </c>
       <c r="D50" t="s">
-        <v>1358</v>
+        <v>1268</v>
       </c>
       <c r="E50" t="s">
-        <v>1367</v>
+        <v>1277</v>
       </c>
       <c r="F50" t="s">
         <v>15</v>
@@ -5826,7 +5673,7 @@
         <v>166</v>
       </c>
       <c r="D51" t="s">
-        <v>1079</v>
+        <v>1064</v>
       </c>
       <c r="E51" t="s">
         <v>96</v>
@@ -5852,7 +5699,7 @@
         <v>167</v>
       </c>
       <c r="D52" t="s">
-        <v>1080</v>
+        <v>1065</v>
       </c>
       <c r="E52" t="s">
         <v>97</v>
@@ -5878,7 +5725,7 @@
         <v>168</v>
       </c>
       <c r="D53" t="s">
-        <v>1081</v>
+        <v>1066</v>
       </c>
       <c r="E53" t="s">
         <v>98</v>
@@ -5904,7 +5751,7 @@
         <v>169</v>
       </c>
       <c r="D54" t="s">
-        <v>1082</v>
+        <v>1067</v>
       </c>
       <c r="E54" t="s">
         <v>99</v>
@@ -5930,7 +5777,7 @@
         <v>170</v>
       </c>
       <c r="D55" t="s">
-        <v>1083</v>
+        <v>1068</v>
       </c>
       <c r="E55" t="s">
         <v>100</v>
@@ -5956,7 +5803,7 @@
         <v>171</v>
       </c>
       <c r="D56" t="s">
-        <v>1084</v>
+        <v>1069</v>
       </c>
       <c r="E56" t="s">
         <v>102</v>
@@ -5982,7 +5829,7 @@
         <v>172</v>
       </c>
       <c r="D57" t="s">
-        <v>1085</v>
+        <v>1070</v>
       </c>
       <c r="E57" t="s">
         <v>103</v>
@@ -6008,10 +5855,10 @@
         <v>173</v>
       </c>
       <c r="D58" t="s">
-        <v>1359</v>
+        <v>1269</v>
       </c>
       <c r="E58" t="s">
-        <v>1368</v>
+        <v>1278</v>
       </c>
       <c r="F58" t="s">
         <v>15</v>
@@ -6034,7 +5881,7 @@
         <v>174</v>
       </c>
       <c r="D59" t="s">
-        <v>1086</v>
+        <v>1071</v>
       </c>
       <c r="E59" t="s">
         <v>104</v>
@@ -6060,7 +5907,7 @@
         <v>175</v>
       </c>
       <c r="D60" t="s">
-        <v>1087</v>
+        <v>1072</v>
       </c>
       <c r="E60" t="s">
         <v>105</v>
@@ -6086,7 +5933,7 @@
         <v>176</v>
       </c>
       <c r="D61" t="s">
-        <v>1088</v>
+        <v>1073</v>
       </c>
       <c r="E61" t="s">
         <v>106</v>
@@ -6112,7 +5959,7 @@
         <v>177</v>
       </c>
       <c r="D62" t="s">
-        <v>1089</v>
+        <v>1074</v>
       </c>
       <c r="E62" t="s">
         <v>107</v>
@@ -6138,7 +5985,7 @@
         <v>178</v>
       </c>
       <c r="D63" t="s">
-        <v>1090</v>
+        <v>1075</v>
       </c>
       <c r="E63" t="s">
         <v>108</v>
@@ -6164,7 +6011,7 @@
         <v>179</v>
       </c>
       <c r="D64" t="s">
-        <v>1091</v>
+        <v>1076</v>
       </c>
       <c r="E64" t="s">
         <v>110</v>
@@ -6190,7 +6037,7 @@
         <v>181</v>
       </c>
       <c r="D65" t="s">
-        <v>1092</v>
+        <v>1077</v>
       </c>
       <c r="E65" t="s">
         <v>111</v>
@@ -6213,13 +6060,13 @@
         <v>180</v>
       </c>
       <c r="B66" t="s">
-        <v>1134</v>
+        <v>1117</v>
       </c>
       <c r="D66" t="s">
-        <v>1128</v>
+        <v>1111</v>
       </c>
       <c r="E66" t="s">
-        <v>1129</v>
+        <v>1112</v>
       </c>
       <c r="F66" t="s">
         <v>15</v>
@@ -6242,10 +6089,10 @@
         <v>308</v>
       </c>
       <c r="D67" t="s">
-        <v>1360</v>
+        <v>1270</v>
       </c>
       <c r="E67" t="s">
-        <v>1369</v>
+        <v>1279</v>
       </c>
       <c r="F67" t="s">
         <v>15</v>
@@ -6268,10 +6115,10 @@
         <v>316</v>
       </c>
       <c r="D68" t="s">
-        <v>1130</v>
+        <v>1113</v>
       </c>
       <c r="E68" t="s">
-        <v>1131</v>
+        <v>1114</v>
       </c>
       <c r="F68" t="s">
         <v>15</v>
@@ -6294,10 +6141,10 @@
         <v>306</v>
       </c>
       <c r="D69" t="s">
-        <v>1132</v>
+        <v>1115</v>
       </c>
       <c r="E69" t="s">
-        <v>1133</v>
+        <v>1116</v>
       </c>
       <c r="F69" t="s">
         <v>15</v>
@@ -6317,13 +6164,13 @@
         <v>180</v>
       </c>
       <c r="B70" t="s">
-        <v>1205</v>
+        <v>1155</v>
       </c>
       <c r="D70" t="s">
-        <v>1207</v>
+        <v>1157</v>
       </c>
       <c r="E70" t="s">
-        <v>1206</v>
+        <v>1156</v>
       </c>
       <c r="F70" t="s">
         <v>15</v>
@@ -6350,8 +6197,8 @@
   </sheetPr>
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6412,13 +6259,13 @@
         <v>184</v>
       </c>
       <c r="E3" t="s">
-        <v>1330</v>
+        <v>1240</v>
       </c>
       <c r="F3" t="s">
-        <v>1332</v>
+        <v>1242</v>
       </c>
       <c r="G3" t="s">
-        <v>1333</v>
+        <v>1243</v>
       </c>
       <c r="H3" t="s">
         <v>15</v>
@@ -6441,13 +6288,13 @@
         <v>184</v>
       </c>
       <c r="E4" t="s">
-        <v>1334</v>
+        <v>1244</v>
       </c>
       <c r="F4" t="s">
-        <v>1331</v>
+        <v>1241</v>
       </c>
       <c r="G4" t="s">
-        <v>1343</v>
+        <v>1253</v>
       </c>
       <c r="H4" t="s">
         <v>15</v>
@@ -6473,10 +6320,10 @@
         <v>494</v>
       </c>
       <c r="F5" t="s">
-        <v>1342</v>
+        <v>1252</v>
       </c>
       <c r="G5" t="s">
-        <v>1344</v>
+        <v>1254</v>
       </c>
       <c r="H5" t="s">
         <v>15</v>
@@ -6502,10 +6349,10 @@
         <v>497</v>
       </c>
       <c r="F6" t="s">
-        <v>1341</v>
+        <v>1251</v>
       </c>
       <c r="G6" t="s">
-        <v>1345</v>
+        <v>1255</v>
       </c>
       <c r="H6" t="s">
         <v>15</v>
@@ -6528,13 +6375,13 @@
         <v>184</v>
       </c>
       <c r="E7" t="s">
-        <v>1335</v>
+        <v>1245</v>
       </c>
       <c r="F7" t="s">
-        <v>1340</v>
+        <v>1250</v>
       </c>
       <c r="G7" t="s">
-        <v>1346</v>
+        <v>1256</v>
       </c>
       <c r="H7" t="s">
         <v>15</v>
@@ -6560,10 +6407,10 @@
         <v>445</v>
       </c>
       <c r="F8" t="s">
-        <v>1339</v>
+        <v>1249</v>
       </c>
       <c r="G8" t="s">
-        <v>1347</v>
+        <v>1257</v>
       </c>
       <c r="H8" t="s">
         <v>15</v>
@@ -6589,10 +6436,10 @@
         <v>564</v>
       </c>
       <c r="F9" t="s">
-        <v>1338</v>
+        <v>1248</v>
       </c>
       <c r="G9" t="s">
-        <v>1348</v>
+        <v>1258</v>
       </c>
       <c r="H9" t="s">
         <v>15</v>
@@ -6615,13 +6462,13 @@
         <v>184</v>
       </c>
       <c r="E10" t="s">
-        <v>1336</v>
+        <v>1246</v>
       </c>
       <c r="F10" t="s">
-        <v>1337</v>
+        <v>1247</v>
       </c>
       <c r="G10" t="s">
-        <v>1349</v>
+        <v>1259</v>
       </c>
       <c r="H10" t="s">
         <v>15</v>
@@ -14136,13 +13983,13 @@
         <v>861</v>
       </c>
       <c r="B3" t="s">
-        <v>1127</v>
+        <v>1110</v>
       </c>
       <c r="F3" t="s">
-        <v>1125</v>
+        <v>1108</v>
       </c>
       <c r="G3" t="s">
-        <v>1126</v>
+        <v>1109</v>
       </c>
       <c r="H3" t="s">
         <v>15</v>
@@ -14162,13 +14009,13 @@
         <v>861</v>
       </c>
       <c r="B4" t="s">
-        <v>1215</v>
+        <v>1165</v>
       </c>
       <c r="F4" t="s">
-        <v>1208</v>
+        <v>1158</v>
       </c>
       <c r="G4" t="s">
-        <v>1209</v>
+        <v>1159</v>
       </c>
       <c r="H4" t="s">
         <v>15</v>
@@ -14188,13 +14035,13 @@
         <v>861</v>
       </c>
       <c r="B5" t="s">
-        <v>1210</v>
+        <v>1160</v>
       </c>
       <c r="F5" t="s">
-        <v>1211</v>
+        <v>1161</v>
       </c>
       <c r="G5" t="s">
-        <v>1213</v>
+        <v>1163</v>
       </c>
       <c r="H5" t="s">
         <v>15</v>
@@ -14214,13 +14061,13 @@
         <v>861</v>
       </c>
       <c r="B6" t="s">
-        <v>1216</v>
+        <v>1166</v>
       </c>
       <c r="F6" t="s">
-        <v>1212</v>
+        <v>1162</v>
       </c>
       <c r="G6" t="s">
-        <v>1214</v>
+        <v>1164</v>
       </c>
       <c r="H6" t="s">
         <v>15</v>
@@ -14237,10 +14084,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>1181</v>
+        <v>1131</v>
       </c>
       <c r="F7" t="s">
-        <v>1093</v>
+        <v>1078</v>
       </c>
       <c r="G7" t="s">
         <v>39</v>
@@ -14260,13 +14107,13 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>1180</v>
+        <v>1130</v>
       </c>
       <c r="F8" t="s">
-        <v>1350</v>
+        <v>1260</v>
       </c>
       <c r="G8" t="s">
-        <v>1351</v>
+        <v>1261</v>
       </c>
       <c r="H8" t="s">
         <v>15</v>
@@ -14283,10 +14130,10 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>1041</v>
+        <v>1026</v>
       </c>
       <c r="F9" t="s">
-        <v>1094</v>
+        <v>1079</v>
       </c>
       <c r="G9" t="s">
         <v>40</v>
@@ -14309,7 +14156,7 @@
         <v>58</v>
       </c>
       <c r="F10" t="s">
-        <v>1095</v>
+        <v>1080</v>
       </c>
       <c r="G10" t="s">
         <v>41</v>
@@ -14332,7 +14179,7 @@
         <v>59</v>
       </c>
       <c r="F11" t="s">
-        <v>1096</v>
+        <v>1081</v>
       </c>
       <c r="G11" t="s">
         <v>42</v>
@@ -14355,7 +14202,7 @@
         <v>60</v>
       </c>
       <c r="F12" t="s">
-        <v>1097</v>
+        <v>1082</v>
       </c>
       <c r="G12" t="s">
         <v>43</v>
@@ -14378,7 +14225,7 @@
         <v>61</v>
       </c>
       <c r="F13" t="s">
-        <v>1098</v>
+        <v>1083</v>
       </c>
       <c r="G13" t="s">
         <v>44</v>
@@ -14466,13 +14313,13 @@
         <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>1002</v>
+        <v>987</v>
       </c>
       <c r="F3" t="s">
-        <v>1003</v>
+        <v>988</v>
       </c>
       <c r="G3" t="s">
-        <v>1004</v>
+        <v>989</v>
       </c>
       <c r="H3" t="s">
         <v>15</v>
@@ -14492,13 +14339,13 @@
         <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>1005</v>
+        <v>990</v>
       </c>
       <c r="F4" t="s">
-        <v>1006</v>
+        <v>991</v>
       </c>
       <c r="G4" t="s">
-        <v>1007</v>
+        <v>992</v>
       </c>
       <c r="H4" t="s">
         <v>15</v>
@@ -14518,13 +14365,13 @@
         <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>1008</v>
+        <v>993</v>
       </c>
       <c r="F5" t="s">
-        <v>1009</v>
+        <v>994</v>
       </c>
       <c r="G5" t="s">
-        <v>1010</v>
+        <v>995</v>
       </c>
       <c r="H5" t="s">
         <v>15</v>
@@ -14544,13 +14391,13 @@
         <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>1011</v>
+        <v>996</v>
       </c>
       <c r="F6" t="s">
-        <v>1012</v>
+        <v>997</v>
       </c>
       <c r="G6" t="s">
-        <v>1013</v>
+        <v>998</v>
       </c>
       <c r="H6" t="s">
         <v>15</v>
@@ -14570,13 +14417,13 @@
         <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>1014</v>
+        <v>999</v>
       </c>
       <c r="F7" t="s">
-        <v>1015</v>
+        <v>1000</v>
       </c>
       <c r="G7" t="s">
-        <v>1016</v>
+        <v>1001</v>
       </c>
       <c r="H7" t="s">
         <v>15</v>
@@ -14596,13 +14443,13 @@
         <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>1017</v>
+        <v>1002</v>
       </c>
       <c r="F8" t="s">
-        <v>1018</v>
+        <v>1003</v>
       </c>
       <c r="G8" t="s">
-        <v>1019</v>
+        <v>1004</v>
       </c>
       <c r="H8" t="s">
         <v>15</v>
@@ -14622,13 +14469,13 @@
         <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>1020</v>
+        <v>1005</v>
       </c>
       <c r="F9" t="s">
-        <v>1021</v>
+        <v>1006</v>
       </c>
       <c r="G9" t="s">
-        <v>1022</v>
+        <v>1007</v>
       </c>
       <c r="H9" t="s">
         <v>15</v>
@@ -14648,13 +14495,13 @@
         <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>1023</v>
+        <v>1008</v>
       </c>
       <c r="F10" t="s">
-        <v>1024</v>
+        <v>1009</v>
       </c>
       <c r="G10" t="s">
-        <v>1025</v>
+        <v>1010</v>
       </c>
       <c r="H10" t="s">
         <v>15</v>
@@ -14674,13 +14521,13 @@
         <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>1026</v>
+        <v>1011</v>
       </c>
       <c r="F11" t="s">
-        <v>1027</v>
+        <v>1012</v>
       </c>
       <c r="G11" t="s">
-        <v>1028</v>
+        <v>1013</v>
       </c>
       <c r="H11" t="s">
         <v>15</v>
@@ -14700,13 +14547,13 @@
         <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>1029</v>
+        <v>1014</v>
       </c>
       <c r="F12" t="s">
-        <v>1030</v>
+        <v>1015</v>
       </c>
       <c r="G12" t="s">
-        <v>1031</v>
+        <v>1016</v>
       </c>
       <c r="H12" t="s">
         <v>15</v>
@@ -14726,13 +14573,13 @@
         <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>1032</v>
+        <v>1017</v>
       </c>
       <c r="F13" t="s">
-        <v>1033</v>
+        <v>1018</v>
       </c>
       <c r="G13" t="s">
-        <v>1034</v>
+        <v>1019</v>
       </c>
       <c r="H13" t="s">
         <v>15</v>
@@ -14752,13 +14599,13 @@
         <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>1035</v>
+        <v>1020</v>
       </c>
       <c r="F14" t="s">
-        <v>1036</v>
+        <v>1021</v>
       </c>
       <c r="G14" t="s">
-        <v>1037</v>
+        <v>1022</v>
       </c>
       <c r="H14" t="s">
         <v>15</v>
@@ -14778,13 +14625,13 @@
         <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>1038</v>
+        <v>1023</v>
       </c>
       <c r="F15" t="s">
-        <v>1039</v>
+        <v>1024</v>
       </c>
       <c r="G15" t="s">
-        <v>1040</v>
+        <v>1025</v>
       </c>
       <c r="H15" t="s">
         <v>15</v>
@@ -14804,13 +14651,13 @@
         <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>1177</v>
+        <v>1127</v>
       </c>
       <c r="F16" t="s">
-        <v>1178</v>
+        <v>1128</v>
       </c>
       <c r="G16" t="s">
-        <v>1179</v>
+        <v>1129</v>
       </c>
       <c r="H16" t="s">
         <v>15</v>
@@ -14835,18 +14682,18 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:L39"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="67.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -14894,13 +14741,13 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>997</v>
+        <v>982</v>
       </c>
       <c r="F3" t="s">
-        <v>996</v>
+        <v>1280</v>
       </c>
       <c r="G3" t="s">
-        <v>995</v>
+        <v>1290</v>
       </c>
       <c r="H3" t="s">
         <v>15</v>
@@ -14917,13 +14764,13 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>994</v>
+        <v>981</v>
       </c>
       <c r="F4" t="s">
-        <v>993</v>
+        <v>1281</v>
       </c>
       <c r="G4" t="s">
-        <v>782</v>
+        <v>1291</v>
       </c>
       <c r="H4" t="s">
         <v>15</v>
@@ -14940,13 +14787,13 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>992</v>
+        <v>980</v>
       </c>
       <c r="F5" t="s">
-        <v>991</v>
+        <v>1282</v>
       </c>
       <c r="G5" t="s">
-        <v>990</v>
+        <v>1292</v>
       </c>
       <c r="H5" t="s">
         <v>15</v>
@@ -14963,13 +14810,13 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>989</v>
+        <v>979</v>
       </c>
       <c r="F6" t="s">
-        <v>988</v>
+        <v>1283</v>
       </c>
       <c r="G6" t="s">
-        <v>787</v>
+        <v>1293</v>
       </c>
       <c r="H6" t="s">
         <v>15</v>
@@ -14986,13 +14833,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>987</v>
+        <v>978</v>
       </c>
       <c r="F7" t="s">
-        <v>986</v>
+        <v>1284</v>
       </c>
       <c r="G7" t="s">
-        <v>823</v>
+        <v>1294</v>
       </c>
       <c r="H7" t="s">
         <v>15</v>
@@ -15009,13 +14856,13 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>985</v>
+        <v>977</v>
       </c>
       <c r="F8" t="s">
-        <v>984</v>
+        <v>1285</v>
       </c>
       <c r="G8" t="s">
-        <v>983</v>
+        <v>1295</v>
       </c>
       <c r="H8" t="s">
         <v>15</v>
@@ -15032,13 +14879,13 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>982</v>
+        <v>976</v>
       </c>
       <c r="F9" t="s">
-        <v>981</v>
+        <v>1286</v>
       </c>
       <c r="G9" t="s">
-        <v>980</v>
+        <v>1296</v>
       </c>
       <c r="H9" t="s">
         <v>15</v>
@@ -15055,13 +14902,13 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>979</v>
+        <v>975</v>
       </c>
       <c r="F10" t="s">
-        <v>978</v>
+        <v>1287</v>
       </c>
       <c r="G10" t="s">
-        <v>977</v>
+        <v>1297</v>
       </c>
       <c r="H10" t="s">
         <v>15</v>
@@ -15078,13 +14925,13 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="F11" t="s">
-        <v>975</v>
+        <v>1288</v>
       </c>
       <c r="G11" t="s">
-        <v>974</v>
+        <v>1298</v>
       </c>
       <c r="H11" t="s">
         <v>15</v>
@@ -15101,163 +14948,178 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>1306</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1106</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1289</v>
+      </c>
+      <c r="G12" t="s">
+        <v>1299</v>
+      </c>
+      <c r="H12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="str">
+        <f>$F$12</f>
+        <v>RSD_BLD-XXX_NRGSRV-WS</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1313</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1303</v>
+      </c>
+      <c r="G13" t="s">
+        <v>1300</v>
+      </c>
+      <c r="H13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="str">
+        <f t="shared" ref="A14:A15" si="0">$F$12</f>
+        <v>RSD_BLD-XXX_NRGSRV-WS</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1314</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1304</v>
+      </c>
+      <c r="G14" t="s">
+        <v>1301</v>
+      </c>
+      <c r="H14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>RSD_BLD-XXX_NRGSRV-WS</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1315</v>
+      </c>
+      <c r="F15" t="s">
+        <v>1305</v>
+      </c>
+      <c r="G15" t="s">
+        <v>1302</v>
+      </c>
+      <c r="H15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" t="s">
+        <v>15</v>
+      </c>
+      <c r="J15" t="s">
+        <v>15</v>
+      </c>
+      <c r="K15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" t="s">
         <v>1124</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F16" t="s">
         <v>1121</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G16" t="s">
+        <v>1118</v>
+      </c>
+      <c r="H16" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" t="s">
+        <v>16</v>
+      </c>
+      <c r="J16" t="s">
+        <v>15</v>
+      </c>
+      <c r="K16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F17" t="s">
+        <v>1122</v>
+      </c>
+      <c r="G17" t="s">
+        <v>1119</v>
+      </c>
+      <c r="H17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" t="s">
+        <v>16</v>
+      </c>
+      <c r="J17" t="s">
+        <v>15</v>
+      </c>
+      <c r="K17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1126</v>
+      </c>
+      <c r="F18" t="s">
         <v>1123</v>
       </c>
-      <c r="G12" t="s">
-        <v>1122</v>
-      </c>
-      <c r="H12" t="s">
-        <v>15</v>
-      </c>
-      <c r="I12" t="s">
-        <v>15</v>
-      </c>
-      <c r="J12" t="s">
-        <v>15</v>
-      </c>
-      <c r="K12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1141</v>
-      </c>
-      <c r="F13" t="s">
-        <v>1138</v>
-      </c>
-      <c r="G13" t="s">
-        <v>1135</v>
-      </c>
-      <c r="H13" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" t="s">
-        <v>16</v>
-      </c>
-      <c r="J13" t="s">
-        <v>15</v>
-      </c>
-      <c r="K13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" t="s">
-        <v>1142</v>
-      </c>
-      <c r="F14" t="s">
-        <v>1139</v>
-      </c>
-      <c r="G14" t="s">
-        <v>1136</v>
-      </c>
-      <c r="H14" t="s">
-        <v>15</v>
-      </c>
-      <c r="I14" t="s">
-        <v>16</v>
-      </c>
-      <c r="J14" t="s">
-        <v>15</v>
-      </c>
-      <c r="K14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1143</v>
-      </c>
-      <c r="F15" t="s">
-        <v>1140</v>
-      </c>
-      <c r="G15" t="s">
-        <v>1137</v>
-      </c>
-      <c r="H15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I15" t="s">
-        <v>16</v>
-      </c>
-      <c r="J15" t="s">
-        <v>15</v>
-      </c>
-      <c r="K15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>1144</v>
-      </c>
-      <c r="F16" t="s">
-        <v>1163</v>
-      </c>
-      <c r="G16" t="s">
-        <v>1154</v>
-      </c>
-      <c r="H16" t="s">
-        <v>15</v>
-      </c>
-      <c r="I16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J16" t="s">
-        <v>15</v>
-      </c>
-      <c r="K16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>1145</v>
-      </c>
-      <c r="F17" t="s">
-        <v>1164</v>
-      </c>
-      <c r="G17" t="s">
-        <v>1155</v>
-      </c>
-      <c r="H17" t="s">
-        <v>15</v>
-      </c>
-      <c r="I17" t="s">
-        <v>16</v>
-      </c>
-      <c r="J17" t="s">
-        <v>15</v>
-      </c>
-      <c r="K17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>1146</v>
-      </c>
-      <c r="F18" t="s">
-        <v>1165</v>
-      </c>
       <c r="G18" t="s">
-        <v>1156</v>
+        <v>1120</v>
       </c>
       <c r="H18" t="s">
         <v>15</v>
@@ -15273,14 +15135,15 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
       <c r="B19" t="s">
-        <v>1147</v>
+        <v>1307</v>
       </c>
       <c r="F19" t="s">
-        <v>1166</v>
+        <v>1308</v>
       </c>
       <c r="G19" t="s">
-        <v>1157</v>
+        <v>1309</v>
       </c>
       <c r="H19" t="s">
         <v>15</v>
@@ -15296,20 +15159,24 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="str">
+        <f>$F$19</f>
+        <v>RSD_BLD-XXX_RTFT</v>
+      </c>
       <c r="B20" t="s">
-        <v>1176</v>
+        <v>1313</v>
       </c>
       <c r="F20" t="s">
-        <v>1167</v>
+        <v>1316</v>
       </c>
       <c r="G20" t="s">
-        <v>1158</v>
+        <v>1310</v>
       </c>
       <c r="H20" t="s">
         <v>15</v>
       </c>
       <c r="I20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J20" t="s">
         <v>15</v>
@@ -15319,20 +15186,24 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="str">
+        <f t="shared" ref="A21:A22" si="1">$F$19</f>
+        <v>RSD_BLD-XXX_RTFT</v>
+      </c>
       <c r="B21" t="s">
-        <v>1148</v>
+        <v>1314</v>
       </c>
       <c r="F21" t="s">
-        <v>1168</v>
+        <v>1317</v>
       </c>
       <c r="G21" t="s">
-        <v>1159</v>
+        <v>1311</v>
       </c>
       <c r="H21" t="s">
         <v>15</v>
       </c>
       <c r="I21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J21" t="s">
         <v>15</v>
@@ -15342,450 +15213,29 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>RSD_BLD-XXX_RTFT</v>
+      </c>
       <c r="B22" t="s">
-        <v>1149</v>
+        <v>1315</v>
       </c>
       <c r="F22" t="s">
-        <v>1169</v>
+        <v>1318</v>
       </c>
       <c r="G22" t="s">
-        <v>1160</v>
+        <v>1312</v>
       </c>
       <c r="H22" t="s">
         <v>15</v>
       </c>
       <c r="I22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J22" t="s">
         <v>15</v>
       </c>
       <c r="K22" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>1150</v>
-      </c>
-      <c r="F23" t="s">
-        <v>1170</v>
-      </c>
-      <c r="G23" t="s">
-        <v>1161</v>
-      </c>
-      <c r="H23" t="s">
-        <v>15</v>
-      </c>
-      <c r="I23" t="s">
-        <v>16</v>
-      </c>
-      <c r="J23" t="s">
-        <v>15</v>
-      </c>
-      <c r="K23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>1151</v>
-      </c>
-      <c r="F24" t="s">
-        <v>1171</v>
-      </c>
-      <c r="G24" t="s">
-        <v>1162</v>
-      </c>
-      <c r="H24" t="s">
-        <v>15</v>
-      </c>
-      <c r="I24" t="s">
-        <v>16</v>
-      </c>
-      <c r="J24" t="s">
-        <v>15</v>
-      </c>
-      <c r="K24" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>1152</v>
-      </c>
-      <c r="F25" t="s">
-        <v>1172</v>
-      </c>
-      <c r="G25" t="s">
-        <v>1175</v>
-      </c>
-      <c r="H25" t="s">
-        <v>15</v>
-      </c>
-      <c r="I25" t="s">
-        <v>16</v>
-      </c>
-      <c r="J25" t="s">
-        <v>15</v>
-      </c>
-      <c r="K25" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>1153</v>
-      </c>
-      <c r="F26" t="s">
-        <v>1173</v>
-      </c>
-      <c r="G26" t="s">
-        <v>1174</v>
-      </c>
-      <c r="H26" t="s">
-        <v>15</v>
-      </c>
-      <c r="I26" t="s">
-        <v>16</v>
-      </c>
-      <c r="J26" t="s">
-        <v>15</v>
-      </c>
-      <c r="K26" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>1225</v>
-      </c>
-      <c r="F27" t="s">
-        <v>1217</v>
-      </c>
-      <c r="G27" t="s">
-        <v>1221</v>
-      </c>
-      <c r="H27" t="s">
-        <v>15</v>
-      </c>
-      <c r="I27" t="s">
-        <v>16</v>
-      </c>
-      <c r="J27" t="s">
-        <v>15</v>
-      </c>
-      <c r="K27" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>1226</v>
-      </c>
-      <c r="F28" t="s">
-        <v>1218</v>
-      </c>
-      <c r="G28" t="s">
-        <v>1223</v>
-      </c>
-      <c r="H28" t="s">
-        <v>15</v>
-      </c>
-      <c r="I28" t="s">
-        <v>16</v>
-      </c>
-      <c r="J28" t="s">
-        <v>15</v>
-      </c>
-      <c r="K28" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>1227</v>
-      </c>
-      <c r="F29" t="s">
-        <v>1219</v>
-      </c>
-      <c r="G29" t="s">
-        <v>1224</v>
-      </c>
-      <c r="H29" t="s">
-        <v>15</v>
-      </c>
-      <c r="I29" t="s">
-        <v>16</v>
-      </c>
-      <c r="J29" t="s">
-        <v>15</v>
-      </c>
-      <c r="K29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" t="str">
-        <f>"-"&amp;_xlfn.TEXTJOIN(",-",TRUE,F27:F29)</f>
-        <v>-RSD_TECH-HP,-RSD_TECH-AC,-RSD_TECH-DH</v>
-      </c>
-      <c r="B30" t="s">
-        <v>1228</v>
-      </c>
-      <c r="E30" t="s">
-        <v>1229</v>
-      </c>
-      <c r="F30" t="s">
-        <v>1220</v>
-      </c>
-      <c r="G30" t="s">
-        <v>1222</v>
-      </c>
-      <c r="H30" t="s">
-        <v>15</v>
-      </c>
-      <c r="I30" t="s">
-        <v>16</v>
-      </c>
-      <c r="J30" t="s">
-        <v>15</v>
-      </c>
-      <c r="K30" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>186</v>
-      </c>
-      <c r="E31" t="s">
-        <v>1239</v>
-      </c>
-      <c r="F31" t="s">
-        <v>1230</v>
-      </c>
-      <c r="G31" t="s">
-        <v>1248</v>
-      </c>
-      <c r="H31" t="s">
-        <v>15</v>
-      </c>
-      <c r="I31" t="s">
-        <v>16</v>
-      </c>
-      <c r="J31" t="s">
-        <v>15</v>
-      </c>
-      <c r="K31" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>186</v>
-      </c>
-      <c r="E32" t="s">
-        <v>1240</v>
-      </c>
-      <c r="F32" t="s">
-        <v>1231</v>
-      </c>
-      <c r="G32" t="s">
-        <v>1249</v>
-      </c>
-      <c r="H32" t="s">
-        <v>15</v>
-      </c>
-      <c r="I32" t="s">
-        <v>16</v>
-      </c>
-      <c r="J32" t="s">
-        <v>15</v>
-      </c>
-      <c r="K32" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>186</v>
-      </c>
-      <c r="E33" t="s">
-        <v>1241</v>
-      </c>
-      <c r="F33" t="s">
-        <v>1232</v>
-      </c>
-      <c r="G33" t="s">
-        <v>1250</v>
-      </c>
-      <c r="H33" t="s">
-        <v>15</v>
-      </c>
-      <c r="I33" t="s">
-        <v>16</v>
-      </c>
-      <c r="J33" t="s">
-        <v>15</v>
-      </c>
-      <c r="K33" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>186</v>
-      </c>
-      <c r="E34" t="s">
-        <v>1242</v>
-      </c>
-      <c r="F34" t="s">
-        <v>1233</v>
-      </c>
-      <c r="G34" t="s">
-        <v>1251</v>
-      </c>
-      <c r="H34" t="s">
-        <v>15</v>
-      </c>
-      <c r="I34" t="s">
-        <v>16</v>
-      </c>
-      <c r="J34" t="s">
-        <v>15</v>
-      </c>
-      <c r="K34" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>186</v>
-      </c>
-      <c r="E35" t="s">
-        <v>1243</v>
-      </c>
-      <c r="F35" t="s">
-        <v>1234</v>
-      </c>
-      <c r="G35" t="s">
-        <v>1252</v>
-      </c>
-      <c r="H35" t="s">
-        <v>15</v>
-      </c>
-      <c r="I35" t="s">
-        <v>16</v>
-      </c>
-      <c r="J35" t="s">
-        <v>15</v>
-      </c>
-      <c r="K35" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>186</v>
-      </c>
-      <c r="E36" t="s">
-        <v>1244</v>
-      </c>
-      <c r="F36" t="s">
-        <v>1235</v>
-      </c>
-      <c r="G36" t="s">
-        <v>1253</v>
-      </c>
-      <c r="H36" t="s">
-        <v>15</v>
-      </c>
-      <c r="I36" t="s">
-        <v>16</v>
-      </c>
-      <c r="J36" t="s">
-        <v>15</v>
-      </c>
-      <c r="K36" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>186</v>
-      </c>
-      <c r="E37" t="s">
-        <v>1246</v>
-      </c>
-      <c r="F37" t="s">
-        <v>1236</v>
-      </c>
-      <c r="G37" t="s">
-        <v>1254</v>
-      </c>
-      <c r="H37" t="s">
-        <v>15</v>
-      </c>
-      <c r="I37" t="s">
-        <v>16</v>
-      </c>
-      <c r="J37" t="s">
-        <v>15</v>
-      </c>
-      <c r="K37" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>186</v>
-      </c>
-      <c r="E38" t="s">
-        <v>1247</v>
-      </c>
-      <c r="F38" t="s">
-        <v>1237</v>
-      </c>
-      <c r="G38" t="s">
-        <v>1255</v>
-      </c>
-      <c r="H38" t="s">
-        <v>15</v>
-      </c>
-      <c r="I38" t="s">
-        <v>16</v>
-      </c>
-      <c r="J38" t="s">
-        <v>15</v>
-      </c>
-      <c r="K38" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>186</v>
-      </c>
-      <c r="E39" t="s">
-        <v>1245</v>
-      </c>
-      <c r="F39" t="s">
-        <v>1238</v>
-      </c>
-      <c r="G39" t="s">
-        <v>1256</v>
-      </c>
-      <c r="H39" t="s">
-        <v>15</v>
-      </c>
-      <c r="I39" t="s">
-        <v>16</v>
-      </c>
-      <c r="J39" t="s">
-        <v>15</v>
-      </c>
-      <c r="K39" t="s">
         <v>16</v>
       </c>
     </row>
@@ -15862,7 +15312,7 @@
         <v>46</v>
       </c>
       <c r="E3" t="s">
-        <v>998</v>
+        <v>983</v>
       </c>
       <c r="F3" t="s">
         <v>13</v>
@@ -15891,7 +15341,7 @@
         <v>47</v>
       </c>
       <c r="E4" t="s">
-        <v>998</v>
+        <v>983</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
@@ -15920,7 +15370,7 @@
         <v>48</v>
       </c>
       <c r="E5" t="s">
-        <v>998</v>
+        <v>983</v>
       </c>
       <c r="F5" t="s">
         <v>19</v>
@@ -15946,16 +15396,16 @@
         <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>999</v>
+        <v>984</v>
       </c>
       <c r="E6" t="s">
-        <v>998</v>
+        <v>983</v>
       </c>
       <c r="F6" t="s">
-        <v>1000</v>
+        <v>985</v>
       </c>
       <c r="G6" t="s">
-        <v>1001</v>
+        <v>986</v>
       </c>
       <c r="H6" t="s">
         <v>15</v>
@@ -15978,7 +15428,7 @@
         <v>49</v>
       </c>
       <c r="E7" t="s">
-        <v>998</v>
+        <v>983</v>
       </c>
       <c r="F7" t="s">
         <v>21</v>
@@ -16239,13 +15689,13 @@
         <v>47</v>
       </c>
       <c r="E16" t="s">
-        <v>1257</v>
+        <v>1167</v>
       </c>
       <c r="F16" t="s">
-        <v>1258</v>
+        <v>1168</v>
       </c>
       <c r="G16" t="s">
-        <v>1259</v>
+        <v>1169</v>
       </c>
       <c r="H16" t="s">
         <v>15</v>
@@ -16268,13 +15718,13 @@
         <v>47</v>
       </c>
       <c r="E17" t="s">
-        <v>1260</v>
+        <v>1170</v>
       </c>
       <c r="F17" t="s">
-        <v>1261</v>
+        <v>1171</v>
       </c>
       <c r="G17" t="s">
-        <v>1262</v>
+        <v>1172</v>
       </c>
       <c r="H17" t="s">
         <v>15</v>
@@ -16297,13 +15747,13 @@
         <v>47</v>
       </c>
       <c r="E18" t="s">
-        <v>1263</v>
+        <v>1173</v>
       </c>
       <c r="F18" t="s">
-        <v>1271</v>
+        <v>1181</v>
       </c>
       <c r="G18" t="s">
-        <v>1264</v>
+        <v>1174</v>
       </c>
       <c r="H18" t="s">
         <v>15</v>
@@ -16326,13 +15776,13 @@
         <v>47</v>
       </c>
       <c r="E19" t="s">
-        <v>1266</v>
+        <v>1176</v>
       </c>
       <c r="F19" t="s">
-        <v>1265</v>
+        <v>1175</v>
       </c>
       <c r="G19" t="s">
-        <v>1267</v>
+        <v>1177</v>
       </c>
       <c r="H19" t="s">
         <v>15</v>
@@ -16355,13 +15805,13 @@
         <v>47</v>
       </c>
       <c r="E20" t="s">
-        <v>1268</v>
+        <v>1178</v>
       </c>
       <c r="F20" t="s">
-        <v>1269</v>
+        <v>1179</v>
       </c>
       <c r="G20" t="s">
-        <v>1270</v>
+        <v>1180</v>
       </c>
       <c r="H20" t="s">
         <v>15</v>
@@ -16381,16 +15831,16 @@
         <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>1272</v>
+        <v>1182</v>
       </c>
       <c r="E21" t="s">
         <v>51</v>
       </c>
       <c r="F21" t="s">
-        <v>1119</v>
+        <v>1104</v>
       </c>
       <c r="G21" t="s">
-        <v>1120</v>
+        <v>1105</v>
       </c>
       <c r="H21" t="s">
         <v>15</v>
@@ -16410,16 +15860,16 @@
         <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>1273</v>
+        <v>1183</v>
       </c>
       <c r="E22" t="s">
         <v>51</v>
       </c>
       <c r="F22" t="s">
-        <v>1281</v>
+        <v>1191</v>
       </c>
       <c r="G22" t="s">
-        <v>1274</v>
+        <v>1184</v>
       </c>
       <c r="H22" t="s">
         <v>15</v>
@@ -16439,16 +15889,16 @@
         <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>1275</v>
+        <v>1185</v>
       </c>
       <c r="E23" t="s">
         <v>51</v>
       </c>
       <c r="F23" t="s">
-        <v>1282</v>
+        <v>1192</v>
       </c>
       <c r="G23" t="s">
-        <v>1276</v>
+        <v>1186</v>
       </c>
       <c r="H23" t="s">
         <v>15</v>
@@ -16468,16 +15918,16 @@
         <v>45</v>
       </c>
       <c r="B24" t="s">
-        <v>1277</v>
+        <v>1187</v>
       </c>
       <c r="E24" t="s">
         <v>51</v>
       </c>
       <c r="F24" t="s">
-        <v>1283</v>
+        <v>1193</v>
       </c>
       <c r="G24" t="s">
-        <v>1278</v>
+        <v>1188</v>
       </c>
       <c r="H24" t="s">
         <v>15</v>
@@ -16497,16 +15947,16 @@
         <v>45</v>
       </c>
       <c r="B25" t="s">
-        <v>1279</v>
+        <v>1189</v>
       </c>
       <c r="E25" t="s">
         <v>51</v>
       </c>
       <c r="F25" t="s">
-        <v>1284</v>
+        <v>1194</v>
       </c>
       <c r="G25" t="s">
-        <v>1280</v>
+        <v>1190</v>
       </c>
       <c r="H25" t="s">
         <v>15</v>
@@ -16526,16 +15976,16 @@
         <v>45</v>
       </c>
       <c r="B26" t="s">
-        <v>1285</v>
+        <v>1195</v>
       </c>
       <c r="E26" t="s">
-        <v>998</v>
+        <v>983</v>
       </c>
       <c r="F26" t="s">
-        <v>1286</v>
+        <v>1196</v>
       </c>
       <c r="G26" t="s">
-        <v>1287</v>
+        <v>1197</v>
       </c>
       <c r="H26" t="s">
         <v>15</v>
@@ -16555,16 +16005,16 @@
         <v>45</v>
       </c>
       <c r="B27" t="s">
-        <v>1288</v>
+        <v>1198</v>
       </c>
       <c r="E27" t="s">
-        <v>998</v>
+        <v>983</v>
       </c>
       <c r="F27" t="s">
-        <v>1309</v>
+        <v>1219</v>
       </c>
       <c r="G27" t="s">
-        <v>1291</v>
+        <v>1201</v>
       </c>
       <c r="H27" t="s">
         <v>15</v>
@@ -16584,16 +16034,16 @@
         <v>45</v>
       </c>
       <c r="B28" t="s">
-        <v>1289</v>
+        <v>1199</v>
       </c>
       <c r="E28" t="s">
-        <v>998</v>
+        <v>983</v>
       </c>
       <c r="F28" t="s">
-        <v>1310</v>
+        <v>1220</v>
       </c>
       <c r="G28" t="s">
-        <v>1292</v>
+        <v>1202</v>
       </c>
       <c r="H28" t="s">
         <v>15</v>
@@ -16613,16 +16063,16 @@
         <v>45</v>
       </c>
       <c r="B29" t="s">
-        <v>1290</v>
+        <v>1200</v>
       </c>
       <c r="E29" t="s">
-        <v>998</v>
+        <v>983</v>
       </c>
       <c r="F29" t="s">
-        <v>1311</v>
+        <v>1221</v>
       </c>
       <c r="G29" t="s">
-        <v>1293</v>
+        <v>1203</v>
       </c>
       <c r="H29" t="s">
         <v>15</v>
@@ -16642,16 +16092,16 @@
         <v>45</v>
       </c>
       <c r="B30" t="s">
-        <v>1294</v>
+        <v>1204</v>
       </c>
       <c r="E30" t="s">
-        <v>998</v>
+        <v>983</v>
       </c>
       <c r="F30" t="s">
-        <v>1298</v>
+        <v>1208</v>
       </c>
       <c r="G30" t="s">
-        <v>1299</v>
+        <v>1209</v>
       </c>
       <c r="H30" t="s">
         <v>15</v>
@@ -16671,16 +16121,16 @@
         <v>45</v>
       </c>
       <c r="B31" t="s">
-        <v>1295</v>
+        <v>1205</v>
       </c>
       <c r="E31" t="s">
-        <v>998</v>
+        <v>983</v>
       </c>
       <c r="F31" t="s">
-        <v>1312</v>
+        <v>1222</v>
       </c>
       <c r="G31" t="s">
-        <v>1300</v>
+        <v>1210</v>
       </c>
       <c r="H31" t="s">
         <v>15</v>
@@ -16700,16 +16150,16 @@
         <v>45</v>
       </c>
       <c r="B32" t="s">
-        <v>1296</v>
+        <v>1206</v>
       </c>
       <c r="E32" t="s">
-        <v>998</v>
+        <v>983</v>
       </c>
       <c r="F32" t="s">
-        <v>1313</v>
+        <v>1223</v>
       </c>
       <c r="G32" t="s">
-        <v>1301</v>
+        <v>1211</v>
       </c>
       <c r="H32" t="s">
         <v>15</v>
@@ -16729,16 +16179,16 @@
         <v>45</v>
       </c>
       <c r="B33" t="s">
-        <v>1297</v>
+        <v>1207</v>
       </c>
       <c r="E33" t="s">
-        <v>998</v>
+        <v>983</v>
       </c>
       <c r="F33" t="s">
-        <v>1314</v>
+        <v>1224</v>
       </c>
       <c r="G33" t="s">
-        <v>1302</v>
+        <v>1212</v>
       </c>
       <c r="H33" t="s">
         <v>15</v>
@@ -16758,16 +16208,16 @@
         <v>45</v>
       </c>
       <c r="B34" t="s">
-        <v>1303</v>
+        <v>1213</v>
       </c>
       <c r="E34" t="s">
-        <v>998</v>
+        <v>983</v>
       </c>
       <c r="F34" t="s">
-        <v>1308</v>
+        <v>1218</v>
       </c>
       <c r="G34" t="s">
-        <v>1319</v>
+        <v>1229</v>
       </c>
       <c r="H34" t="s">
         <v>15</v>
@@ -16787,16 +16237,16 @@
         <v>45</v>
       </c>
       <c r="B35" t="s">
-        <v>1304</v>
+        <v>1214</v>
       </c>
       <c r="E35" t="s">
-        <v>998</v>
+        <v>983</v>
       </c>
       <c r="F35" t="s">
-        <v>1315</v>
+        <v>1225</v>
       </c>
       <c r="G35" t="s">
-        <v>1320</v>
+        <v>1230</v>
       </c>
       <c r="H35" t="s">
         <v>15</v>
@@ -16816,16 +16266,16 @@
         <v>45</v>
       </c>
       <c r="B36" t="s">
-        <v>1305</v>
+        <v>1215</v>
       </c>
       <c r="E36" t="s">
-        <v>998</v>
+        <v>983</v>
       </c>
       <c r="F36" t="s">
-        <v>1316</v>
+        <v>1226</v>
       </c>
       <c r="G36" t="s">
-        <v>1321</v>
+        <v>1231</v>
       </c>
       <c r="H36" t="s">
         <v>15</v>
@@ -16845,16 +16295,16 @@
         <v>45</v>
       </c>
       <c r="B37" t="s">
-        <v>1306</v>
+        <v>1216</v>
       </c>
       <c r="E37" t="s">
-        <v>998</v>
+        <v>983</v>
       </c>
       <c r="F37" t="s">
-        <v>1317</v>
+        <v>1227</v>
       </c>
       <c r="G37" t="s">
-        <v>1322</v>
+        <v>1232</v>
       </c>
       <c r="H37" t="s">
         <v>15</v>
@@ -16874,16 +16324,16 @@
         <v>45</v>
       </c>
       <c r="B38" t="s">
-        <v>1307</v>
+        <v>1217</v>
       </c>
       <c r="E38" t="s">
-        <v>998</v>
+        <v>983</v>
       </c>
       <c r="F38" t="s">
-        <v>1318</v>
+        <v>1228</v>
       </c>
       <c r="G38" t="s">
-        <v>1323</v>
+        <v>1233</v>
       </c>
       <c r="H38" t="s">
         <v>15</v>
@@ -16965,13 +16415,13 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>1193</v>
+        <v>1143</v>
       </c>
       <c r="F3" t="s">
-        <v>1099</v>
+        <v>1084</v>
       </c>
       <c r="G3" t="s">
-        <v>1186</v>
+        <v>1136</v>
       </c>
       <c r="H3" t="s">
         <v>15</v>
@@ -16982,13 +16432,13 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>1194</v>
+        <v>1144</v>
       </c>
       <c r="F4" t="s">
-        <v>1187</v>
+        <v>1137</v>
       </c>
       <c r="G4" t="s">
-        <v>1188</v>
+        <v>1138</v>
       </c>
       <c r="H4" t="s">
         <v>15</v>
@@ -16999,13 +16449,13 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>1183</v>
+        <v>1133</v>
       </c>
       <c r="F5" t="s">
-        <v>1185</v>
+        <v>1135</v>
       </c>
       <c r="G5" t="s">
-        <v>1184</v>
+        <v>1134</v>
       </c>
       <c r="H5" t="s">
         <v>15</v>
@@ -17016,13 +16466,13 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>1195</v>
+        <v>1145</v>
       </c>
       <c r="F6" t="s">
-        <v>1100</v>
+        <v>1085</v>
       </c>
       <c r="G6" t="s">
-        <v>1190</v>
+        <v>1140</v>
       </c>
       <c r="H6" t="s">
         <v>15</v>
@@ -17039,13 +16489,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>1196</v>
+        <v>1146</v>
       </c>
       <c r="F7" t="s">
-        <v>1191</v>
+        <v>1141</v>
       </c>
       <c r="G7" t="s">
-        <v>1192</v>
+        <v>1142</v>
       </c>
       <c r="H7" t="s">
         <v>15</v>
@@ -17056,13 +16506,13 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>1198</v>
+        <v>1148</v>
       </c>
       <c r="F8" t="s">
-        <v>1189</v>
+        <v>1139</v>
       </c>
       <c r="G8" t="s">
-        <v>1199</v>
+        <v>1149</v>
       </c>
       <c r="H8" t="s">
         <v>15</v>
@@ -17073,13 +16523,13 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>1197</v>
+        <v>1147</v>
       </c>
       <c r="F9" t="s">
-        <v>1201</v>
+        <v>1151</v>
       </c>
       <c r="G9" t="s">
-        <v>1200</v>
+        <v>1150</v>
       </c>
       <c r="H9" t="s">
         <v>15</v>
@@ -17093,10 +16543,10 @@
         <v>62</v>
       </c>
       <c r="F10" t="s">
-        <v>1101</v>
+        <v>1086</v>
       </c>
       <c r="G10" t="s">
-        <v>1118</v>
+        <v>1103</v>
       </c>
       <c r="H10" t="s">
         <v>15</v>
@@ -17110,10 +16560,10 @@
         <v>63</v>
       </c>
       <c r="F11" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G11" t="s">
         <v>1102</v>
-      </c>
-      <c r="G11" t="s">
-        <v>1117</v>
       </c>
       <c r="H11" t="s">
         <v>15</v>
@@ -17127,10 +16577,10 @@
         <v>64</v>
       </c>
       <c r="F12" t="s">
-        <v>1103</v>
+        <v>1088</v>
       </c>
       <c r="G12" t="s">
-        <v>1116</v>
+        <v>1101</v>
       </c>
       <c r="H12" t="s">
         <v>15</v>
@@ -17147,13 +16597,13 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>1182</v>
+        <v>1132</v>
       </c>
       <c r="F13" t="s">
-        <v>1104</v>
+        <v>1089</v>
       </c>
       <c r="G13" t="s">
-        <v>1115</v>
+        <v>1100</v>
       </c>
       <c r="H13" t="s">
         <v>15</v>
@@ -17167,10 +16617,10 @@
         <v>65</v>
       </c>
       <c r="F14" t="s">
-        <v>1105</v>
+        <v>1090</v>
       </c>
       <c r="G14" t="s">
-        <v>1114</v>
+        <v>1099</v>
       </c>
       <c r="H14" t="s">
         <v>15</v>
@@ -17184,10 +16634,10 @@
         <v>66</v>
       </c>
       <c r="F15" t="s">
-        <v>1106</v>
+        <v>1091</v>
       </c>
       <c r="G15" t="s">
-        <v>1113</v>
+        <v>1098</v>
       </c>
       <c r="H15" t="s">
         <v>15</v>
@@ -17201,10 +16651,10 @@
         <v>67</v>
       </c>
       <c r="F16" t="s">
-        <v>1107</v>
+        <v>1092</v>
       </c>
       <c r="G16" t="s">
-        <v>1110</v>
+        <v>1095</v>
       </c>
       <c r="H16" t="s">
         <v>15</v>
@@ -17218,10 +16668,10 @@
         <v>68</v>
       </c>
       <c r="F17" t="s">
-        <v>1108</v>
+        <v>1093</v>
       </c>
       <c r="G17" t="s">
-        <v>1111</v>
+        <v>1096</v>
       </c>
       <c r="H17" t="s">
         <v>15</v>
@@ -17235,10 +16685,10 @@
         <v>69</v>
       </c>
       <c r="F18" t="s">
-        <v>1109</v>
+        <v>1094</v>
       </c>
       <c r="G18" t="s">
-        <v>1112</v>
+        <v>1097</v>
       </c>
       <c r="H18" t="s">
         <v>15</v>
@@ -17249,13 +16699,13 @@
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>1202</v>
+        <v>1152</v>
       </c>
       <c r="F19" t="s">
-        <v>1203</v>
+        <v>1153</v>
       </c>
       <c r="G19" t="s">
-        <v>1204</v>
+        <v>1154</v>
       </c>
       <c r="H19" t="s">
         <v>15</v>
@@ -17334,13 +16784,13 @@
         <v>788</v>
       </c>
       <c r="B3" t="s">
-        <v>1327</v>
+        <v>1237</v>
       </c>
       <c r="F3" t="s">
-        <v>1328</v>
+        <v>1238</v>
       </c>
       <c r="G3" t="s">
-        <v>1329</v>
+        <v>1239</v>
       </c>
       <c r="H3" t="s">
         <v>15</v>
@@ -17423,13 +16873,13 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>1324</v>
+        <v>1234</v>
       </c>
       <c r="F3" t="s">
-        <v>1325</v>
+        <v>1235</v>
       </c>
       <c r="G3" t="s">
-        <v>1326</v>
+        <v>1236</v>
       </c>
       <c r="H3" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Add SEAI aggregate fuel categories
</commit_message>
<xml_diff>
--- a/SetRules.xlsx
+++ b/SetRules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D667FB43-5CF1-41D1-8B1E-D348AE4B4C94}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D870E49-1AC0-4CD2-B643-EA0B86F40E55}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="4" xr2:uid="{69765015-6AAF-4B94-8956-691CCC759B47}"/>
+    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" xr2:uid="{69765015-6AAF-4B94-8956-691CCC759B47}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets-Comm" sheetId="5" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3390" uniqueCount="1319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3454" uniqueCount="1343">
   <si>
     <t>~TFM_Psets</t>
   </si>
@@ -4003,6 +4003,78 @@
   </si>
   <si>
     <t>RSD_BLD-DET_RTFT</t>
+  </si>
+  <si>
+    <t>SEAI_COAL</t>
+  </si>
+  <si>
+    <t>Coal - SEAI grouping</t>
+  </si>
+  <si>
+    <t>SEAI_PEAT</t>
+  </si>
+  <si>
+    <t>SEAI_OIL</t>
+  </si>
+  <si>
+    <t>Oil - SEAI grouping</t>
+  </si>
+  <si>
+    <t>Peat - SEAI grouping</t>
+  </si>
+  <si>
+    <t>SEAI_NATGAS</t>
+  </si>
+  <si>
+    <t>Natural gas - SEAI grouping</t>
+  </si>
+  <si>
+    <t>SEAI_RENEWABLES</t>
+  </si>
+  <si>
+    <t>Renewables - SEAI grouping</t>
+  </si>
+  <si>
+    <t>SEAI_ELECTRICITY</t>
+  </si>
+  <si>
+    <t>SEAI_HEAT</t>
+  </si>
+  <si>
+    <t>Electricity - SEAI grouping</t>
+  </si>
+  <si>
+    <t>Heat - SEAI grouping</t>
+  </si>
+  <si>
+    <t>*COA*</t>
+  </si>
+  <si>
+    <t>*PEA*</t>
+  </si>
+  <si>
+    <t>*OIL*,*LPG,*HFO,*GSL,*DST,*KER,INDCOK</t>
+  </si>
+  <si>
+    <t>*ELC*</t>
+  </si>
+  <si>
+    <t>*HET*</t>
+  </si>
+  <si>
+    <t>*REN*,BIO*,AMBHET</t>
+  </si>
+  <si>
+    <t>SUPH2*</t>
+  </si>
+  <si>
+    <t>SEAI_HYDROGEN</t>
+  </si>
+  <si>
+    <t>Hydrogen - SEAI grouping</t>
+  </si>
+  <si>
+    <t>*NAT*,*GAS,*LNG</t>
   </si>
 </sst>
 </file>
@@ -4368,15 +4440,15 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:J70"/>
+  <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E70"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6182,6 +6254,214 @@
         <v>15</v>
       </c>
       <c r="I70" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>180</v>
+      </c>
+      <c r="B71" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D71" t="s">
+        <v>1319</v>
+      </c>
+      <c r="E71" t="s">
+        <v>1320</v>
+      </c>
+      <c r="F71" t="s">
+        <v>15</v>
+      </c>
+      <c r="G71" t="s">
+        <v>16</v>
+      </c>
+      <c r="H71" t="s">
+        <v>15</v>
+      </c>
+      <c r="I71" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>180</v>
+      </c>
+      <c r="B72" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D72" t="s">
+        <v>1321</v>
+      </c>
+      <c r="E72" t="s">
+        <v>1324</v>
+      </c>
+      <c r="F72" t="s">
+        <v>15</v>
+      </c>
+      <c r="G72" t="s">
+        <v>16</v>
+      </c>
+      <c r="H72" t="s">
+        <v>15</v>
+      </c>
+      <c r="I72" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>180</v>
+      </c>
+      <c r="B73" t="s">
+        <v>1335</v>
+      </c>
+      <c r="D73" t="s">
+        <v>1322</v>
+      </c>
+      <c r="E73" t="s">
+        <v>1323</v>
+      </c>
+      <c r="F73" t="s">
+        <v>15</v>
+      </c>
+      <c r="G73" t="s">
+        <v>16</v>
+      </c>
+      <c r="H73" t="s">
+        <v>15</v>
+      </c>
+      <c r="I73" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>180</v>
+      </c>
+      <c r="B74" t="s">
+        <v>1342</v>
+      </c>
+      <c r="D74" t="s">
+        <v>1325</v>
+      </c>
+      <c r="E74" t="s">
+        <v>1326</v>
+      </c>
+      <c r="F74" t="s">
+        <v>15</v>
+      </c>
+      <c r="G74" t="s">
+        <v>16</v>
+      </c>
+      <c r="H74" t="s">
+        <v>15</v>
+      </c>
+      <c r="I74" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>180</v>
+      </c>
+      <c r="B75" t="s">
+        <v>1338</v>
+      </c>
+      <c r="D75" t="s">
+        <v>1327</v>
+      </c>
+      <c r="E75" t="s">
+        <v>1328</v>
+      </c>
+      <c r="F75" t="s">
+        <v>15</v>
+      </c>
+      <c r="G75" t="s">
+        <v>16</v>
+      </c>
+      <c r="H75" t="s">
+        <v>15</v>
+      </c>
+      <c r="I75" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>180</v>
+      </c>
+      <c r="B76" t="s">
+        <v>1336</v>
+      </c>
+      <c r="D76" t="s">
+        <v>1329</v>
+      </c>
+      <c r="E76" t="s">
+        <v>1331</v>
+      </c>
+      <c r="F76" t="s">
+        <v>15</v>
+      </c>
+      <c r="G76" t="s">
+        <v>16</v>
+      </c>
+      <c r="H76" t="s">
+        <v>15</v>
+      </c>
+      <c r="I76" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>180</v>
+      </c>
+      <c r="B77" t="s">
+        <v>1337</v>
+      </c>
+      <c r="D77" t="s">
+        <v>1330</v>
+      </c>
+      <c r="E77" t="s">
+        <v>1332</v>
+      </c>
+      <c r="F77" t="s">
+        <v>15</v>
+      </c>
+      <c r="G77" t="s">
+        <v>16</v>
+      </c>
+      <c r="H77" t="s">
+        <v>15</v>
+      </c>
+      <c r="I77" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>180</v>
+      </c>
+      <c r="B78" t="s">
+        <v>1339</v>
+      </c>
+      <c r="D78" t="s">
+        <v>1340</v>
+      </c>
+      <c r="E78" t="s">
+        <v>1341</v>
+      </c>
+      <c r="F78" t="s">
+        <v>15</v>
+      </c>
+      <c r="G78" t="s">
+        <v>16</v>
+      </c>
+      <c r="H78" t="s">
+        <v>15</v>
+      </c>
+      <c r="I78" t="s">
         <v>16</v>
       </c>
     </row>
@@ -14684,7 +14964,7 @@
   </sheetPr>
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Sets: split bioenergy and other renewables
</commit_message>
<xml_diff>
--- a/SetRules.xlsx
+++ b/SetRules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D870E49-1AC0-4CD2-B643-EA0B86F40E55}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B1E673-DCE1-4A55-A52D-E87A7330B70D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" xr2:uid="{69765015-6AAF-4B94-8956-691CCC759B47}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3454" uniqueCount="1343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3462" uniqueCount="1346">
   <si>
     <t>~TFM_Psets</t>
   </si>
@@ -4029,12 +4029,6 @@
     <t>Natural gas - SEAI grouping</t>
   </si>
   <si>
-    <t>SEAI_RENEWABLES</t>
-  </si>
-  <si>
-    <t>Renewables - SEAI grouping</t>
-  </si>
-  <si>
     <t>SEAI_ELECTRICITY</t>
   </si>
   <si>
@@ -4062,9 +4056,6 @@
     <t>*HET*</t>
   </si>
   <si>
-    <t>*REN*,BIO*,AMBHET</t>
-  </si>
-  <si>
     <t>SUPH2*</t>
   </si>
   <si>
@@ -4075,6 +4066,24 @@
   </si>
   <si>
     <t>*NAT*,*GAS,*LNG</t>
+  </si>
+  <si>
+    <t>*REN*,AMBHET</t>
+  </si>
+  <si>
+    <t>BIO*</t>
+  </si>
+  <si>
+    <t>Other renewables - SEAI grouping</t>
+  </si>
+  <si>
+    <t>SEAI_OTHER_RENEWABLES</t>
+  </si>
+  <si>
+    <t>SEAI_BIOENERGY</t>
+  </si>
+  <si>
+    <t>Bioenergy - SEAI grouping</t>
   </si>
 </sst>
 </file>
@@ -4440,10 +4449,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:J78"/>
+  <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D83" sqref="D83"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6262,7 +6271,7 @@
         <v>180</v>
       </c>
       <c r="B71" t="s">
-        <v>1333</v>
+        <v>1331</v>
       </c>
       <c r="D71" t="s">
         <v>1319</v>
@@ -6288,7 +6297,7 @@
         <v>180</v>
       </c>
       <c r="B72" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="D72" t="s">
         <v>1321</v>
@@ -6314,7 +6323,7 @@
         <v>180</v>
       </c>
       <c r="B73" t="s">
-        <v>1335</v>
+        <v>1333</v>
       </c>
       <c r="D73" t="s">
         <v>1322</v>
@@ -6340,7 +6349,7 @@
         <v>180</v>
       </c>
       <c r="B74" t="s">
-        <v>1342</v>
+        <v>1339</v>
       </c>
       <c r="D74" t="s">
         <v>1325</v>
@@ -6366,13 +6375,13 @@
         <v>180</v>
       </c>
       <c r="B75" t="s">
-        <v>1338</v>
+        <v>1340</v>
       </c>
       <c r="D75" t="s">
-        <v>1327</v>
+        <v>1343</v>
       </c>
       <c r="E75" t="s">
-        <v>1328</v>
+        <v>1342</v>
       </c>
       <c r="F75" t="s">
         <v>15</v>
@@ -6392,13 +6401,13 @@
         <v>180</v>
       </c>
       <c r="B76" t="s">
-        <v>1336</v>
+        <v>1341</v>
       </c>
       <c r="D76" t="s">
-        <v>1329</v>
+        <v>1344</v>
       </c>
       <c r="E76" t="s">
-        <v>1331</v>
+        <v>1345</v>
       </c>
       <c r="F76" t="s">
         <v>15</v>
@@ -6418,13 +6427,13 @@
         <v>180</v>
       </c>
       <c r="B77" t="s">
-        <v>1337</v>
+        <v>1334</v>
       </c>
       <c r="D77" t="s">
-        <v>1330</v>
+        <v>1327</v>
       </c>
       <c r="E77" t="s">
-        <v>1332</v>
+        <v>1329</v>
       </c>
       <c r="F77" t="s">
         <v>15</v>
@@ -6444,13 +6453,13 @@
         <v>180</v>
       </c>
       <c r="B78" t="s">
-        <v>1339</v>
+        <v>1335</v>
       </c>
       <c r="D78" t="s">
-        <v>1340</v>
+        <v>1328</v>
       </c>
       <c r="E78" t="s">
-        <v>1341</v>
+        <v>1330</v>
       </c>
       <c r="F78" t="s">
         <v>15</v>
@@ -6462,6 +6471,32 @@
         <v>15</v>
       </c>
       <c r="I78" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>180</v>
+      </c>
+      <c r="B79" t="s">
+        <v>1336</v>
+      </c>
+      <c r="D79" t="s">
+        <v>1337</v>
+      </c>
+      <c r="E79" t="s">
+        <v>1338</v>
+      </c>
+      <c r="F79" t="s">
+        <v>15</v>
+      </c>
+      <c r="G79" t="s">
+        <v>16</v>
+      </c>
+      <c r="H79" t="s">
+        <v>15</v>
+      </c>
+      <c r="I79" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Keep only primary ambient heat commodity
</commit_message>
<xml_diff>
--- a/SetRules.xlsx
+++ b/SetRules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B1E673-DCE1-4A55-A52D-E87A7330B70D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5D40EB-590E-4D46-8F6E-219345022048}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" xr2:uid="{69765015-6AAF-4B94-8956-691CCC759B47}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{69765015-6AAF-4B94-8956-691CCC759B47}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets-Comm" sheetId="5" r:id="rId1"/>
@@ -4068,9 +4068,6 @@
     <t>*NAT*,*GAS,*LNG</t>
   </si>
   <si>
-    <t>*REN*,AMBHET</t>
-  </si>
-  <si>
     <t>BIO*</t>
   </si>
   <si>
@@ -4084,6 +4081,9 @@
   </si>
   <si>
     <t>Bioenergy - SEAI grouping</t>
+  </si>
+  <si>
+    <t>*REN*</t>
   </si>
 </sst>
 </file>
@@ -4451,8 +4451,8 @@
   </sheetPr>
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E77" sqref="E77"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6375,13 +6375,13 @@
         <v>180</v>
       </c>
       <c r="B75" t="s">
-        <v>1340</v>
+        <v>1345</v>
       </c>
       <c r="D75" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="E75" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="F75" t="s">
         <v>15</v>
@@ -6401,13 +6401,13 @@
         <v>180</v>
       </c>
       <c r="B76" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="D76" t="s">
+        <v>1343</v>
+      </c>
+      <c r="E76" t="s">
         <v>1344</v>
-      </c>
-      <c r="E76" t="s">
-        <v>1345</v>
       </c>
       <c r="F76" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
SRV DC add a set with HPs for upgrading excess heat
</commit_message>
<xml_diff>
--- a/SetRules.xlsx
+++ b/SetRules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005907B0-C45D-4C33-9459-57B09F9566A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C31C6096-5609-479A-BFFF-5729BFC0D5B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" xr2:uid="{69765015-6AAF-4B94-8956-691CCC759B47}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{69765015-6AAF-4B94-8956-691CCC759B47}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets-Comm" sheetId="5" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1613" uniqueCount="602">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1621" uniqueCount="605">
   <si>
     <t>~TFM_Psets</t>
   </si>
@@ -1848,6 +1848,15 @@
   </si>
   <si>
     <t>Commercial Services - All Except Data Centers</t>
+  </si>
+  <si>
+    <t>SRV_CS-DC-EH-HP</t>
+  </si>
+  <si>
+    <t>SRVHET-LT</t>
+  </si>
+  <si>
+    <t>Commercial Services - DC Excess Heat - Heat Pumps</t>
   </si>
 </sst>
 </file>
@@ -2205,8 +2214,8 @@
   </sheetPr>
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H62" sqref="H62"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7245,14 +7254,15 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="57.85546875" bestFit="1" customWidth="1"/>
@@ -7678,6 +7688,32 @@
         <v>16</v>
       </c>
     </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>546</v>
+      </c>
+      <c r="D17" t="s">
+        <v>603</v>
+      </c>
+      <c r="F17" t="s">
+        <v>602</v>
+      </c>
+      <c r="G17" t="s">
+        <v>604</v>
+      </c>
+      <c r="H17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" t="s">
+        <v>16</v>
+      </c>
+      <c r="J17" t="s">
+        <v>15</v>
+      </c>
+      <c r="K17" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add HPs sets for services
</commit_message>
<xml_diff>
--- a/SetRules.xlsx
+++ b/SetRules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C31C6096-5609-479A-BFFF-5729BFC0D5B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E932C3CC-2658-44FD-A540-416023D3C1DA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{69765015-6AAF-4B94-8956-691CCC759B47}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1621" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1637" uniqueCount="612">
   <si>
     <t>~TFM_Psets</t>
   </si>
@@ -1857,6 +1857,27 @@
   </si>
   <si>
     <t>Commercial Services - DC Excess Heat - Heat Pumps</t>
+  </si>
+  <si>
+    <t>SRVAHT</t>
+  </si>
+  <si>
+    <t>S*PU*</t>
+  </si>
+  <si>
+    <t>SRV_PU-HP</t>
+  </si>
+  <si>
+    <t>S*CS*</t>
+  </si>
+  <si>
+    <t>SRV_CS-HP</t>
+  </si>
+  <si>
+    <t>Public Services - Heat Pumps</t>
+  </si>
+  <si>
+    <t>Commercial Services - Heat Pumps</t>
   </si>
 </sst>
 </file>
@@ -7254,10 +7275,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7714,6 +7735,58 @@
         <v>16</v>
       </c>
     </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>606</v>
+      </c>
+      <c r="D18" t="s">
+        <v>605</v>
+      </c>
+      <c r="F18" t="s">
+        <v>607</v>
+      </c>
+      <c r="G18" t="s">
+        <v>610</v>
+      </c>
+      <c r="H18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" t="s">
+        <v>16</v>
+      </c>
+      <c r="J18" t="s">
+        <v>15</v>
+      </c>
+      <c r="K18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>608</v>
+      </c>
+      <c r="D19" t="s">
+        <v>605</v>
+      </c>
+      <c r="F19" t="s">
+        <v>609</v>
+      </c>
+      <c r="G19" t="s">
+        <v>611</v>
+      </c>
+      <c r="H19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" t="s">
+        <v>16</v>
+      </c>
+      <c r="J19" t="s">
+        <v>15</v>
+      </c>
+      <c r="K19" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Include process sets splitting processes by sector
</commit_message>
<xml_diff>
--- a/SetRules.xlsx
+++ b/SetRules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E932C3CC-2658-44FD-A540-416023D3C1DA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58EFB912-37D6-4F5E-9355-AC2393FA7669}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{69765015-6AAF-4B94-8956-691CCC759B47}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{69765015-6AAF-4B94-8956-691CCC759B47}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets-Comm" sheetId="5" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1637" uniqueCount="612">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1688" uniqueCount="633">
   <si>
     <t>~TFM_Psets</t>
   </si>
@@ -1878,6 +1878,69 @@
   </si>
   <si>
     <t>Commercial Services - Heat Pumps</t>
+  </si>
+  <si>
+    <t>PRC_AGR</t>
+  </si>
+  <si>
+    <t>PRC_SRV</t>
+  </si>
+  <si>
+    <t>PRC_IND</t>
+  </si>
+  <si>
+    <t>PRC_PWR</t>
+  </si>
+  <si>
+    <t>PRC_RSD</t>
+  </si>
+  <si>
+    <t>PRC_SUP</t>
+  </si>
+  <si>
+    <t>PRC_TRA</t>
+  </si>
+  <si>
+    <t>All AGR processes</t>
+  </si>
+  <si>
+    <t>All SRV processes</t>
+  </si>
+  <si>
+    <t>All IND processes</t>
+  </si>
+  <si>
+    <t>All PWR processes</t>
+  </si>
+  <si>
+    <t>All RSD processes</t>
+  </si>
+  <si>
+    <t>All SUP processes</t>
+  </si>
+  <si>
+    <t>All TRA processes</t>
+  </si>
+  <si>
+    <t>A*,FT-AGR*</t>
+  </si>
+  <si>
+    <t>R*,FT-RSD*</t>
+  </si>
+  <si>
+    <t>P*,FT-PWR*,*GRID*</t>
+  </si>
+  <si>
+    <t>I*,FT-IND*</t>
+  </si>
+  <si>
+    <t>S-*,FT-SRV*</t>
+  </si>
+  <si>
+    <t>T*,FT-TRA*</t>
+  </si>
+  <si>
+    <t>S*,FT-SUP*,-S-*</t>
   </si>
 </sst>
 </file>
@@ -4294,10 +4357,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4611,6 +4674,173 @@
         <v>15</v>
       </c>
       <c r="K13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>626</v>
+      </c>
+      <c r="F14" t="s">
+        <v>612</v>
+      </c>
+      <c r="G14" t="s">
+        <v>619</v>
+      </c>
+      <c r="H14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" t="s">
+        <v>16</v>
+      </c>
+      <c r="J14" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>630</v>
+      </c>
+      <c r="F15" t="s">
+        <v>613</v>
+      </c>
+      <c r="G15" t="s">
+        <v>620</v>
+      </c>
+      <c r="H15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J15" t="s">
+        <v>15</v>
+      </c>
+      <c r="K15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B16" t="s">
+        <v>629</v>
+      </c>
+      <c r="F16" t="s">
+        <v>614</v>
+      </c>
+      <c r="G16" t="s">
+        <v>621</v>
+      </c>
+      <c r="H16" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" t="s">
+        <v>16</v>
+      </c>
+      <c r="J16" t="s">
+        <v>15</v>
+      </c>
+      <c r="K16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>628</v>
+      </c>
+      <c r="F17" t="s">
+        <v>615</v>
+      </c>
+      <c r="G17" t="s">
+        <v>622</v>
+      </c>
+      <c r="H17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" t="s">
+        <v>16</v>
+      </c>
+      <c r="J17" t="s">
+        <v>15</v>
+      </c>
+      <c r="K17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>627</v>
+      </c>
+      <c r="F18" t="s">
+        <v>616</v>
+      </c>
+      <c r="G18" t="s">
+        <v>623</v>
+      </c>
+      <c r="H18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" t="s">
+        <v>16</v>
+      </c>
+      <c r="J18" t="s">
+        <v>15</v>
+      </c>
+      <c r="K18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>632</v>
+      </c>
+      <c r="F19" t="s">
+        <v>617</v>
+      </c>
+      <c r="G19" t="s">
+        <v>624</v>
+      </c>
+      <c r="H19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" t="s">
+        <v>16</v>
+      </c>
+      <c r="J19" t="s">
+        <v>15</v>
+      </c>
+      <c r="K19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B20" t="s">
+        <v>631</v>
+      </c>
+      <c r="F20" t="s">
+        <v>618</v>
+      </c>
+      <c r="G20" t="s">
+        <v>625</v>
+      </c>
+      <c r="H20" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" t="s">
+        <v>16</v>
+      </c>
+      <c r="J20" t="s">
+        <v>15</v>
+      </c>
+      <c r="K20" t="s">
         <v>16</v>
       </c>
     </row>
@@ -7277,8 +7507,8 @@
   </sheetPr>
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Capture all AGR process in the relevant set
</commit_message>
<xml_diff>
--- a/SetRules.xlsx
+++ b/SetRules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr backupFile="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58EFB912-37D6-4F5E-9355-AC2393FA7669}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E46CE5-263A-4F40-AC1E-409B701C8B99}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{69765015-6AAF-4B94-8956-691CCC759B47}"/>
+    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" activeTab="1" xr2:uid="{69765015-6AAF-4B94-8956-691CCC759B47}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets-Comm" sheetId="5" r:id="rId1"/>
@@ -1922,9 +1922,6 @@
     <t>All TRA processes</t>
   </si>
   <si>
-    <t>A*,FT-AGR*</t>
-  </si>
-  <si>
     <t>R*,FT-RSD*</t>
   </si>
   <si>
@@ -1941,6 +1938,9 @@
   </si>
   <si>
     <t>S*,FT-SUP*,-S-*</t>
+  </si>
+  <si>
+    <t>A*,*AGR*</t>
   </si>
 </sst>
 </file>
@@ -4360,7 +4360,7 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4679,7 +4679,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>626</v>
+        <v>632</v>
       </c>
       <c r="F14" t="s">
         <v>612</v>
@@ -4702,7 +4702,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="F15" t="s">
         <v>613</v>
@@ -4728,7 +4728,7 @@
         <v>325</v>
       </c>
       <c r="B16" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="F16" t="s">
         <v>614</v>
@@ -4751,7 +4751,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="F17" t="s">
         <v>615</v>
@@ -4774,7 +4774,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F18" t="s">
         <v>616</v>
@@ -4797,7 +4797,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="F19" t="s">
         <v>617</v>
@@ -4823,7 +4823,7 @@
         <v>325</v>
       </c>
       <c r="B20" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="F20" t="s">
         <v>618</v>

</xml_diff>

<commit_message>
Include IMP/EXP/MIN processes together with other SUP processes
</commit_message>
<xml_diff>
--- a/SetRules.xlsx
+++ b/SetRules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E46CE5-263A-4F40-AC1E-409B701C8B99}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD2C40A-699B-4CE4-9753-B9E06BE51D2C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" activeTab="1" xr2:uid="{69765015-6AAF-4B94-8956-691CCC759B47}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{69765015-6AAF-4B94-8956-691CCC759B47}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets-Comm" sheetId="5" r:id="rId1"/>
@@ -1937,10 +1937,10 @@
     <t>T*,FT-TRA*</t>
   </si>
   <si>
-    <t>S*,FT-SUP*,-S-*</t>
-  </si>
-  <si>
     <t>A*,*AGR*</t>
+  </si>
+  <si>
+    <t>S*,FT-SUP*,IMP*,EXP*,MIN*,-S-*</t>
   </si>
 </sst>
 </file>
@@ -4360,7 +4360,7 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4679,7 +4679,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="F14" t="s">
         <v>612</v>
@@ -4797,7 +4797,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="F19" t="s">
         <v>617</v>

</xml_diff>

<commit_message>
Correct the description of wind offshore and onshore
</commit_message>
<xml_diff>
--- a/SetRules.xlsx
+++ b/SetRules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr backupFile="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD2C40A-699B-4CE4-9753-B9E06BE51D2C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C9C4B48-1DEE-48E5-849E-9281725DECAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{69765015-6AAF-4B94-8956-691CCC759B47}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{69765015-6AAF-4B94-8956-691CCC759B47}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets-Comm" sheetId="5" r:id="rId1"/>
@@ -4359,8 +4359,8 @@
   </sheetPr>
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6961,8 +6961,8 @@
   </sheetPr>
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7272,7 +7272,7 @@
         <v>311</v>
       </c>
       <c r="G17" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="H17" t="s">
         <v>15</v>
@@ -7289,7 +7289,7 @@
         <v>312</v>
       </c>
       <c r="G18" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H18" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Update cover pages of some files
</commit_message>
<xml_diff>
--- a/SetRules.xlsx
+++ b/SetRules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91F43E5-4D5A-4405-B66A-C12391594DA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E332CD-8857-4FF5-9ADC-8731981B702F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{69765015-6AAF-4B94-8956-691CCC759B47}"/>
   </bookViews>
@@ -24,9 +24,6 @@
     <sheet name="SUP_Sets-Proc" sheetId="12" r:id="rId9"/>
     <sheet name="SRV_Sets-Proc" sheetId="15" r:id="rId10"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId11"/>
-  </externalReferences>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
     <definedName name="_AtRisk_SimSetting_AutomaticallyGenerateReports" hidden="1">FALSE</definedName>
@@ -2019,27 +2016,15 @@
     <t>Document type:</t>
   </si>
   <si>
-    <t>Template type</t>
-  </si>
-  <si>
     <t>Sector(s):</t>
   </si>
   <si>
-    <t>Sector name</t>
-  </si>
-  <si>
     <t>Purpose:</t>
   </si>
   <si>
-    <t>Brief description of what this file is for</t>
-  </si>
-  <si>
     <t>Original developer(s):</t>
   </si>
   <si>
-    <t>Full Name(s) (Affiliation, email)</t>
-  </si>
-  <si>
     <t>Current maintainer(s):</t>
   </si>
   <si>
@@ -2059,6 +2044,18 @@
   </si>
   <si>
     <t>https://creativecommons.org/licenses/by-nc-sa/4.0/</t>
+  </si>
+  <si>
+    <t>Set Rules</t>
+  </si>
+  <si>
+    <t>All sectors</t>
+  </si>
+  <si>
+    <t>Specifies aggrigation rules for user-defined sets</t>
+  </si>
+  <si>
+    <t>Olexandr Balyk (UCC, olexandr.balyk@ucc.ie)</t>
   </si>
 </sst>
 </file>
@@ -2202,9 +2199,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2223,9 +2217,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2238,14 +2229,20 @@
     <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2578,19 +2575,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Cover"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2892,7 +2876,7 @@
   <dimension ref="A1:Z99"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3329,20 +3313,20 @@
       <c r="Z15" s="3"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="18" t="s">
         <v>633</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
@@ -3359,10 +3343,10 @@
       <c r="Z16" s="3"/>
     </row>
     <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -3387,18 +3371,18 @@
       <c r="Z17" s="3"/>
     </row>
     <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
@@ -3415,22 +3399,22 @@
       <c r="Z18" s="3"/>
     </row>
     <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="9" t="s">
         <v>634</v>
       </c>
-      <c r="B19" s="11" t="s">
-        <v>635</v>
-      </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
+      <c r="B19" s="17" t="s">
+        <v>645</v>
+      </c>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
@@ -3447,22 +3431,22 @@
       <c r="Z19" s="3"/>
     </row>
     <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
-        <v>636</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>637</v>
-      </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
+      <c r="A20" s="9" t="s">
+        <v>635</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>646</v>
+      </c>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
@@ -3479,22 +3463,22 @@
       <c r="Z20" s="3"/>
     </row>
     <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
-        <v>638</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>639</v>
-      </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
+      <c r="A21" s="9" t="s">
+        <v>636</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>647</v>
+      </c>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
@@ -3511,18 +3495,18 @@
       <c r="Z21" s="3"/>
     </row>
     <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
+      <c r="A22" s="9"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
@@ -3539,14 +3523,14 @@
       <c r="Z22" s="3"/>
     </row>
     <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
-        <v>640</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>641</v>
-      </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
+      <c r="A23" s="9" t="s">
+        <v>637</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>648</v>
+      </c>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
@@ -3571,10 +3555,10 @@
       <c r="Z23" s="3"/>
     </row>
     <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
@@ -3599,10 +3583,10 @@
       <c r="Z24" s="3"/>
     </row>
     <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
+      <c r="A25" s="9"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
@@ -3627,14 +3611,14 @@
       <c r="Z25" s="3"/>
     </row>
     <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
-        <v>642</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>641</v>
-      </c>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
+      <c r="A26" s="9" t="s">
+        <v>638</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>648</v>
+      </c>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
@@ -3659,10 +3643,10 @@
       <c r="Z26" s="3"/>
     </row>
     <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
+      <c r="A27" s="9"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
@@ -3687,10 +3671,10 @@
       <c r="Z27" s="3"/>
     </row>
     <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="10"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
+      <c r="A28" s="9"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
@@ -3715,14 +3699,14 @@
       <c r="Z28" s="3"/>
     </row>
     <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
-        <v>643</v>
-      </c>
-      <c r="B29" s="15">
+      <c r="A29" s="9" t="s">
+        <v>639</v>
+      </c>
+      <c r="B29" s="13">
         <v>1</v>
       </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
@@ -3747,16 +3731,16 @@
       <c r="Z29" s="3"/>
     </row>
     <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
-        <v>644</v>
-      </c>
-      <c r="B30" s="16" t="s">
-        <v>645</v>
-      </c>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
+      <c r="A30" s="9" t="s">
+        <v>640</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>641</v>
+      </c>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
@@ -3779,16 +3763,16 @@
       <c r="Z30" s="3"/>
     </row>
     <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
-        <v>646</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
+      <c r="A31" s="9" t="s">
+        <v>642</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>643</v>
+      </c>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
@@ -3811,12 +3795,12 @@
       <c r="Z31" s="3"/>
     </row>
     <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
-      <c r="B32" s="19" t="s">
-        <v>648</v>
-      </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
+      <c r="A32" s="15"/>
+      <c r="B32" s="16" t="s">
+        <v>644</v>
+      </c>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>

</xml_diff>

<commit_message>
Add sensitivity analysis for hurdle rates
</commit_message>
<xml_diff>
--- a/SetRules.xlsx
+++ b/SetRules.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr backupFile="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58EFB912-37D6-4F5E-9355-AC2393FA7669}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD2C40A-699B-4CE4-9753-B9E06BE51D2C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{69765015-6AAF-4B94-8956-691CCC759B47}"/>
   </bookViews>
@@ -1922,9 +1922,6 @@
     <t>All TRA processes</t>
   </si>
   <si>
-    <t>A*,FT-AGR*</t>
-  </si>
-  <si>
     <t>R*,FT-RSD*</t>
   </si>
   <si>
@@ -1940,7 +1937,10 @@
     <t>T*,FT-TRA*</t>
   </si>
   <si>
-    <t>S*,FT-SUP*,-S-*</t>
+    <t>A*,*AGR*</t>
+  </si>
+  <si>
+    <t>S*,FT-SUP*,IMP*,EXP*,MIN*,-S-*</t>
   </si>
 </sst>
 </file>
@@ -4360,7 +4360,7 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4679,7 +4679,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>626</v>
+        <v>631</v>
       </c>
       <c r="F14" t="s">
         <v>612</v>
@@ -4702,7 +4702,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="F15" t="s">
         <v>613</v>
@@ -4728,7 +4728,7 @@
         <v>325</v>
       </c>
       <c r="B16" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="F16" t="s">
         <v>614</v>
@@ -4751,7 +4751,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="F17" t="s">
         <v>615</v>
@@ -4774,7 +4774,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F18" t="s">
         <v>616</v>
@@ -4823,7 +4823,7 @@
         <v>325</v>
       </c>
       <c r="B20" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="F20" t="s">
         <v>618</v>

</xml_diff>